<commit_message>
Actualización del check list de calidad
</commit_message>
<xml_diff>
--- a/Organización/Calidad/PTL_Checklist_Calidad_aammdd.xlsx
+++ b/Organización/Calidad/PTL_Checklist_Calidad_aammdd.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095"/>
+    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -243,19 +243,19 @@
     <t>Garantía</t>
   </si>
   <si>
-    <t>¿Se recibió la solicitud del problema?</t>
-  </si>
-  <si>
-    <t>¿La solicitud tiene asignado a un responsable de ejecución?</t>
-  </si>
-  <si>
     <t>¿Se resolvió el inconveniente presentado?</t>
   </si>
   <si>
-    <t>¿Esta validado el problema presentado?</t>
+    <t>¿Todas las solicitud tiene asignado a un responsable de ejecución?</t>
   </si>
   <si>
-    <t>¿Se cerro la tarea alfinalizar la validación del problema?</t>
+    <t>¿Todas las inconformidad estan validadas?</t>
+  </si>
+  <si>
+    <t>¿Todas las tareas solucionadas estan cerradas?</t>
+  </si>
+  <si>
+    <t>carta de aceptación</t>
   </si>
 </sst>
 </file>
@@ -659,7 +659,7 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -753,56 +753,6 @@
     <xf numFmtId="165" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -866,6 +816,59 @@
     <xf numFmtId="165" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1185,7 +1188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1205,66 +1208,66 @@
     <row r="1" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="2"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
     </row>
     <row r="4" spans="1:6" ht="15.75">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
     </row>
     <row r="6" spans="1:6" ht="13.9" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="12" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
       <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1">
@@ -1351,11 +1354,11 @@
         <v>Garantía</v>
       </c>
       <c r="C19" s="20">
-        <f>COUNTA(procesos!C49:C54)</f>
+        <f>COUNTA(procesos!C49:C53)</f>
         <v>0</v>
       </c>
       <c r="D19" s="21" t="e">
-        <f>COUNTIF(procesos!C49:C54,"x")/(COUNTIF((procesos!C49:C54),"x")+COUNTIF((procesos!D49:D54),"x"))</f>
+        <f>COUNTIF(procesos!C49:C53,"x")/(COUNTIF((procesos!C49:C53),"x")+COUNTIF((procesos!D49:D53),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1363,11 +1366,11 @@
     <row r="21" spans="2:4" s="5" customFormat="1" ht="12.75"/>
     <row r="22" spans="2:4" s="5" customFormat="1" ht="12.75"/>
     <row r="23" spans="2:4" ht="15.75">
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="6" t="s">
@@ -1435,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMI192"/>
+  <dimension ref="A1:AMI191"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1451,22 +1454,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="44" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="47" t="s">
+      <c r="D1" s="63"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="65" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51"/>
+      <c r="A2" s="68"/>
+      <c r="B2" s="69"/>
       <c r="C2" s="14" t="s">
         <v>14</v>
       </c>
@@ -1476,75 +1479,75 @@
       <c r="E2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="47"/>
+      <c r="F2" s="65"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="55">
+      <c r="A3" s="37">
         <v>1</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="58"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="55">
+      <c r="A4" s="37">
         <v>2</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="60"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="42"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="55">
+      <c r="A5" s="37">
         <v>3</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="60"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="42"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="55">
+      <c r="A6" s="37">
         <v>4</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="60"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:6" s="15" customFormat="1"/>
     <row r="8" spans="1:6" s="15" customFormat="1"/>
     <row r="9" spans="1:6" s="15" customFormat="1">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="42" t="s">
+      <c r="B9" s="71"/>
+      <c r="C9" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="52" t="s">
+      <c r="D9" s="72"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="74" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="15" customFormat="1">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="36" t="s">
         <v>9</v>
       </c>
@@ -1554,7 +1557,7 @@
       <c r="E10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="54"/>
+      <c r="F10" s="75"/>
     </row>
     <row r="11" spans="1:6" s="15" customFormat="1">
       <c r="A11" s="24">
@@ -1655,22 +1658,22 @@
     <row r="19" spans="1:6" s="15" customFormat="1"/>
     <row r="20" spans="1:6" s="15" customFormat="1"/>
     <row r="21" spans="1:6" s="15" customFormat="1">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="42" t="s">
+      <c r="B21" s="71"/>
+      <c r="C21" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="42"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="52" t="s">
+      <c r="D21" s="72"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="74" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="15" customFormat="1">
-      <c r="A22" s="41"/>
-      <c r="B22" s="41"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="71"/>
       <c r="C22" s="31" t="s">
         <v>9</v>
       </c>
@@ -1680,87 +1683,87 @@
       <c r="E22" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="53"/>
+      <c r="F22" s="76"/>
     </row>
     <row r="23" spans="1:6" s="15" customFormat="1">
-      <c r="A23" s="65">
+      <c r="A23" s="47">
         <v>1</v>
       </c>
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="63"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="45"/>
     </row>
     <row r="24" spans="1:6" s="15" customFormat="1">
-      <c r="A24" s="66">
+      <c r="A24" s="48">
         <v>2</v>
       </c>
-      <c r="B24" s="64" t="s">
+      <c r="B24" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="63"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="45"/>
     </row>
     <row r="25" spans="1:6" s="15" customFormat="1">
-      <c r="A25" s="66">
+      <c r="A25" s="48">
         <v>3</v>
       </c>
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="63"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="45"/>
     </row>
     <row r="26" spans="1:6" s="15" customFormat="1">
-      <c r="A26" s="66">
+      <c r="A26" s="48">
         <v>4</v>
       </c>
-      <c r="B26" s="64" t="s">
+      <c r="B26" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="63"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="45"/>
     </row>
     <row r="27" spans="1:6" s="15" customFormat="1">
-      <c r="A27" s="66">
+      <c r="A27" s="48">
         <v>5</v>
       </c>
-      <c r="B27" s="67" t="s">
+      <c r="B27" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="63"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="45"/>
     </row>
     <row r="28" spans="1:6" s="15" customFormat="1"/>
     <row r="29" spans="1:6" s="15" customFormat="1"/>
     <row r="30" spans="1:6" s="15" customFormat="1">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="41"/>
-      <c r="C30" s="42" t="s">
+      <c r="B30" s="71"/>
+      <c r="C30" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="42"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="52" t="s">
+      <c r="D30" s="72"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="74" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="15" customFormat="1">
-      <c r="A31" s="41"/>
-      <c r="B31" s="41"/>
+      <c r="A31" s="71"/>
+      <c r="B31" s="71"/>
       <c r="C31" s="32" t="s">
         <v>9</v>
       </c>
@@ -1770,76 +1773,76 @@
       <c r="E31" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="53"/>
+      <c r="F31" s="76"/>
     </row>
     <row r="32" spans="1:6" s="15" customFormat="1">
-      <c r="A32" s="65">
+      <c r="A32" s="47">
         <v>1</v>
       </c>
-      <c r="B32" s="61" t="s">
+      <c r="B32" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="63"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="45"/>
     </row>
     <row r="33" spans="1:6" s="15" customFormat="1">
-      <c r="A33" s="66">
+      <c r="A33" s="48">
         <v>2</v>
       </c>
-      <c r="B33" s="64" t="s">
+      <c r="B33" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="63"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="45"/>
     </row>
     <row r="34" spans="1:6" s="15" customFormat="1">
-      <c r="A34" s="66">
+      <c r="A34" s="48">
         <v>3</v>
       </c>
-      <c r="B34" s="64" t="s">
+      <c r="B34" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="63"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="45"/>
     </row>
     <row r="35" spans="1:6" s="15" customFormat="1">
-      <c r="A35" s="66">
+      <c r="A35" s="48">
         <v>4</v>
       </c>
-      <c r="B35" s="64" t="s">
+      <c r="B35" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="63"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="45"/>
     </row>
     <row r="36" spans="1:6" s="15" customFormat="1"/>
     <row r="37" spans="1:6" s="15" customFormat="1"/>
     <row r="38" spans="1:6" s="15" customFormat="1"/>
     <row r="39" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A39" s="41" t="s">
+      <c r="A39" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="41"/>
-      <c r="C39" s="42" t="s">
+      <c r="B39" s="71"/>
+      <c r="C39" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="42"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="52" t="s">
+      <c r="D39" s="72"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="74" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A40" s="41"/>
-      <c r="B40" s="41"/>
+      <c r="A40" s="71"/>
+      <c r="B40" s="71"/>
       <c r="C40" s="36" t="s">
         <v>9</v>
       </c>
@@ -1849,7 +1852,7 @@
       <c r="E40" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F40" s="54"/>
+      <c r="F40" s="75"/>
     </row>
     <row r="41" spans="1:6" s="15" customFormat="1">
       <c r="A41" s="24">
@@ -1901,28 +1904,28 @@
     </row>
     <row r="45" spans="1:6" s="15" customFormat="1"/>
     <row r="46" spans="1:6" s="15" customFormat="1">
-      <c r="B46" s="40"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="40"/>
-      <c r="E46" s="40"/>
+      <c r="B46" s="70"/>
+      <c r="C46" s="70"/>
+      <c r="D46" s="70"/>
+      <c r="E46" s="70"/>
     </row>
     <row r="47" spans="1:6" s="15" customFormat="1">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="41"/>
-      <c r="C47" s="42" t="s">
+      <c r="B47" s="71"/>
+      <c r="C47" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="42"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="52" t="s">
+      <c r="D47" s="72"/>
+      <c r="E47" s="73"/>
+      <c r="F47" s="74" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="15" customFormat="1">
-      <c r="A48" s="41"/>
-      <c r="B48" s="41"/>
+      <c r="A48" s="71"/>
+      <c r="B48" s="71"/>
       <c r="C48" s="36" t="s">
         <v>9</v>
       </c>
@@ -1932,14 +1935,14 @@
       <c r="E48" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F48" s="54"/>
+      <c r="F48" s="75"/>
     </row>
     <row r="49" spans="1:6" s="15" customFormat="1">
       <c r="A49" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C49" s="26"/>
       <c r="D49" s="26"/>
@@ -1948,10 +1951,10 @@
     </row>
     <row r="50" spans="1:6" s="15" customFormat="1">
       <c r="A50" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C50" s="26"/>
       <c r="D50" s="26"/>
@@ -1960,10 +1963,10 @@
     </row>
     <row r="51" spans="1:6" s="15" customFormat="1">
       <c r="A51" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C51" s="26"/>
       <c r="D51" s="26"/>
@@ -1972,9 +1975,9 @@
     </row>
     <row r="52" spans="1:6" s="15" customFormat="1">
       <c r="A52" s="24">
-        <v>4</v>
+        <v>5</v>
       </c>
-      <c r="B52" s="25" t="s">
+      <c r="B52" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C52" s="26"/>
@@ -1984,7 +1987,7 @@
     </row>
     <row r="53" spans="1:6" s="15" customFormat="1">
       <c r="A53" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B53" s="27" t="s">
         <v>78</v>
@@ -1994,18 +1997,7 @@
       <c r="E53" s="26"/>
       <c r="F53" s="25"/>
     </row>
-    <row r="54" spans="1:6" s="15" customFormat="1">
-      <c r="A54" s="24">
-        <v>6</v>
-      </c>
-      <c r="B54" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="25"/>
-    </row>
+    <row r="54" spans="1:6" s="15" customFormat="1"/>
     <row r="55" spans="1:6" s="15" customFormat="1"/>
     <row r="56" spans="1:6" s="15" customFormat="1"/>
     <row r="57" spans="1:6" s="15" customFormat="1"/>
@@ -2014,45 +2006,45 @@
     <row r="60" spans="1:6" s="15" customFormat="1"/>
     <row r="61" spans="1:6" s="15" customFormat="1"/>
     <row r="62" spans="1:6" s="15" customFormat="1"/>
-    <row r="63" spans="1:6" s="15" customFormat="1"/>
+    <row r="63" spans="1:6" s="15" customFormat="1" ht="409.6"/>
     <row r="64" spans="1:6" s="15" customFormat="1"/>
     <row r="65" spans="2:5" s="15" customFormat="1"/>
     <row r="66" spans="2:5" s="15" customFormat="1"/>
     <row r="67" spans="2:5" s="15" customFormat="1"/>
-    <row r="68" spans="2:5" s="15" customFormat="1"/>
-    <row r="69" spans="2:5" s="15" customFormat="1">
-      <c r="B69" s="40"/>
-      <c r="C69" s="40"/>
-      <c r="D69" s="40"/>
-      <c r="E69" s="40"/>
+    <row r="68" spans="2:5" s="15" customFormat="1">
+      <c r="B68" s="70"/>
+      <c r="C68" s="70"/>
+      <c r="D68" s="70"/>
+      <c r="E68" s="70"/>
     </row>
-    <row r="70" spans="2:5" s="15" customFormat="1"/>
-    <row r="71" spans="2:5" s="15" customFormat="1">
-      <c r="C71" s="16"/>
-      <c r="D71" s="16"/>
-      <c r="E71" s="16"/>
+    <row r="69" spans="2:5" s="15" customFormat="1"/>
+    <row r="70" spans="2:5" s="15" customFormat="1">
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
     </row>
+    <row r="71" spans="2:5" s="15" customFormat="1"/>
     <row r="72" spans="2:5" s="15" customFormat="1"/>
     <row r="73" spans="2:5" s="15" customFormat="1"/>
     <row r="74" spans="2:5" s="15" customFormat="1"/>
     <row r="75" spans="2:5" s="15" customFormat="1"/>
     <row r="76" spans="2:5" s="15" customFormat="1"/>
     <row r="77" spans="2:5" s="15" customFormat="1"/>
-    <row r="78" spans="2:5" s="15" customFormat="1" ht="409.6"/>
+    <row r="78" spans="2:5" s="15" customFormat="1"/>
     <row r="79" spans="2:5" s="15" customFormat="1"/>
-    <row r="80" spans="2:5" s="15" customFormat="1"/>
-    <row r="81" spans="2:5" s="15" customFormat="1" ht="409.6">
-      <c r="B81" s="40"/>
-      <c r="C81" s="40"/>
-      <c r="D81" s="40"/>
-      <c r="E81" s="40"/>
+    <row r="80" spans="2:5" s="15" customFormat="1">
+      <c r="B80" s="70"/>
+      <c r="C80" s="70"/>
+      <c r="D80" s="70"/>
+      <c r="E80" s="70"/>
     </row>
-    <row r="82" spans="2:5" s="15" customFormat="1" ht="409.6"/>
-    <row r="83" spans="2:5" s="15" customFormat="1">
-      <c r="C83" s="16"/>
-      <c r="D83" s="16"/>
-      <c r="E83" s="16"/>
+    <row r="81" spans="2:5" s="15" customFormat="1"/>
+    <row r="82" spans="2:5" s="15" customFormat="1">
+      <c r="C82" s="16"/>
+      <c r="D82" s="16"/>
+      <c r="E82" s="16"/>
     </row>
+    <row r="83" spans="2:5" s="15" customFormat="1"/>
     <row r="84" spans="2:5" s="15" customFormat="1"/>
     <row r="85" spans="2:5" s="15" customFormat="1"/>
     <row r="86" spans="2:5" s="15" customFormat="1"/>
@@ -2065,32 +2057,32 @@
     <row r="93" spans="2:5" s="15" customFormat="1"/>
     <row r="94" spans="2:5" s="15" customFormat="1"/>
     <row r="95" spans="2:5" s="15" customFormat="1"/>
-    <row r="96" spans="2:5" s="15" customFormat="1"/>
-    <row r="97" spans="2:5" s="15" customFormat="1">
-      <c r="B97" s="40"/>
-      <c r="C97" s="40"/>
-      <c r="D97" s="40"/>
-      <c r="E97" s="40"/>
+    <row r="96" spans="2:5" s="15" customFormat="1">
+      <c r="B96" s="70"/>
+      <c r="C96" s="70"/>
+      <c r="D96" s="70"/>
+      <c r="E96" s="70"/>
     </row>
-    <row r="98" spans="2:5" s="15" customFormat="1"/>
-    <row r="99" spans="2:5" s="15" customFormat="1">
-      <c r="C99" s="16"/>
-      <c r="D99" s="16"/>
-      <c r="E99" s="16"/>
+    <row r="97" spans="3:5" s="15" customFormat="1"/>
+    <row r="98" spans="3:5" s="15" customFormat="1">
+      <c r="C98" s="16"/>
+      <c r="D98" s="16"/>
+      <c r="E98" s="16"/>
     </row>
-    <row r="100" spans="2:5" s="15" customFormat="1"/>
-    <row r="101" spans="2:5" s="15" customFormat="1"/>
-    <row r="102" spans="2:5" s="15" customFormat="1"/>
-    <row r="103" spans="2:5" s="15" customFormat="1"/>
-    <row r="104" spans="2:5" s="15" customFormat="1"/>
-    <row r="105" spans="2:5" s="15" customFormat="1"/>
-    <row r="106" spans="2:5" s="15" customFormat="1"/>
-    <row r="107" spans="2:5" s="15" customFormat="1"/>
-    <row r="108" spans="2:5" s="15" customFormat="1"/>
-    <row r="109" spans="2:5" s="15" customFormat="1"/>
-    <row r="110" spans="2:5" s="15" customFormat="1"/>
-    <row r="111" spans="2:5" s="15" customFormat="1"/>
-    <row r="112" spans="2:5" s="15" customFormat="1"/>
+    <row r="99" spans="3:5" s="15" customFormat="1"/>
+    <row r="100" spans="3:5" s="15" customFormat="1"/>
+    <row r="101" spans="3:5" s="15" customFormat="1"/>
+    <row r="102" spans="3:5" s="15" customFormat="1"/>
+    <row r="103" spans="3:5" s="15" customFormat="1"/>
+    <row r="104" spans="3:5" s="15" customFormat="1"/>
+    <row r="105" spans="3:5" s="15" customFormat="1"/>
+    <row r="106" spans="3:5" s="15" customFormat="1"/>
+    <row r="107" spans="3:5" s="15" customFormat="1"/>
+    <row r="108" spans="3:5" s="15" customFormat="1"/>
+    <row r="109" spans="3:5" s="15" customFormat="1"/>
+    <row r="110" spans="3:5" s="15" customFormat="1"/>
+    <row r="111" spans="3:5" s="15" customFormat="1"/>
+    <row r="112" spans="3:5" s="15" customFormat="1"/>
     <row r="113" s="15" customFormat="1"/>
     <row r="114" s="15" customFormat="1"/>
     <row r="115" s="15" customFormat="1"/>
@@ -2170,14 +2162,19 @@
     <row r="189" s="15" customFormat="1"/>
     <row r="190" s="15" customFormat="1"/>
     <row r="191" s="15" customFormat="1"/>
-    <row r="192" s="15" customFormat="1"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B96:E96"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="A9:B10"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="C21:E21"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:B2"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="B80:E80"/>
     <mergeCell ref="A30:B31"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="A39:B40"/>
@@ -2189,12 +2186,6 @@
     <mergeCell ref="A47:B48"/>
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="F47:F48"/>
-    <mergeCell ref="B97:E97"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="A9:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="C21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2204,10 +2195,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ31"/>
+  <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2217,22 +2208,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="42" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="52" t="s">
+      <c r="D1" s="72"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="74" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1024">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
+      <c r="A2" s="71"/>
+      <c r="B2" s="71"/>
       <c r="C2" s="31" t="s">
         <v>9</v>
       </c>
@@ -2242,67 +2233,67 @@
       <c r="E2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="53"/>
+      <c r="F2" s="76"/>
     </row>
     <row r="3" spans="1:1024" ht="30">
-      <c r="A3" s="68">
+      <c r="A3" s="50">
         <v>1</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="71"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="53"/>
     </row>
     <row r="4" spans="1:1024" ht="32.25" customHeight="1">
-      <c r="A4" s="66">
+      <c r="A4" s="48">
         <v>2</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="74"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="56"/>
     </row>
     <row r="5" spans="1:1024" ht="30">
-      <c r="A5" s="66">
+      <c r="A5" s="48">
         <v>3</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
     </row>
     <row r="6" spans="1:1024" ht="30">
-      <c r="A6" s="66">
+      <c r="A6" s="48">
         <v>4</v>
       </c>
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
     </row>
     <row r="7" spans="1:1024">
-      <c r="A7" s="76">
+      <c r="A7" s="58">
         <v>5</v>
       </c>
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
     </row>
     <row r="8" spans="1:1024">
       <c r="A8" s="35"/>
@@ -2313,22 +2304,22 @@
       <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:1024" ht="15" customHeight="1">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="42" t="s">
+      <c r="B9" s="71"/>
+      <c r="C9" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="52" t="s">
+      <c r="D9" s="72"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="74" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:1024" ht="15" customHeight="1">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="31" t="s">
         <v>9</v>
       </c>
@@ -2338,19 +2329,19 @@
       <c r="E10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="53"/>
+      <c r="F10" s="76"/>
     </row>
     <row r="11" spans="1:1024" ht="30">
-      <c r="A11" s="68">
+      <c r="A11" s="50">
         <v>1</v>
       </c>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="70"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="71"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="53"/>
     </row>
     <row r="12" spans="1:1024">
       <c r="A12" s="35"/>
@@ -2361,16 +2352,16 @@
       <c r="F12" s="34"/>
     </row>
     <row r="13" spans="1:1024" ht="15" customHeight="1">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="42" t="s">
+      <c r="B13" s="71"/>
+      <c r="C13" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="52" t="s">
+      <c r="D13" s="72"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="74" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="12"/>
@@ -3393,8 +3384,8 @@
       <c r="AMJ13" s="12"/>
     </row>
     <row r="14" spans="1:1024" ht="15" customHeight="1">
-      <c r="A14" s="41"/>
-      <c r="B14" s="41"/>
+      <c r="A14" s="71"/>
+      <c r="B14" s="71"/>
       <c r="C14" s="31" t="s">
         <v>9</v>
       </c>
@@ -3404,7 +3395,7 @@
       <c r="E14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="53"/>
+      <c r="F14" s="76"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
@@ -4425,16 +4416,16 @@
       <c r="AMJ14" s="12"/>
     </row>
     <row r="15" spans="1:1024">
-      <c r="A15" s="65">
+      <c r="A15" s="47">
         <v>1</v>
       </c>
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="63"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="45"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -5455,16 +5446,16 @@
       <c r="AMJ15" s="12"/>
     </row>
     <row r="16" spans="1:1024">
-      <c r="A16" s="66">
+      <c r="A16" s="48">
         <v>2</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="63"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="45"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
@@ -6485,16 +6476,16 @@
       <c r="AMJ16" s="12"/>
     </row>
     <row r="17" spans="1:1024">
-      <c r="A17" s="66">
+      <c r="A17" s="48">
         <v>3</v>
       </c>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="63"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="45"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
@@ -7515,16 +7506,16 @@
       <c r="AMJ17" s="12"/>
     </row>
     <row r="18" spans="1:1024">
-      <c r="A18" s="66">
+      <c r="A18" s="48">
         <v>4</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="63"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="45"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
@@ -8545,16 +8536,16 @@
       <c r="AMJ18" s="12"/>
     </row>
     <row r="19" spans="1:1024">
-      <c r="A19" s="66">
+      <c r="A19" s="48">
         <v>5</v>
       </c>
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="63"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="45"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
@@ -9575,16 +9566,16 @@
       <c r="AMJ19" s="12"/>
     </row>
     <row r="20" spans="1:1024">
-      <c r="A20" s="66">
+      <c r="A20" s="48">
         <v>6</v>
       </c>
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="63"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="45"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
@@ -10605,16 +10596,16 @@
       <c r="AMJ20" s="12"/>
     </row>
     <row r="21" spans="1:1024" ht="30">
-      <c r="A21" s="66">
+      <c r="A21" s="48">
         <v>7</v>
       </c>
-      <c r="B21" s="67" t="s">
+      <c r="B21" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="63"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="45"/>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
@@ -11635,16 +11626,16 @@
       <c r="AMJ21" s="12"/>
     </row>
     <row r="22" spans="1:1024">
-      <c r="A22" s="66">
+      <c r="A22" s="48">
         <v>8</v>
       </c>
-      <c r="B22" s="67" t="s">
+      <c r="B22" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="63"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="45"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -12665,16 +12656,16 @@
       <c r="AMJ22" s="12"/>
     </row>
     <row r="23" spans="1:1024">
-      <c r="A23" s="66">
+      <c r="A23" s="48">
         <v>9</v>
       </c>
-      <c r="B23" s="67" t="s">
+      <c r="B23" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="63"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="45"/>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -13695,16 +13686,16 @@
       <c r="AMJ23" s="12"/>
     </row>
     <row r="24" spans="1:1024" ht="30">
-      <c r="A24" s="66">
+      <c r="A24" s="48">
         <v>10</v>
       </c>
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="63"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="45"/>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
@@ -14725,16 +14716,16 @@
       <c r="AMJ24" s="12"/>
     </row>
     <row r="25" spans="1:1024">
-      <c r="A25" s="66">
+      <c r="A25" s="48">
         <v>11</v>
       </c>
-      <c r="B25" s="67" t="s">
+      <c r="B25" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="63"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="45"/>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
@@ -15755,16 +15746,16 @@
       <c r="AMJ25" s="12"/>
     </row>
     <row r="26" spans="1:1024">
-      <c r="A26" s="66">
+      <c r="A26" s="48">
         <v>12</v>
       </c>
-      <c r="B26" s="67" t="s">
+      <c r="B26" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="63"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="45"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
@@ -16785,16 +16776,16 @@
       <c r="AMJ26" s="12"/>
     </row>
     <row r="27" spans="1:1024" ht="30">
-      <c r="A27" s="66">
+      <c r="A27" s="48">
         <v>11</v>
       </c>
-      <c r="B27" s="67" t="s">
+      <c r="B27" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="63"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="45"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
@@ -17815,16 +17806,16 @@
       <c r="AMJ27" s="12"/>
     </row>
     <row r="28" spans="1:1024">
-      <c r="A28" s="66">
+      <c r="A28" s="48">
         <v>12</v>
       </c>
-      <c r="B28" s="64" t="s">
+      <c r="B28" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="63"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="45"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
@@ -18845,16 +18836,16 @@
       <c r="AMJ28" s="12"/>
     </row>
     <row r="29" spans="1:1024">
-      <c r="A29" s="66">
+      <c r="A29" s="48">
         <v>13</v>
       </c>
-      <c r="B29" s="64" t="s">
+      <c r="B29" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="63"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="45"/>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
@@ -19875,16 +19866,16 @@
       <c r="AMJ29" s="12"/>
     </row>
     <row r="30" spans="1:1024">
-      <c r="A30" s="66">
+      <c r="A30" s="48">
         <v>14</v>
       </c>
-      <c r="B30" s="64" t="s">
+      <c r="B30" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="62"/>
-      <c r="F30" s="63"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="45"/>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
@@ -20905,16 +20896,16 @@
       <c r="AMJ30" s="12"/>
     </row>
     <row r="31" spans="1:1024">
-      <c r="A31" s="66">
+      <c r="A31" s="48">
         <v>15</v>
       </c>
-      <c r="B31" s="64" t="s">
+      <c r="B31" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="63"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="45"/>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
@@ -21934,6 +21925,11 @@
       <c r="AMI31" s="12"/>
       <c r="AMJ31" s="12"/>
     </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="77" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="F13:F14"/>

</xml_diff>

<commit_message>
Actualizacion checklist de calidad
</commit_message>
<xml_diff>
--- a/Organización/Calidad/PTL_Checklist_Calidad_aammdd.xlsx
+++ b/Organización/Calidad/PTL_Checklist_Calidad_aammdd.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095" activeTab="2"/>
+    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="85">
   <si>
     <t>DATOS GENERALES</t>
   </si>
@@ -257,6 +257,21 @@
   <si>
     <t>carta de aceptación</t>
   </si>
+  <si>
+    <t>¿Tiene definido el nombre del cliente atendido?</t>
+  </si>
+  <si>
+    <t>¿Se tiene especificado el inconveniente que fue resuelto?</t>
+  </si>
+  <si>
+    <t>¿Se cuenta con las respuestas solicitadas al cliente?</t>
+  </si>
+  <si>
+    <t>No aplica</t>
+  </si>
+  <si>
+    <t>Carta de aceptación</t>
+  </si>
 </sst>
 </file>
 
@@ -364,7 +379,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,6 +455,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFE6E6FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor rgb="FFE6E6FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -659,7 +704,7 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="90">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -824,6 +869,16 @@
     <xf numFmtId="165" fontId="8" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -848,16 +903,6 @@
     <xf numFmtId="165" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -867,8 +912,42 @@
     <xf numFmtId="165" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="14" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="14" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="14" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="14" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="14" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1186,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ27"/>
+  <dimension ref="A1:AMJ28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1384,38 +1463,51 @@
       </c>
     </row>
     <row r="25" spans="2:4">
-      <c r="B25" s="8" t="str">
+      <c r="B25" s="83" t="str">
         <f>Productos!A1</f>
         <v>Estimación</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="84">
         <f>COUNTA(Productos!C3:C7)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="10" t="e">
+      <c r="D25" s="85" t="e">
         <f>COUNTIF(Productos!C3:C7,"x")/(COUNTIF((Productos!C3:C7),"x")+COUNTIF((Productos!D3:D7),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26" s="23" t="str">
+      <c r="B26" s="86" t="str">
         <f>Productos!A9</f>
         <v>Requerimientos</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="10"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="85"/>
     </row>
     <row r="27" spans="2:4">
-      <c r="B27" s="19" t="str">
+      <c r="B27" s="88" t="str">
         <f>Productos!A13</f>
         <v>Plan de proyecto</v>
       </c>
-      <c r="C27" s="20">
+      <c r="C27" s="89">
         <f>COUNTA(Productos!C15:C31)</f>
         <v>0</v>
       </c>
-      <c r="D27" s="10" t="e">
+      <c r="D27" s="85" t="e">
         <f>COUNTIF(Productos!C15:C31,"x")/(COUNTIF((Productos!C15:C31),"x")+COUNTIF((Productos!D15:D31),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="82" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="89">
+        <f>COUNTA(Productos!C35:C37)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="85" t="e">
+        <f>COUNTIF(Productos!C35:C37,"x")/(COUNTIF((Productos!C35:C37),"x")+COUNTIF((Productos!D35:D37),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1454,22 +1546,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="62" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65" t="s">
+      <c r="D1" s="67"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="69" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="68"/>
-      <c r="B2" s="69"/>
+      <c r="A2" s="72"/>
+      <c r="B2" s="73"/>
       <c r="C2" s="14" t="s">
         <v>14</v>
       </c>
@@ -1479,7 +1571,7 @@
       <c r="E2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="65"/>
+      <c r="F2" s="69"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="37">
@@ -1532,22 +1624,22 @@
     <row r="7" spans="1:6" s="15" customFormat="1"/>
     <row r="8" spans="1:6" s="15" customFormat="1"/>
     <row r="9" spans="1:6" s="15" customFormat="1">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="71"/>
-      <c r="C9" s="72" t="s">
+      <c r="B9" s="63"/>
+      <c r="C9" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="73"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="65"/>
       <c r="F9" s="74" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="15" customFormat="1">
-      <c r="A10" s="71"/>
-      <c r="B10" s="71"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="36" t="s">
         <v>9</v>
       </c>
@@ -1658,22 +1750,22 @@
     <row r="19" spans="1:6" s="15" customFormat="1"/>
     <row r="20" spans="1:6" s="15" customFormat="1"/>
     <row r="21" spans="1:6" s="15" customFormat="1">
-      <c r="A21" s="71" t="s">
+      <c r="A21" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="71"/>
-      <c r="C21" s="72" t="s">
+      <c r="B21" s="63"/>
+      <c r="C21" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="72"/>
-      <c r="E21" s="73"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="65"/>
       <c r="F21" s="74" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="15" customFormat="1">
-      <c r="A22" s="71"/>
-      <c r="B22" s="71"/>
+      <c r="A22" s="63"/>
+      <c r="B22" s="63"/>
       <c r="C22" s="31" t="s">
         <v>9</v>
       </c>
@@ -1748,22 +1840,22 @@
     <row r="28" spans="1:6" s="15" customFormat="1"/>
     <row r="29" spans="1:6" s="15" customFormat="1"/>
     <row r="30" spans="1:6" s="15" customFormat="1">
-      <c r="A30" s="71" t="s">
+      <c r="A30" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="71"/>
-      <c r="C30" s="72" t="s">
+      <c r="B30" s="63"/>
+      <c r="C30" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="72"/>
-      <c r="E30" s="73"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="65"/>
       <c r="F30" s="74" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="15" customFormat="1">
-      <c r="A31" s="71"/>
-      <c r="B31" s="71"/>
+      <c r="A31" s="63"/>
+      <c r="B31" s="63"/>
       <c r="C31" s="32" t="s">
         <v>9</v>
       </c>
@@ -1827,22 +1919,22 @@
     <row r="37" spans="1:6" s="15" customFormat="1"/>
     <row r="38" spans="1:6" s="15" customFormat="1"/>
     <row r="39" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A39" s="71" t="s">
+      <c r="A39" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="71"/>
-      <c r="C39" s="72" t="s">
+      <c r="B39" s="63"/>
+      <c r="C39" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="72"/>
-      <c r="E39" s="73"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="65"/>
       <c r="F39" s="74" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A40" s="71"/>
-      <c r="B40" s="71"/>
+      <c r="A40" s="63"/>
+      <c r="B40" s="63"/>
       <c r="C40" s="36" t="s">
         <v>9</v>
       </c>
@@ -1904,28 +1996,28 @@
     </row>
     <row r="45" spans="1:6" s="15" customFormat="1"/>
     <row r="46" spans="1:6" s="15" customFormat="1">
-      <c r="B46" s="70"/>
-      <c r="C46" s="70"/>
-      <c r="D46" s="70"/>
-      <c r="E46" s="70"/>
+      <c r="B46" s="62"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="62"/>
+      <c r="E46" s="62"/>
     </row>
     <row r="47" spans="1:6" s="15" customFormat="1">
-      <c r="A47" s="71" t="s">
+      <c r="A47" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="71"/>
-      <c r="C47" s="72" t="s">
+      <c r="B47" s="63"/>
+      <c r="C47" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="72"/>
-      <c r="E47" s="73"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="65"/>
       <c r="F47" s="74" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="15" customFormat="1">
-      <c r="A48" s="71"/>
-      <c r="B48" s="71"/>
+      <c r="A48" s="63"/>
+      <c r="B48" s="63"/>
       <c r="C48" s="36" t="s">
         <v>9</v>
       </c>
@@ -2006,16 +2098,16 @@
     <row r="60" spans="1:6" s="15" customFormat="1"/>
     <row r="61" spans="1:6" s="15" customFormat="1"/>
     <row r="62" spans="1:6" s="15" customFormat="1"/>
-    <row r="63" spans="1:6" s="15" customFormat="1" ht="409.6"/>
+    <row r="63" spans="1:6" s="15" customFormat="1"/>
     <row r="64" spans="1:6" s="15" customFormat="1"/>
     <row r="65" spans="2:5" s="15" customFormat="1"/>
     <row r="66" spans="2:5" s="15" customFormat="1"/>
     <row r="67" spans="2:5" s="15" customFormat="1"/>
     <row r="68" spans="2:5" s="15" customFormat="1">
-      <c r="B68" s="70"/>
-      <c r="C68" s="70"/>
-      <c r="D68" s="70"/>
-      <c r="E68" s="70"/>
+      <c r="B68" s="62"/>
+      <c r="C68" s="62"/>
+      <c r="D68" s="62"/>
+      <c r="E68" s="62"/>
     </row>
     <row r="69" spans="2:5" s="15" customFormat="1"/>
     <row r="70" spans="2:5" s="15" customFormat="1">
@@ -2033,10 +2125,10 @@
     <row r="78" spans="2:5" s="15" customFormat="1"/>
     <row r="79" spans="2:5" s="15" customFormat="1"/>
     <row r="80" spans="2:5" s="15" customFormat="1">
-      <c r="B80" s="70"/>
-      <c r="C80" s="70"/>
-      <c r="D80" s="70"/>
-      <c r="E80" s="70"/>
+      <c r="B80" s="62"/>
+      <c r="C80" s="62"/>
+      <c r="D80" s="62"/>
+      <c r="E80" s="62"/>
     </row>
     <row r="81" spans="2:5" s="15" customFormat="1"/>
     <row r="82" spans="2:5" s="15" customFormat="1">
@@ -2058,10 +2150,10 @@
     <row r="94" spans="2:5" s="15" customFormat="1"/>
     <row r="95" spans="2:5" s="15" customFormat="1"/>
     <row r="96" spans="2:5" s="15" customFormat="1">
-      <c r="B96" s="70"/>
-      <c r="C96" s="70"/>
-      <c r="D96" s="70"/>
-      <c r="E96" s="70"/>
+      <c r="B96" s="62"/>
+      <c r="C96" s="62"/>
+      <c r="D96" s="62"/>
+      <c r="E96" s="62"/>
     </row>
     <row r="97" spans="3:5" s="15" customFormat="1"/>
     <row r="98" spans="3:5" s="15" customFormat="1">
@@ -2164,12 +2256,6 @@
     <row r="191" s="15" customFormat="1"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B96:E96"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="A9:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="C21:E21"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:B2"/>
@@ -2186,6 +2272,12 @@
     <mergeCell ref="A47:B48"/>
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="F47:F48"/>
+    <mergeCell ref="B96:E96"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="A9:B10"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="C21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2195,10 +2287,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ33"/>
+  <dimension ref="A1:AMJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2208,22 +2300,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="72" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="73"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="65"/>
       <c r="F1" s="74" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1024">
-      <c r="A2" s="71"/>
-      <c r="B2" s="71"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
       <c r="C2" s="31" t="s">
         <v>9</v>
       </c>
@@ -2304,22 +2396,22 @@
       <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:1024" ht="15" customHeight="1">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="71"/>
-      <c r="C9" s="72" t="s">
+      <c r="B9" s="63"/>
+      <c r="C9" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="73"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="65"/>
       <c r="F9" s="74" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:1024" ht="15" customHeight="1">
-      <c r="A10" s="71"/>
-      <c r="B10" s="71"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="31" t="s">
         <v>9</v>
       </c>
@@ -2352,15 +2444,15 @@
       <c r="F12" s="34"/>
     </row>
     <row r="13" spans="1:1024" ht="15" customHeight="1">
-      <c r="A13" s="71" t="s">
+      <c r="A13" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="71"/>
-      <c r="C13" s="72" t="s">
+      <c r="B13" s="63"/>
+      <c r="C13" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="72"/>
-      <c r="E13" s="73"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="65"/>
       <c r="F13" s="74" t="s">
         <v>13</v>
       </c>
@@ -3384,8 +3476,8 @@
       <c r="AMJ13" s="12"/>
     </row>
     <row r="14" spans="1:1024" ht="15" customHeight="1">
-      <c r="A14" s="71"/>
-      <c r="B14" s="71"/>
+      <c r="A14" s="63"/>
+      <c r="B14" s="63"/>
       <c r="C14" s="31" t="s">
         <v>9</v>
       </c>
@@ -21925,13 +22017,75 @@
       <c r="AMI31" s="12"/>
       <c r="AMJ31" s="12"/>
     </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="77" t="s">
+    <row r="33" spans="1:6">
+      <c r="A33" s="79" t="s">
         <v>79</v>
       </c>
+      <c r="B33" s="79"/>
+      <c r="C33" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="81" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="79"/>
+      <c r="B34" s="79"/>
+      <c r="C34" s="78" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="78" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="78" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" s="81"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="58">
+        <v>1</v>
+      </c>
+      <c r="B35" s="77" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="58">
+        <v>2</v>
+      </c>
+      <c r="B36" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="58">
+        <v>3</v>
+      </c>
+      <c r="B37" s="77" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="A33:B34"/>
+    <mergeCell ref="F33:F34"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="A13:B14"/>
     <mergeCell ref="C13:E13"/>

</xml_diff>

<commit_message>
Actualizacion check list de calidad (carta de aceptacion)
</commit_message>
<xml_diff>
--- a/Organización/Calidad/PTL_Checklist_Calidad_aammdd.xlsx
+++ b/Organización/Calidad/PTL_Checklist_Calidad_aammdd.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095"/>
+    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="86">
   <si>
     <t>DATOS GENERALES</t>
   </si>
@@ -261,16 +261,19 @@
     <t>¿Tiene definido el nombre del cliente atendido?</t>
   </si>
   <si>
-    <t>¿Se tiene especificado el inconveniente que fue resuelto?</t>
-  </si>
-  <si>
-    <t>¿Se cuenta con las respuestas solicitadas al cliente?</t>
-  </si>
-  <si>
     <t>No aplica</t>
   </si>
   <si>
     <t>Carta de aceptación</t>
+  </si>
+  <si>
+    <t>¿Se tiene especificado el software/hardware entregado?</t>
+  </si>
+  <si>
+    <t>¿Se tiene especificada la necesidad del cliente?</t>
+  </si>
+  <si>
+    <t>¿La carta de aceptación tiene las respuestas de servicio por parte del cliente, es decir el clietne definió el tipo de servicio y trato recibido?</t>
   </si>
 </sst>
 </file>
@@ -862,22 +865,40 @@
     <xf numFmtId="165" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="14" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="14" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="14" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="14" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="14" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="8" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -903,6 +924,16 @@
     <xf numFmtId="165" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -912,42 +943,14 @@
     <xf numFmtId="165" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="165" fontId="10" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="10" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="10" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="14" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="14" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="14" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="14" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="14" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="14" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1267,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1287,66 +1290,66 @@
     <row r="1" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="2"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
     </row>
     <row r="4" spans="1:6" ht="15.75">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
     </row>
     <row r="6" spans="1:6" ht="13.9" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="12" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
       <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1">
@@ -1445,11 +1448,11 @@
     <row r="21" spans="2:4" s="5" customFormat="1" ht="12.75"/>
     <row r="22" spans="2:4" s="5" customFormat="1" ht="12.75"/>
     <row r="23" spans="2:4" ht="15.75">
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="6" t="s">
@@ -1463,51 +1466,51 @@
       </c>
     </row>
     <row r="25" spans="2:4">
-      <c r="B25" s="83" t="str">
+      <c r="B25" s="62" t="str">
         <f>Productos!A1</f>
         <v>Estimación</v>
       </c>
-      <c r="C25" s="84">
+      <c r="C25" s="63">
         <f>COUNTA(Productos!C3:C7)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="85" t="e">
+      <c r="D25" s="64" t="e">
         <f>COUNTIF(Productos!C3:C7,"x")/(COUNTIF((Productos!C3:C7),"x")+COUNTIF((Productos!D3:D7),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26" s="86" t="str">
+      <c r="B26" s="65" t="str">
         <f>Productos!A9</f>
         <v>Requerimientos</v>
       </c>
-      <c r="C26" s="87"/>
-      <c r="D26" s="85"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="64"/>
     </row>
     <row r="27" spans="2:4">
-      <c r="B27" s="88" t="str">
+      <c r="B27" s="67" t="str">
         <f>Productos!A13</f>
         <v>Plan de proyecto</v>
       </c>
-      <c r="C27" s="89">
+      <c r="C27" s="68">
         <f>COUNTA(Productos!C15:C31)</f>
         <v>0</v>
       </c>
-      <c r="D27" s="85" t="e">
+      <c r="D27" s="64" t="e">
         <f>COUNTIF(Productos!C15:C31,"x")/(COUNTIF((Productos!C15:C31),"x")+COUNTIF((Productos!D15:D31),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28" s="82" t="s">
-        <v>84</v>
+      <c r="B28" s="61" t="s">
+        <v>82</v>
       </c>
-      <c r="C28" s="89">
+      <c r="C28" s="68">
         <f>COUNTA(Productos!C35:C37)</f>
         <v>0</v>
       </c>
-      <c r="D28" s="85" t="e">
-        <f>COUNTIF(Productos!C35:C37,"x")/(COUNTIF((Productos!C35:C37),"x")+COUNTIF((Productos!D35:D37),"x"))</f>
+      <c r="D28" s="64" t="e">
+        <f>COUNTIF(Productos!C35:C38,"x")/(COUNTIF((Productos!C35:C38),"x")+COUNTIF((Productos!D35:D38),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1533,7 +1536,7 @@
   <dimension ref="A1:AMI191"/>
   <sheetViews>
     <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1546,22 +1549,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="66" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="67"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="69" t="s">
+      <c r="D1" s="73"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="75" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="72"/>
-      <c r="B2" s="73"/>
+      <c r="A2" s="78"/>
+      <c r="B2" s="79"/>
       <c r="C2" s="14" t="s">
         <v>14</v>
       </c>
@@ -1571,7 +1574,7 @@
       <c r="E2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="69"/>
+      <c r="F2" s="75"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="37">
@@ -1624,22 +1627,22 @@
     <row r="7" spans="1:6" s="15" customFormat="1"/>
     <row r="8" spans="1:6" s="15" customFormat="1"/>
     <row r="9" spans="1:6" s="15" customFormat="1">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="64" t="s">
+      <c r="B9" s="81"/>
+      <c r="C9" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="64"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="74" t="s">
+      <c r="D9" s="82"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="84" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="15" customFormat="1">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
+      <c r="A10" s="81"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="36" t="s">
         <v>9</v>
       </c>
@@ -1649,7 +1652,7 @@
       <c r="E10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="75"/>
+      <c r="F10" s="85"/>
     </row>
     <row r="11" spans="1:6" s="15" customFormat="1">
       <c r="A11" s="24">
@@ -1750,22 +1753,22 @@
     <row r="19" spans="1:6" s="15" customFormat="1"/>
     <row r="20" spans="1:6" s="15" customFormat="1"/>
     <row r="21" spans="1:6" s="15" customFormat="1">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="64" t="s">
+      <c r="B21" s="81"/>
+      <c r="C21" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="64"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="74" t="s">
+      <c r="D21" s="82"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="84" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="15" customFormat="1">
-      <c r="A22" s="63"/>
-      <c r="B22" s="63"/>
+      <c r="A22" s="81"/>
+      <c r="B22" s="81"/>
       <c r="C22" s="31" t="s">
         <v>9</v>
       </c>
@@ -1775,7 +1778,7 @@
       <c r="E22" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="76"/>
+      <c r="F22" s="86"/>
     </row>
     <row r="23" spans="1:6" s="15" customFormat="1">
       <c r="A23" s="47">
@@ -1840,22 +1843,22 @@
     <row r="28" spans="1:6" s="15" customFormat="1"/>
     <row r="29" spans="1:6" s="15" customFormat="1"/>
     <row r="30" spans="1:6" s="15" customFormat="1">
-      <c r="A30" s="63" t="s">
+      <c r="A30" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="63"/>
-      <c r="C30" s="64" t="s">
+      <c r="B30" s="81"/>
+      <c r="C30" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="64"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="74" t="s">
+      <c r="D30" s="82"/>
+      <c r="E30" s="83"/>
+      <c r="F30" s="84" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="15" customFormat="1">
-      <c r="A31" s="63"/>
-      <c r="B31" s="63"/>
+      <c r="A31" s="81"/>
+      <c r="B31" s="81"/>
       <c r="C31" s="32" t="s">
         <v>9</v>
       </c>
@@ -1865,7 +1868,7 @@
       <c r="E31" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="76"/>
+      <c r="F31" s="86"/>
     </row>
     <row r="32" spans="1:6" s="15" customFormat="1">
       <c r="A32" s="47">
@@ -1919,22 +1922,22 @@
     <row r="37" spans="1:6" s="15" customFormat="1"/>
     <row r="38" spans="1:6" s="15" customFormat="1"/>
     <row r="39" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A39" s="63" t="s">
+      <c r="A39" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="63"/>
-      <c r="C39" s="64" t="s">
+      <c r="B39" s="81"/>
+      <c r="C39" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="64"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="74" t="s">
+      <c r="D39" s="82"/>
+      <c r="E39" s="83"/>
+      <c r="F39" s="84" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A40" s="63"/>
-      <c r="B40" s="63"/>
+      <c r="A40" s="81"/>
+      <c r="B40" s="81"/>
       <c r="C40" s="36" t="s">
         <v>9</v>
       </c>
@@ -1944,7 +1947,7 @@
       <c r="E40" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F40" s="75"/>
+      <c r="F40" s="85"/>
     </row>
     <row r="41" spans="1:6" s="15" customFormat="1">
       <c r="A41" s="24">
@@ -1996,28 +1999,28 @@
     </row>
     <row r="45" spans="1:6" s="15" customFormat="1"/>
     <row r="46" spans="1:6" s="15" customFormat="1">
-      <c r="B46" s="62"/>
-      <c r="C46" s="62"/>
-      <c r="D46" s="62"/>
-      <c r="E46" s="62"/>
+      <c r="B46" s="80"/>
+      <c r="C46" s="80"/>
+      <c r="D46" s="80"/>
+      <c r="E46" s="80"/>
     </row>
     <row r="47" spans="1:6" s="15" customFormat="1">
-      <c r="A47" s="63" t="s">
+      <c r="A47" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="63"/>
-      <c r="C47" s="64" t="s">
+      <c r="B47" s="81"/>
+      <c r="C47" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="64"/>
-      <c r="E47" s="65"/>
-      <c r="F47" s="74" t="s">
+      <c r="D47" s="82"/>
+      <c r="E47" s="83"/>
+      <c r="F47" s="84" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="15" customFormat="1">
-      <c r="A48" s="63"/>
-      <c r="B48" s="63"/>
+      <c r="A48" s="81"/>
+      <c r="B48" s="81"/>
       <c r="C48" s="36" t="s">
         <v>9</v>
       </c>
@@ -2027,7 +2030,7 @@
       <c r="E48" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F48" s="75"/>
+      <c r="F48" s="85"/>
     </row>
     <row r="49" spans="1:6" s="15" customFormat="1">
       <c r="A49" s="24">
@@ -2104,10 +2107,10 @@
     <row r="66" spans="2:5" s="15" customFormat="1"/>
     <row r="67" spans="2:5" s="15" customFormat="1"/>
     <row r="68" spans="2:5" s="15" customFormat="1">
-      <c r="B68" s="62"/>
-      <c r="C68" s="62"/>
-      <c r="D68" s="62"/>
-      <c r="E68" s="62"/>
+      <c r="B68" s="80"/>
+      <c r="C68" s="80"/>
+      <c r="D68" s="80"/>
+      <c r="E68" s="80"/>
     </row>
     <row r="69" spans="2:5" s="15" customFormat="1"/>
     <row r="70" spans="2:5" s="15" customFormat="1">
@@ -2125,10 +2128,10 @@
     <row r="78" spans="2:5" s="15" customFormat="1"/>
     <row r="79" spans="2:5" s="15" customFormat="1"/>
     <row r="80" spans="2:5" s="15" customFormat="1">
-      <c r="B80" s="62"/>
-      <c r="C80" s="62"/>
-      <c r="D80" s="62"/>
-      <c r="E80" s="62"/>
+      <c r="B80" s="80"/>
+      <c r="C80" s="80"/>
+      <c r="D80" s="80"/>
+      <c r="E80" s="80"/>
     </row>
     <row r="81" spans="2:5" s="15" customFormat="1"/>
     <row r="82" spans="2:5" s="15" customFormat="1">
@@ -2150,10 +2153,10 @@
     <row r="94" spans="2:5" s="15" customFormat="1"/>
     <row r="95" spans="2:5" s="15" customFormat="1"/>
     <row r="96" spans="2:5" s="15" customFormat="1">
-      <c r="B96" s="62"/>
-      <c r="C96" s="62"/>
-      <c r="D96" s="62"/>
-      <c r="E96" s="62"/>
+      <c r="B96" s="80"/>
+      <c r="C96" s="80"/>
+      <c r="D96" s="80"/>
+      <c r="E96" s="80"/>
     </row>
     <row r="97" spans="3:5" s="15" customFormat="1"/>
     <row r="98" spans="3:5" s="15" customFormat="1">
@@ -2256,6 +2259,12 @@
     <row r="191" s="15" customFormat="1"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B96:E96"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="A9:B10"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="C21:E21"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:B2"/>
@@ -2272,12 +2281,6 @@
     <mergeCell ref="A47:B48"/>
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="F47:F48"/>
-    <mergeCell ref="B96:E96"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="A9:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="C21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2287,10 +2290,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ37"/>
+  <dimension ref="A1:AMJ38"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2300,22 +2303,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="64" t="s">
+      <c r="B1" s="81"/>
+      <c r="C1" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="74" t="s">
+      <c r="D1" s="82"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="84" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1024">
-      <c r="A2" s="63"/>
-      <c r="B2" s="63"/>
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
       <c r="C2" s="31" t="s">
         <v>9</v>
       </c>
@@ -2325,7 +2328,7 @@
       <c r="E2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="76"/>
+      <c r="F2" s="86"/>
     </row>
     <row r="3" spans="1:1024" ht="30">
       <c r="A3" s="50">
@@ -2396,22 +2399,22 @@
       <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:1024" ht="15" customHeight="1">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="64" t="s">
+      <c r="B9" s="81"/>
+      <c r="C9" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="64"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="74" t="s">
+      <c r="D9" s="82"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="84" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:1024" ht="15" customHeight="1">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
+      <c r="A10" s="81"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="31" t="s">
         <v>9</v>
       </c>
@@ -2421,7 +2424,7 @@
       <c r="E10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="76"/>
+      <c r="F10" s="86"/>
     </row>
     <row r="11" spans="1:1024" ht="30">
       <c r="A11" s="50">
@@ -2444,16 +2447,16 @@
       <c r="F12" s="34"/>
     </row>
     <row r="13" spans="1:1024" ht="15" customHeight="1">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="64" t="s">
+      <c r="B13" s="81"/>
+      <c r="C13" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="64"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="74" t="s">
+      <c r="D13" s="82"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="84" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="12"/>
@@ -3476,8 +3479,8 @@
       <c r="AMJ13" s="12"/>
     </row>
     <row r="14" spans="1:1024" ht="15" customHeight="1">
-      <c r="A14" s="63"/>
-      <c r="B14" s="63"/>
+      <c r="A14" s="81"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="31" t="s">
         <v>9</v>
       </c>
@@ -3487,7 +3490,7 @@
       <c r="E14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="76"/>
+      <c r="F14" s="86"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
@@ -22018,38 +22021,38 @@
       <c r="AMJ31" s="12"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="79" t="s">
+      <c r="A33" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="B33" s="79"/>
-      <c r="C33" s="80" t="s">
+      <c r="B33" s="88"/>
+      <c r="C33" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="80"/>
-      <c r="E33" s="80"/>
-      <c r="F33" s="81" t="s">
+      <c r="D33" s="87"/>
+      <c r="E33" s="87"/>
+      <c r="F33" s="89" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="79"/>
-      <c r="B34" s="79"/>
-      <c r="C34" s="78" t="s">
+      <c r="A34" s="88"/>
+      <c r="B34" s="88"/>
+      <c r="C34" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="78" t="s">
+      <c r="D34" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="78" t="s">
-        <v>83</v>
+      <c r="E34" s="60" t="s">
+        <v>81</v>
       </c>
-      <c r="F34" s="81"/>
+      <c r="F34" s="89"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="58">
         <v>1</v>
       </c>
-      <c r="B35" s="77" t="s">
+      <c r="B35" s="59" t="s">
         <v>80</v>
       </c>
       <c r="C35" s="57"/>
@@ -22061,40 +22064,52 @@
       <c r="A36" s="58">
         <v>2</v>
       </c>
-      <c r="B36" s="77" t="s">
-        <v>81</v>
+      <c r="B36" s="59" t="s">
+        <v>84</v>
       </c>
       <c r="C36" s="57"/>
       <c r="D36" s="57"/>
       <c r="E36" s="57"/>
       <c r="F36" s="57"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" ht="30">
       <c r="A37" s="58">
         <v>3</v>
       </c>
-      <c r="B37" s="77" t="s">
-        <v>82</v>
+      <c r="B37" s="54" t="s">
+        <v>85</v>
       </c>
       <c r="C37" s="57"/>
       <c r="D37" s="57"/>
       <c r="E37" s="57"/>
       <c r="F37" s="57"/>
     </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="58">
+        <v>4</v>
+      </c>
+      <c r="B38" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A9:B10"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:F10"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="A33:B34"/>
     <mergeCell ref="F33:F34"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="A13:B14"/>
     <mergeCell ref="C13:E13"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A9:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Check list de calidad actualizado
</commit_message>
<xml_diff>
--- a/Organización/Calidad/PTL_Checklist_Calidad_aammdd.xlsx
+++ b/Organización/Calidad/PTL_Checklist_Calidad_aammdd.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095" activeTab="2"/>
+    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
     <sheet name="procesos" sheetId="5" r:id="rId2"/>
     <sheet name="Productos" sheetId="7" r:id="rId3"/>
+    <sheet name="Física" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="109">
   <si>
     <t>DATOS GENERALES</t>
   </si>
@@ -255,9 +256,6 @@
     <t>¿Todas las tareas solucionadas estan cerradas?</t>
   </si>
   <si>
-    <t>carta de aceptación</t>
-  </si>
-  <si>
     <t>¿Tiene definido el nombre del cliente atendido?</t>
   </si>
   <si>
@@ -275,6 +273,78 @@
   <si>
     <t>¿La carta de aceptación tiene las respuestas de servicio por parte del cliente, es decir el clietne definió el tipo de servicio y trato recibido?</t>
   </si>
+  <si>
+    <t>Verificación</t>
+  </si>
+  <si>
+    <t>Elementos de Configuración</t>
+  </si>
+  <si>
+    <t>Línea Base</t>
+  </si>
+  <si>
+    <t>¿Se tiene identificada la versión de las linea base en los documentos?</t>
+  </si>
+  <si>
+    <t>¿Están identificados los elementos de configuración que forman parte de la Línea Base?</t>
+  </si>
+  <si>
+    <t>¿Los elementos de configuración que forman parte de la Línea Base se encuentran aprobados por el cliente?</t>
+  </si>
+  <si>
+    <t>Control de Cambios</t>
+  </si>
+  <si>
+    <t>¿Los elementos de configuración respetan la ubicación física definida en el documento Plan Configuración?</t>
+  </si>
+  <si>
+    <t>¿Los elementos de configuración respetan el nombrado establecido en el documento Plan configuración?</t>
+  </si>
+  <si>
+    <t>¿Se indicó el cambio dentro de los elementos de configuración afectados por un cambio?</t>
+  </si>
+  <si>
+    <t>¿Se actualizarón apropiadamente los elementos de configuración afectados por algún cambio?</t>
+  </si>
+  <si>
+    <t>¿Se actualizó la versión y el contenido de los documentos pertenecientes a la linea base ante algún cambio que afectara su estructura?</t>
+  </si>
+  <si>
+    <t>Física</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket de servicio </t>
+  </si>
+  <si>
+    <t>¿Se asignó un responsable por ticket?</t>
+  </si>
+  <si>
+    <t>¿Todos los tickets cuentan con un nombre descriptivo?</t>
+  </si>
+  <si>
+    <t>¿Todos los tickets cuentan con una descripción?</t>
+  </si>
+  <si>
+    <t>¿Cada ticket cuenta con un creador?</t>
+  </si>
+  <si>
+    <t>¿Todos los tickets tienen un estado de ejecución?</t>
+  </si>
+  <si>
+    <t>¿Todos los tickets cerrados muestran hora definalización?</t>
+  </si>
+  <si>
+    <t>¿Cada ticket tiene una prioridad de ejecución?</t>
+  </si>
+  <si>
+    <t>¿Todos los tickets tienen registrada una fecha de creación?</t>
+  </si>
+  <si>
+    <t>¿Todos los tickets tienen un tiempo de duración utilizado para su resolución?</t>
+  </si>
+  <si>
+    <t>Tickets de Servicio</t>
+  </si>
 </sst>
 </file>
 
@@ -286,7 +356,7 @@
     <numFmt numFmtId="166" formatCode="[$-80A]0%"/>
     <numFmt numFmtId="167" formatCode="[$$-80A]#,##0.00;[Red]&quot;-&quot;[$$-80A]#,##0.00"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -381,8 +451,19 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="American Typewriter"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="American Typewriter"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,8 +572,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -692,8 +797,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0">
@@ -706,8 +822,9 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="114">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -893,6 +1010,30 @@
     <xf numFmtId="165" fontId="8" fillId="14" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -946,19 +1087,62 @@
     <xf numFmtId="165" fontId="10" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="10" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="21" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="20" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="21" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="22" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="18" borderId="11" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="ConditionalStyle_1" xfId="1"/>
     <cellStyle name="Heading" xfId="2"/>
     <cellStyle name="Heading1" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 3" xfId="4"/>
+    <cellStyle name="Porcentaje" xfId="8" builtinId="5"/>
     <cellStyle name="Porcentaje 2" xfId="5"/>
     <cellStyle name="Result" xfId="6"/>
     <cellStyle name="Result2" xfId="7"/>
@@ -1268,10 +1452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ28"/>
+  <dimension ref="A1:AMJ35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1290,66 +1474,66 @@
     <row r="1" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="2"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
     </row>
     <row r="4" spans="1:6" ht="15.75">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
     </row>
     <row r="6" spans="1:6" ht="13.9" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="12" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B12" s="69" t="s">
+      <c r="B12" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
       <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1">
@@ -1448,11 +1632,11 @@
     <row r="21" spans="2:4" s="5" customFormat="1" ht="12.75"/>
     <row r="22" spans="2:4" s="5" customFormat="1" ht="12.75"/>
     <row r="23" spans="2:4" ht="15.75">
-      <c r="B23" s="69" t="s">
+      <c r="B23" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="77"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="6" t="s">
@@ -1503,7 +1687,7 @@
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C28" s="68">
         <f>COUNTA(Productos!C35:C37)</f>
@@ -1514,8 +1698,82 @@
         <v>#DIV/0!</v>
       </c>
     </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="61" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="68">
+        <f>COUNTA(Productos!C43:C51)</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="64" t="e">
+        <f>COUNTIF(Productos!C43:C51,"x")/(COUNTIF((Productos!C43:C51),"x")+COUNTIF((Productos!D43:D51),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="18">
+      <c r="B31" s="110" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="110"/>
+      <c r="D31" s="110"/>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="111" t="str">
+        <f>Física!A3</f>
+        <v>Elementos de Configuración</v>
+      </c>
+      <c r="C33" s="112">
+        <f>COUNTA(Física!C4:C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="113" t="e">
+        <f>COUNTIF(Física!C4:C7,"x")/(COUNTIF((Física!C4:C7),"x")+COUNTIF((Física!D4:D7),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="111" t="str">
+        <f>Física!A8</f>
+        <v>Línea Base</v>
+      </c>
+      <c r="C34" s="112">
+        <f>COUNTA(Física!C9:C12)</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="113" t="e">
+        <f>COUNTIF(Física!C9:C12,"x")/(COUNTIF((Física!C9:C12),"x")+COUNTIF((Física!D9:D12),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="111" t="str">
+        <f>Física!A13</f>
+        <v>Control de Cambios</v>
+      </c>
+      <c r="C35" s="112">
+        <f>COUNTA(Física!C14:C14)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="113" t="e">
+        <f>COUNTIF(Física!C14:C14,"x")/(COUNTIF((Física!C14:C14),"x")+COUNTIF((Física!D14:D14),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="B31:D31"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B2:F2"/>
@@ -1526,7 +1784,7 @@
     <mergeCell ref="C8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
-  <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -1535,7 +1793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMI191"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
@@ -1549,22 +1807,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="72" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="73"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="75" t="s">
+      <c r="D1" s="81"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="83" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="78"/>
-      <c r="B2" s="79"/>
+      <c r="A2" s="86"/>
+      <c r="B2" s="87"/>
       <c r="C2" s="14" t="s">
         <v>14</v>
       </c>
@@ -1574,7 +1832,7 @@
       <c r="E2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="75"/>
+      <c r="F2" s="83"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="37">
@@ -1627,22 +1885,22 @@
     <row r="7" spans="1:6" s="15" customFormat="1"/>
     <row r="8" spans="1:6" s="15" customFormat="1"/>
     <row r="9" spans="1:6" s="15" customFormat="1">
-      <c r="A9" s="81" t="s">
+      <c r="A9" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="81"/>
-      <c r="C9" s="82" t="s">
+      <c r="B9" s="89"/>
+      <c r="C9" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="84" t="s">
+      <c r="D9" s="90"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="92" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="15" customFormat="1">
-      <c r="A10" s="81"/>
-      <c r="B10" s="81"/>
+      <c r="A10" s="89"/>
+      <c r="B10" s="89"/>
       <c r="C10" s="36" t="s">
         <v>9</v>
       </c>
@@ -1652,7 +1910,7 @@
       <c r="E10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="85"/>
+      <c r="F10" s="93"/>
     </row>
     <row r="11" spans="1:6" s="15" customFormat="1">
       <c r="A11" s="24">
@@ -1753,22 +2011,22 @@
     <row r="19" spans="1:6" s="15" customFormat="1"/>
     <row r="20" spans="1:6" s="15" customFormat="1"/>
     <row r="21" spans="1:6" s="15" customFormat="1">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="81"/>
-      <c r="C21" s="82" t="s">
+      <c r="B21" s="89"/>
+      <c r="C21" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="82"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="84" t="s">
+      <c r="D21" s="90"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="92" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="15" customFormat="1">
-      <c r="A22" s="81"/>
-      <c r="B22" s="81"/>
+      <c r="A22" s="89"/>
+      <c r="B22" s="89"/>
       <c r="C22" s="31" t="s">
         <v>9</v>
       </c>
@@ -1778,7 +2036,7 @@
       <c r="E22" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="86"/>
+      <c r="F22" s="94"/>
     </row>
     <row r="23" spans="1:6" s="15" customFormat="1">
       <c r="A23" s="47">
@@ -1843,22 +2101,22 @@
     <row r="28" spans="1:6" s="15" customFormat="1"/>
     <row r="29" spans="1:6" s="15" customFormat="1"/>
     <row r="30" spans="1:6" s="15" customFormat="1">
-      <c r="A30" s="81" t="s">
+      <c r="A30" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="81"/>
-      <c r="C30" s="82" t="s">
+      <c r="B30" s="89"/>
+      <c r="C30" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="82"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="84" t="s">
+      <c r="D30" s="90"/>
+      <c r="E30" s="91"/>
+      <c r="F30" s="92" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="15" customFormat="1">
-      <c r="A31" s="81"/>
-      <c r="B31" s="81"/>
+      <c r="A31" s="89"/>
+      <c r="B31" s="89"/>
       <c r="C31" s="32" t="s">
         <v>9</v>
       </c>
@@ -1868,7 +2126,7 @@
       <c r="E31" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="86"/>
+      <c r="F31" s="94"/>
     </row>
     <row r="32" spans="1:6" s="15" customFormat="1">
       <c r="A32" s="47">
@@ -1922,22 +2180,22 @@
     <row r="37" spans="1:6" s="15" customFormat="1"/>
     <row r="38" spans="1:6" s="15" customFormat="1"/>
     <row r="39" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A39" s="81" t="s">
+      <c r="A39" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="81"/>
-      <c r="C39" s="82" t="s">
+      <c r="B39" s="89"/>
+      <c r="C39" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="82"/>
-      <c r="E39" s="83"/>
-      <c r="F39" s="84" t="s">
+      <c r="D39" s="90"/>
+      <c r="E39" s="91"/>
+      <c r="F39" s="92" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A40" s="81"/>
-      <c r="B40" s="81"/>
+      <c r="A40" s="89"/>
+      <c r="B40" s="89"/>
       <c r="C40" s="36" t="s">
         <v>9</v>
       </c>
@@ -1947,7 +2205,7 @@
       <c r="E40" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F40" s="85"/>
+      <c r="F40" s="93"/>
     </row>
     <row r="41" spans="1:6" s="15" customFormat="1">
       <c r="A41" s="24">
@@ -1999,28 +2257,28 @@
     </row>
     <row r="45" spans="1:6" s="15" customFormat="1"/>
     <row r="46" spans="1:6" s="15" customFormat="1">
-      <c r="B46" s="80"/>
-      <c r="C46" s="80"/>
-      <c r="D46" s="80"/>
-      <c r="E46" s="80"/>
+      <c r="B46" s="88"/>
+      <c r="C46" s="88"/>
+      <c r="D46" s="88"/>
+      <c r="E46" s="88"/>
     </row>
     <row r="47" spans="1:6" s="15" customFormat="1">
-      <c r="A47" s="81" t="s">
+      <c r="A47" s="89" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="81"/>
-      <c r="C47" s="82" t="s">
+      <c r="B47" s="89"/>
+      <c r="C47" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="82"/>
-      <c r="E47" s="83"/>
-      <c r="F47" s="84" t="s">
+      <c r="D47" s="90"/>
+      <c r="E47" s="91"/>
+      <c r="F47" s="92" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="15" customFormat="1">
-      <c r="A48" s="81"/>
-      <c r="B48" s="81"/>
+      <c r="A48" s="89"/>
+      <c r="B48" s="89"/>
       <c r="C48" s="36" t="s">
         <v>9</v>
       </c>
@@ -2030,7 +2288,7 @@
       <c r="E48" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F48" s="85"/>
+      <c r="F48" s="93"/>
     </row>
     <row r="49" spans="1:6" s="15" customFormat="1">
       <c r="A49" s="24">
@@ -2107,10 +2365,10 @@
     <row r="66" spans="2:5" s="15" customFormat="1"/>
     <row r="67" spans="2:5" s="15" customFormat="1"/>
     <row r="68" spans="2:5" s="15" customFormat="1">
-      <c r="B68" s="80"/>
-      <c r="C68" s="80"/>
-      <c r="D68" s="80"/>
-      <c r="E68" s="80"/>
+      <c r="B68" s="88"/>
+      <c r="C68" s="88"/>
+      <c r="D68" s="88"/>
+      <c r="E68" s="88"/>
     </row>
     <row r="69" spans="2:5" s="15" customFormat="1"/>
     <row r="70" spans="2:5" s="15" customFormat="1">
@@ -2128,10 +2386,10 @@
     <row r="78" spans="2:5" s="15" customFormat="1"/>
     <row r="79" spans="2:5" s="15" customFormat="1"/>
     <row r="80" spans="2:5" s="15" customFormat="1">
-      <c r="B80" s="80"/>
-      <c r="C80" s="80"/>
-      <c r="D80" s="80"/>
-      <c r="E80" s="80"/>
+      <c r="B80" s="88"/>
+      <c r="C80" s="88"/>
+      <c r="D80" s="88"/>
+      <c r="E80" s="88"/>
     </row>
     <row r="81" spans="2:5" s="15" customFormat="1"/>
     <row r="82" spans="2:5" s="15" customFormat="1">
@@ -2153,10 +2411,10 @@
     <row r="94" spans="2:5" s="15" customFormat="1"/>
     <row r="95" spans="2:5" s="15" customFormat="1"/>
     <row r="96" spans="2:5" s="15" customFormat="1">
-      <c r="B96" s="80"/>
-      <c r="C96" s="80"/>
-      <c r="D96" s="80"/>
-      <c r="E96" s="80"/>
+      <c r="B96" s="88"/>
+      <c r="C96" s="88"/>
+      <c r="D96" s="88"/>
+      <c r="E96" s="88"/>
     </row>
     <row r="97" spans="3:5" s="15" customFormat="1"/>
     <row r="98" spans="3:5" s="15" customFormat="1">
@@ -2290,10 +2548,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ38"/>
+  <dimension ref="A1:AMJ51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2303,22 +2561,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="82" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="82"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="84" t="s">
+      <c r="D1" s="90"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="92" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1024">
-      <c r="A2" s="81"/>
-      <c r="B2" s="81"/>
+      <c r="A2" s="89"/>
+      <c r="B2" s="89"/>
       <c r="C2" s="31" t="s">
         <v>9</v>
       </c>
@@ -2328,7 +2586,7 @@
       <c r="E2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="86"/>
+      <c r="F2" s="94"/>
     </row>
     <row r="3" spans="1:1024" ht="30">
       <c r="A3" s="50">
@@ -2399,22 +2657,22 @@
       <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:1024" ht="15" customHeight="1">
-      <c r="A9" s="81" t="s">
+      <c r="A9" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="81"/>
-      <c r="C9" s="82" t="s">
+      <c r="B9" s="89"/>
+      <c r="C9" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="84" t="s">
+      <c r="D9" s="90"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="92" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:1024" ht="15" customHeight="1">
-      <c r="A10" s="81"/>
-      <c r="B10" s="81"/>
+      <c r="A10" s="89"/>
+      <c r="B10" s="89"/>
       <c r="C10" s="31" t="s">
         <v>9</v>
       </c>
@@ -2424,7 +2682,7 @@
       <c r="E10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="86"/>
+      <c r="F10" s="94"/>
     </row>
     <row r="11" spans="1:1024" ht="30">
       <c r="A11" s="50">
@@ -2447,16 +2705,16 @@
       <c r="F12" s="34"/>
     </row>
     <row r="13" spans="1:1024" ht="15" customHeight="1">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="81"/>
-      <c r="C13" s="82" t="s">
+      <c r="B13" s="89"/>
+      <c r="C13" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="82"/>
-      <c r="E13" s="83"/>
-      <c r="F13" s="84" t="s">
+      <c r="D13" s="90"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="92" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="12"/>
@@ -3479,8 +3737,8 @@
       <c r="AMJ13" s="12"/>
     </row>
     <row r="14" spans="1:1024" ht="15" customHeight="1">
-      <c r="A14" s="81"/>
-      <c r="B14" s="81"/>
+      <c r="A14" s="89"/>
+      <c r="B14" s="89"/>
       <c r="C14" s="31" t="s">
         <v>9</v>
       </c>
@@ -3490,7 +3748,7 @@
       <c r="E14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="86"/>
+      <c r="F14" s="94"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
@@ -22021,22 +22279,22 @@
       <c r="AMJ31" s="12"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="88" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="88"/>
-      <c r="C33" s="87" t="s">
+      <c r="A33" s="109" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="109"/>
+      <c r="C33" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="89" t="s">
+      <c r="D33" s="95"/>
+      <c r="E33" s="95"/>
+      <c r="F33" s="96" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="88"/>
-      <c r="B34" s="88"/>
+      <c r="A34" s="109"/>
+      <c r="B34" s="109"/>
       <c r="C34" s="60" t="s">
         <v>14</v>
       </c>
@@ -22044,16 +22302,16 @@
         <v>15</v>
       </c>
       <c r="E34" s="60" t="s">
-        <v>81</v>
-      </c>
-      <c r="F34" s="89"/>
+        <v>80</v>
+      </c>
+      <c r="F34" s="96"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="58">
         <v>1</v>
       </c>
       <c r="B35" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C35" s="57"/>
       <c r="D35" s="57"/>
@@ -22065,7 +22323,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="59" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C36" s="57"/>
       <c r="D36" s="57"/>
@@ -22077,7 +22335,7 @@
         <v>3</v>
       </c>
       <c r="B37" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C37" s="57"/>
       <c r="D37" s="57"/>
@@ -22089,15 +22347,152 @@
         <v>4</v>
       </c>
       <c r="B38" s="59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38" s="57"/>
       <c r="D38" s="57"/>
       <c r="E38" s="57"/>
       <c r="F38" s="57"/>
     </row>
+    <row r="41" spans="1:6" ht="15" customHeight="1">
+      <c r="A41" s="104" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" s="104"/>
+      <c r="C41" s="105" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="105"/>
+      <c r="E41" s="105"/>
+      <c r="F41" s="106"/>
+    </row>
+    <row r="42" spans="1:6" ht="15" customHeight="1">
+      <c r="A42" s="104"/>
+      <c r="B42" s="104"/>
+      <c r="C42" s="107" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="107" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="107" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="106"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="58">
+        <v>1</v>
+      </c>
+      <c r="B43" s="108" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43" s="108"/>
+      <c r="D43" s="108"/>
+      <c r="E43" s="108"/>
+      <c r="F43" s="108"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="58">
+        <v>2</v>
+      </c>
+      <c r="B44" s="108" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" s="108"/>
+      <c r="D44" s="108"/>
+      <c r="E44" s="108"/>
+      <c r="F44" s="108"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="58">
+        <v>3</v>
+      </c>
+      <c r="B45" s="108" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="108"/>
+      <c r="D45" s="108"/>
+      <c r="E45" s="108"/>
+      <c r="F45" s="108"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="58">
+        <v>4</v>
+      </c>
+      <c r="B46" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="108"/>
+      <c r="D46" s="108"/>
+      <c r="E46" s="108"/>
+      <c r="F46" s="108"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="58">
+        <v>5</v>
+      </c>
+      <c r="B47" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="108"/>
+      <c r="D47" s="108"/>
+      <c r="E47" s="108"/>
+      <c r="F47" s="108"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="58">
+        <v>6</v>
+      </c>
+      <c r="B48" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="108"/>
+      <c r="D48" s="108"/>
+      <c r="E48" s="108"/>
+      <c r="F48" s="108"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="58">
+        <v>7</v>
+      </c>
+      <c r="B49" s="108" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="108"/>
+      <c r="D49" s="108"/>
+      <c r="E49" s="108"/>
+      <c r="F49" s="108"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="58">
+        <v>8</v>
+      </c>
+      <c r="B50" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="58">
+        <v>9</v>
+      </c>
+      <c r="B51" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="15">
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="A41:B42"/>
+    <mergeCell ref="C41:E41"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:F2"/>
@@ -22114,4 +22509,199 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="49.28515625" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="98" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="83"/>
+      <c r="C1" s="101" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="102"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="83" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="99"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="73" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="83"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="97"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="74"/>
+    </row>
+    <row r="4" spans="1:6" ht="26.25">
+      <c r="A4" s="69">
+        <v>1</v>
+      </c>
+      <c r="B4" s="70" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="72"/>
+    </row>
+    <row r="5" spans="1:6" ht="26.25">
+      <c r="A5" s="69">
+        <v>2</v>
+      </c>
+      <c r="B5" s="70" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="72"/>
+    </row>
+    <row r="6" spans="1:6" ht="26.25">
+      <c r="A6" s="69">
+        <v>3</v>
+      </c>
+      <c r="B6" s="70" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="72"/>
+    </row>
+    <row r="7" spans="1:6" ht="26.25">
+      <c r="A7" s="69">
+        <v>4</v>
+      </c>
+      <c r="B7" s="70" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="97"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="74"/>
+    </row>
+    <row r="9" spans="1:6" ht="26.25">
+      <c r="A9" s="69">
+        <v>4</v>
+      </c>
+      <c r="B9" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="72"/>
+    </row>
+    <row r="10" spans="1:6" ht="26.25">
+      <c r="A10" s="69">
+        <v>5</v>
+      </c>
+      <c r="B10" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="72"/>
+    </row>
+    <row r="11" spans="1:6" ht="26.25">
+      <c r="A11" s="69">
+        <v>6</v>
+      </c>
+      <c r="B11" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="72"/>
+    </row>
+    <row r="12" spans="1:6" ht="39">
+      <c r="A12" s="69">
+        <v>7</v>
+      </c>
+      <c r="B12" s="70" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="72"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="97" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="97"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="74"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="69">
+        <v>8</v>
+      </c>
+      <c r="B14" s="72"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="72"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" s="76"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A8:B8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
actualizacion del check list de calidad
</commit_message>
<xml_diff>
--- a/Organización/Calidad/PTL_Checklist_Calidad_aammdd.xlsx
+++ b/Organización/Calidad/PTL_Checklist_Calidad_aammdd.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095"/>
+    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="117">
   <si>
     <t>DATOS GENERALES</t>
   </si>
@@ -301,9 +301,6 @@
     <t>¿Los elementos de configuración respetan el nombrado establecido en el documento Plan configuración?</t>
   </si>
   <si>
-    <t>¿Se indicó el cambio dentro de los elementos de configuración afectados por un cambio?</t>
-  </si>
-  <si>
     <t>¿Se actualizarón apropiadamente los elementos de configuración afectados por algún cambio?</t>
   </si>
   <si>
@@ -348,6 +345,30 @@
   <si>
     <t>¿Se identificó el producto a vender dentro de todas las opciones?</t>
   </si>
+  <si>
+    <t>Reporte de Monitoreo</t>
+  </si>
+  <si>
+    <t>¿Se revisó que los hitos se encontraran completos?(Nombre del hito, fecha planeada y fecha real)</t>
+  </si>
+  <si>
+    <t>¿Se revisaron que los costos planeados y reales sean consistentes al proyecto especificado?</t>
+  </si>
+  <si>
+    <t>¿Se reviso que el esfuerzo planeado y real sean consistentes al proyecto?</t>
+  </si>
+  <si>
+    <t>¿Se revisaron los resultados de las auditorias?</t>
+  </si>
+  <si>
+    <t>De acuerdo a dichos resultados, ¿se realizó el análisis de los mismos?</t>
+  </si>
+  <si>
+    <t>¿Se analizaron los riesgos?</t>
+  </si>
+  <si>
+    <t>¿Se agregarón comentarios para el seguimiento de los riesgos ?</t>
+  </si>
 </sst>
 </file>
 
@@ -359,7 +380,7 @@
     <numFmt numFmtId="166" formatCode="[$-80A]0%"/>
     <numFmt numFmtId="167" formatCode="[$$-80A]#,##0.00;[Red]&quot;-&quot;[$$-80A]#,##0.00"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -465,8 +486,14 @@
       <color rgb="FF000000"/>
       <name val="American Typewriter"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -597,6 +624,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor rgb="FFCFE7F5"/>
       </patternFill>
     </fill>
   </fills>
@@ -840,7 +873,7 @@
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="130">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1050,15 +1083,15 @@
     <xf numFmtId="165" fontId="13" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="21" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="22" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="8" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="18" borderId="11" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="21" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="15" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1068,16 +1101,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="8" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1103,6 +1126,16 @@
     <xf numFmtId="165" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1118,8 +1151,11 @@
     <xf numFmtId="165" fontId="9" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="21" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="10" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1151,12 +1187,47 @@
     <xf numFmtId="165" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="21" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="20" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="ConditionalStyle_1" xfId="1"/>
@@ -1474,10 +1545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ35"/>
+  <dimension ref="A1:AMJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1718,90 +1789,104 @@
         <v>81</v>
       </c>
       <c r="C28" s="68">
-        <f>COUNTA(Productos!C36:C38)</f>
+        <f>COUNTA(Productos!C48:C51)</f>
         <v>0</v>
       </c>
       <c r="D28" s="64" t="e">
-        <f>COUNTIF(Productos!C36:C39,"x")/(COUNTIF((Productos!C36:C39),"x")+COUNTIF((Productos!D36:D39),"x"))</f>
+        <f>COUNTIF(Productos!C48:C51,"x")/(COUNTIF((Productos!C48:C51),"x")+COUNTIF((Productos!D48:D51),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="61" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C29" s="68">
-        <f>COUNTA(Productos!C44:C52)</f>
+        <f>COUNTA(Productos!C36:C44)</f>
         <v>0</v>
       </c>
       <c r="D29" s="64" t="e">
-        <f>COUNTIF(Productos!C44:C52,"x")/(COUNTIF((Productos!C44:C52),"x")+COUNTIF((Productos!D44:D52),"x"))</f>
+        <f>COUNTIF(Productos!C36:C44,"x")/(COUNTIF((Productos!C36:C44),"x")+COUNTIF((Productos!D36:D44),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="18">
-      <c r="B31" s="82" t="s">
-        <v>97</v>
-      </c>
-      <c r="C31" s="82"/>
-      <c r="D31" s="82"/>
+    <row r="30" spans="2:4">
+      <c r="B30" s="129" t="str">
+        <f>Productos!A54</f>
+        <v>Reporte de Monitoreo</v>
+      </c>
+      <c r="C30" s="68">
+        <f>COUNTA(Productos!C56:C62)</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="64" t="e">
+        <f>COUNTIF(Productos!C56:C62,"x")/(COUNTIF((Productos!C56:C62),"x")+COUNTIF((Productos!D56:D62),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="32" spans="2:4">
-      <c r="B32" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>8</v>
-      </c>
+    <row r="32" spans="2:4" ht="18">
+      <c r="B32" s="82" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="82"/>
+      <c r="D32" s="82"/>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="79" t="str">
+      <c r="B33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="78" t="str">
         <f>Física!A3</f>
         <v>Elementos de Configuración</v>
       </c>
-      <c r="C33" s="80">
-        <f>COUNTA(Física!C4:C7)</f>
+      <c r="C34" s="79">
+        <f>COUNTA(Física!C4:C6)</f>
         <v>0</v>
       </c>
-      <c r="D33" s="81" t="e">
-        <f>COUNTIF(Física!C4:C7,"x")/(COUNTIF((Física!C4:C7),"x")+COUNTIF((Física!D4:D7),"x"))</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34" s="79" t="str">
-        <f>Física!A8</f>
-        <v>Línea Base</v>
-      </c>
-      <c r="C34" s="80">
-        <f>COUNTA(Física!C9:C12)</f>
-        <v>0</v>
-      </c>
-      <c r="D34" s="81" t="e">
-        <f>COUNTIF(Física!C9:C12,"x")/(COUNTIF((Física!C9:C12),"x")+COUNTIF((Física!D9:D12),"x"))</f>
+      <c r="D34" s="80" t="e">
+        <f>COUNTIF(Física!C4:C6,"x")/(COUNTIF((Física!C4:C6),"x")+COUNTIF((Física!D4:D6),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="35" spans="2:4">
-      <c r="B35" s="79" t="str">
-        <f>Física!A13</f>
+      <c r="B35" s="78" t="str">
+        <f>Física!A7</f>
+        <v>Línea Base</v>
+      </c>
+      <c r="C35" s="79">
+        <f>COUNTA(Física!C8:C11)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="80" t="e">
+        <f>COUNTIF(Física!C8:C11,"x")/(COUNTIF((Física!C8:C11),"x")+COUNTIF((Física!D8:D11),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="78" t="str">
+        <f>Física!A12</f>
         <v>Control de Cambios</v>
       </c>
-      <c r="C35" s="80">
-        <f>COUNTA(Física!C14:C14)</f>
+      <c r="C36" s="79">
+        <f>COUNTA(Física!C13:C13)</f>
         <v>0</v>
       </c>
-      <c r="D35" s="81" t="e">
-        <f>COUNTIF(Física!C14:C14,"x")/(COUNTIF((Física!C14:C14),"x")+COUNTIF((Física!D14:D14),"x"))</f>
+      <c r="D36" s="80" t="e">
+        <f>COUNTIF(Física!C13:C13,"x")/(COUNTIF((Física!C13:C13),"x")+COUNTIF((Física!D13:D13),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B2:F2"/>
@@ -1835,22 +1920,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="90" t="s">
+      <c r="B1" s="91"/>
+      <c r="C1" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="91"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="93" t="s">
+      <c r="D1" s="87"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="89" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="96"/>
-      <c r="B2" s="97"/>
+      <c r="A2" s="92"/>
+      <c r="B2" s="93"/>
       <c r="C2" s="14" t="s">
         <v>14</v>
       </c>
@@ -1860,7 +1945,7 @@
       <c r="E2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="93"/>
+      <c r="F2" s="89"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="37">
@@ -1913,22 +1998,22 @@
     <row r="7" spans="1:6" s="15" customFormat="1"/>
     <row r="8" spans="1:6" s="15" customFormat="1"/>
     <row r="9" spans="1:6" s="15" customFormat="1">
-      <c r="A9" s="87" t="s">
+      <c r="A9" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="87"/>
-      <c r="C9" s="88" t="s">
+      <c r="B9" s="95"/>
+      <c r="C9" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="88"/>
-      <c r="E9" s="89"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="97"/>
       <c r="F9" s="98" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="15" customFormat="1">
-      <c r="A10" s="87"/>
-      <c r="B10" s="87"/>
+      <c r="A10" s="95"/>
+      <c r="B10" s="95"/>
       <c r="C10" s="36" t="s">
         <v>9</v>
       </c>
@@ -2039,22 +2124,22 @@
     <row r="19" spans="1:6" s="15" customFormat="1"/>
     <row r="20" spans="1:6" s="15" customFormat="1"/>
     <row r="21" spans="1:6" s="15" customFormat="1">
-      <c r="A21" s="87" t="s">
+      <c r="A21" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="87"/>
-      <c r="C21" s="88" t="s">
+      <c r="B21" s="95"/>
+      <c r="C21" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="88"/>
-      <c r="E21" s="89"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="97"/>
       <c r="F21" s="98" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="15" customFormat="1">
-      <c r="A22" s="87"/>
-      <c r="B22" s="87"/>
+      <c r="A22" s="95"/>
+      <c r="B22" s="95"/>
       <c r="C22" s="31" t="s">
         <v>9</v>
       </c>
@@ -2129,22 +2214,22 @@
     <row r="28" spans="1:6" s="15" customFormat="1"/>
     <row r="29" spans="1:6" s="15" customFormat="1"/>
     <row r="30" spans="1:6" s="15" customFormat="1">
-      <c r="A30" s="87" t="s">
+      <c r="A30" s="95" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="87"/>
-      <c r="C30" s="88" t="s">
+      <c r="B30" s="95"/>
+      <c r="C30" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="88"/>
-      <c r="E30" s="89"/>
+      <c r="D30" s="96"/>
+      <c r="E30" s="97"/>
       <c r="F30" s="98" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="15" customFormat="1">
-      <c r="A31" s="87"/>
-      <c r="B31" s="87"/>
+      <c r="A31" s="95"/>
+      <c r="B31" s="95"/>
       <c r="C31" s="32" t="s">
         <v>9</v>
       </c>
@@ -2208,22 +2293,22 @@
     <row r="37" spans="1:6" s="15" customFormat="1"/>
     <row r="38" spans="1:6" s="15" customFormat="1"/>
     <row r="39" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A39" s="87" t="s">
+      <c r="A39" s="95" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="87"/>
-      <c r="C39" s="88" t="s">
+      <c r="B39" s="95"/>
+      <c r="C39" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="88"/>
-      <c r="E39" s="89"/>
+      <c r="D39" s="96"/>
+      <c r="E39" s="97"/>
       <c r="F39" s="98" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A40" s="87"/>
-      <c r="B40" s="87"/>
+      <c r="A40" s="95"/>
+      <c r="B40" s="95"/>
       <c r="C40" s="36" t="s">
         <v>9</v>
       </c>
@@ -2285,28 +2370,28 @@
     </row>
     <row r="45" spans="1:6" s="15" customFormat="1"/>
     <row r="46" spans="1:6" s="15" customFormat="1">
-      <c r="B46" s="86"/>
-      <c r="C46" s="86"/>
-      <c r="D46" s="86"/>
-      <c r="E46" s="86"/>
+      <c r="B46" s="94"/>
+      <c r="C46" s="94"/>
+      <c r="D46" s="94"/>
+      <c r="E46" s="94"/>
     </row>
     <row r="47" spans="1:6" s="15" customFormat="1">
-      <c r="A47" s="87" t="s">
+      <c r="A47" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="87"/>
-      <c r="C47" s="88" t="s">
+      <c r="B47" s="95"/>
+      <c r="C47" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="88"/>
-      <c r="E47" s="89"/>
+      <c r="D47" s="96"/>
+      <c r="E47" s="97"/>
       <c r="F47" s="98" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="15" customFormat="1">
-      <c r="A48" s="87"/>
-      <c r="B48" s="87"/>
+      <c r="A48" s="95"/>
+      <c r="B48" s="95"/>
       <c r="C48" s="36" t="s">
         <v>9</v>
       </c>
@@ -2393,10 +2478,10 @@
     <row r="66" spans="2:5" s="15" customFormat="1"/>
     <row r="67" spans="2:5" s="15" customFormat="1"/>
     <row r="68" spans="2:5" s="15" customFormat="1">
-      <c r="B68" s="86"/>
-      <c r="C68" s="86"/>
-      <c r="D68" s="86"/>
-      <c r="E68" s="86"/>
+      <c r="B68" s="94"/>
+      <c r="C68" s="94"/>
+      <c r="D68" s="94"/>
+      <c r="E68" s="94"/>
     </row>
     <row r="69" spans="2:5" s="15" customFormat="1"/>
     <row r="70" spans="2:5" s="15" customFormat="1">
@@ -2414,10 +2499,10 @@
     <row r="78" spans="2:5" s="15" customFormat="1"/>
     <row r="79" spans="2:5" s="15" customFormat="1"/>
     <row r="80" spans="2:5" s="15" customFormat="1">
-      <c r="B80" s="86"/>
-      <c r="C80" s="86"/>
-      <c r="D80" s="86"/>
-      <c r="E80" s="86"/>
+      <c r="B80" s="94"/>
+      <c r="C80" s="94"/>
+      <c r="D80" s="94"/>
+      <c r="E80" s="94"/>
     </row>
     <row r="81" spans="2:5" s="15" customFormat="1"/>
     <row r="82" spans="2:5" s="15" customFormat="1">
@@ -2439,10 +2524,10 @@
     <row r="94" spans="2:5" s="15" customFormat="1"/>
     <row r="95" spans="2:5" s="15" customFormat="1"/>
     <row r="96" spans="2:5" s="15" customFormat="1">
-      <c r="B96" s="86"/>
-      <c r="C96" s="86"/>
-      <c r="D96" s="86"/>
-      <c r="E96" s="86"/>
+      <c r="B96" s="94"/>
+      <c r="C96" s="94"/>
+      <c r="D96" s="94"/>
+      <c r="E96" s="94"/>
     </row>
     <row r="97" spans="3:5" s="15" customFormat="1"/>
     <row r="98" spans="3:5" s="15" customFormat="1">
@@ -2545,6 +2630,12 @@
     <row r="191" s="15" customFormat="1"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B96:E96"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="A9:B10"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="C21:E21"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:B2"/>
@@ -2561,12 +2652,6 @@
     <mergeCell ref="A47:B48"/>
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="F47:F48"/>
-    <mergeCell ref="B96:E96"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="A9:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="C21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2576,10 +2661,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ52"/>
+  <dimension ref="A1:AMJ62"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2589,22 +2674,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="95" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="88" t="s">
+      <c r="B1" s="95"/>
+      <c r="C1" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="88"/>
-      <c r="E1" s="89"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="97"/>
       <c r="F1" s="98" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1024">
-      <c r="A2" s="87"/>
-      <c r="B2" s="87"/>
+      <c r="A2" s="95"/>
+      <c r="B2" s="95"/>
       <c r="C2" s="31" t="s">
         <v>9</v>
       </c>
@@ -2685,22 +2770,22 @@
       <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:1024" ht="15" customHeight="1">
-      <c r="A9" s="87" t="s">
+      <c r="A9" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="87"/>
-      <c r="C9" s="88" t="s">
+      <c r="B9" s="95"/>
+      <c r="C9" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="88"/>
-      <c r="E9" s="89"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="97"/>
       <c r="F9" s="98" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:1024" ht="15" customHeight="1">
-      <c r="A10" s="114"/>
-      <c r="B10" s="114"/>
+      <c r="A10" s="103"/>
+      <c r="B10" s="103"/>
       <c r="C10" s="36" t="s">
         <v>9</v>
       </c>
@@ -2710,7 +2795,7 @@
       <c r="E10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="115"/>
+      <c r="F10" s="104"/>
     </row>
     <row r="11" spans="1:1024" ht="30">
       <c r="A11" s="48">
@@ -2729,7 +2814,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="54" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12" s="55"/>
       <c r="D12" s="55"/>
@@ -2745,15 +2830,15 @@
       <c r="F13" s="34"/>
     </row>
     <row r="14" spans="1:1024" ht="15" customHeight="1">
-      <c r="A14" s="87" t="s">
+      <c r="A14" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="87"/>
-      <c r="C14" s="88" t="s">
+      <c r="B14" s="95"/>
+      <c r="C14" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="88"/>
-      <c r="E14" s="89"/>
+      <c r="D14" s="96"/>
+      <c r="E14" s="97"/>
       <c r="F14" s="98" t="s">
         <v>13</v>
       </c>
@@ -3777,8 +3862,8 @@
       <c r="AMJ14" s="12"/>
     </row>
     <row r="15" spans="1:1024" ht="15" customHeight="1">
-      <c r="A15" s="87"/>
-      <c r="B15" s="87"/>
+      <c r="A15" s="95"/>
+      <c r="B15" s="95"/>
       <c r="C15" s="31" t="s">
         <v>9</v>
       </c>
@@ -21289,16 +21374,16 @@
       <c r="AMJ31" s="12"/>
     </row>
     <row r="32" spans="1:1024">
-      <c r="A32" s="48">
+      <c r="A32" s="118">
         <v>15</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="119" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="45"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
@@ -22318,233 +22403,1374 @@
       <c r="AMI32" s="12"/>
       <c r="AMJ32" s="12"/>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="105" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="105"/>
-      <c r="C34" s="104" t="s">
+    <row r="33" spans="1:1024">
+      <c r="A33" s="123"/>
+      <c r="B33" s="115"/>
+      <c r="C33" s="116"/>
+      <c r="D33" s="116"/>
+      <c r="E33" s="116"/>
+      <c r="F33" s="117"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="12"/>
+      <c r="U33" s="12"/>
+      <c r="V33" s="12"/>
+      <c r="W33" s="12"/>
+      <c r="X33" s="12"/>
+      <c r="Y33" s="12"/>
+      <c r="Z33" s="12"/>
+      <c r="AA33" s="12"/>
+      <c r="AB33" s="12"/>
+      <c r="AC33" s="12"/>
+      <c r="AD33" s="12"/>
+      <c r="AE33" s="12"/>
+      <c r="AF33" s="12"/>
+      <c r="AG33" s="12"/>
+      <c r="AH33" s="12"/>
+      <c r="AI33" s="12"/>
+      <c r="AJ33" s="12"/>
+      <c r="AK33" s="12"/>
+      <c r="AL33" s="12"/>
+      <c r="AM33" s="12"/>
+      <c r="AN33" s="12"/>
+      <c r="AO33" s="12"/>
+      <c r="AP33" s="12"/>
+      <c r="AQ33" s="12"/>
+      <c r="AR33" s="12"/>
+      <c r="AS33" s="12"/>
+      <c r="AT33" s="12"/>
+      <c r="AU33" s="12"/>
+      <c r="AV33" s="12"/>
+      <c r="AW33" s="12"/>
+      <c r="AX33" s="12"/>
+      <c r="AY33" s="12"/>
+      <c r="AZ33" s="12"/>
+      <c r="BA33" s="12"/>
+      <c r="BB33" s="12"/>
+      <c r="BC33" s="12"/>
+      <c r="BD33" s="12"/>
+      <c r="BE33" s="12"/>
+      <c r="BF33" s="12"/>
+      <c r="BG33" s="12"/>
+      <c r="BH33" s="12"/>
+      <c r="BI33" s="12"/>
+      <c r="BJ33" s="12"/>
+      <c r="BK33" s="12"/>
+      <c r="BL33" s="12"/>
+      <c r="BM33" s="12"/>
+      <c r="BN33" s="12"/>
+      <c r="BO33" s="12"/>
+      <c r="BP33" s="12"/>
+      <c r="BQ33" s="12"/>
+      <c r="BR33" s="12"/>
+      <c r="BS33" s="12"/>
+      <c r="BT33" s="12"/>
+      <c r="BU33" s="12"/>
+      <c r="BV33" s="12"/>
+      <c r="BW33" s="12"/>
+      <c r="BX33" s="12"/>
+      <c r="BY33" s="12"/>
+      <c r="BZ33" s="12"/>
+      <c r="CA33" s="12"/>
+      <c r="CB33" s="12"/>
+      <c r="CC33" s="12"/>
+      <c r="CD33" s="12"/>
+      <c r="CE33" s="12"/>
+      <c r="CF33" s="12"/>
+      <c r="CG33" s="12"/>
+      <c r="CH33" s="12"/>
+      <c r="CI33" s="12"/>
+      <c r="CJ33" s="12"/>
+      <c r="CK33" s="12"/>
+      <c r="CL33" s="12"/>
+      <c r="CM33" s="12"/>
+      <c r="CN33" s="12"/>
+      <c r="CO33" s="12"/>
+      <c r="CP33" s="12"/>
+      <c r="CQ33" s="12"/>
+      <c r="CR33" s="12"/>
+      <c r="CS33" s="12"/>
+      <c r="CT33" s="12"/>
+      <c r="CU33" s="12"/>
+      <c r="CV33" s="12"/>
+      <c r="CW33" s="12"/>
+      <c r="CX33" s="12"/>
+      <c r="CY33" s="12"/>
+      <c r="CZ33" s="12"/>
+      <c r="DA33" s="12"/>
+      <c r="DB33" s="12"/>
+      <c r="DC33" s="12"/>
+      <c r="DD33" s="12"/>
+      <c r="DE33" s="12"/>
+      <c r="DF33" s="12"/>
+      <c r="DG33" s="12"/>
+      <c r="DH33" s="12"/>
+      <c r="DI33" s="12"/>
+      <c r="DJ33" s="12"/>
+      <c r="DK33" s="12"/>
+      <c r="DL33" s="12"/>
+      <c r="DM33" s="12"/>
+      <c r="DN33" s="12"/>
+      <c r="DO33" s="12"/>
+      <c r="DP33" s="12"/>
+      <c r="DQ33" s="12"/>
+      <c r="DR33" s="12"/>
+      <c r="DS33" s="12"/>
+      <c r="DT33" s="12"/>
+      <c r="DU33" s="12"/>
+      <c r="DV33" s="12"/>
+      <c r="DW33" s="12"/>
+      <c r="DX33" s="12"/>
+      <c r="DY33" s="12"/>
+      <c r="DZ33" s="12"/>
+      <c r="EA33" s="12"/>
+      <c r="EB33" s="12"/>
+      <c r="EC33" s="12"/>
+      <c r="ED33" s="12"/>
+      <c r="EE33" s="12"/>
+      <c r="EF33" s="12"/>
+      <c r="EG33" s="12"/>
+      <c r="EH33" s="12"/>
+      <c r="EI33" s="12"/>
+      <c r="EJ33" s="12"/>
+      <c r="EK33" s="12"/>
+      <c r="EL33" s="12"/>
+      <c r="EM33" s="12"/>
+      <c r="EN33" s="12"/>
+      <c r="EO33" s="12"/>
+      <c r="EP33" s="12"/>
+      <c r="EQ33" s="12"/>
+      <c r="ER33" s="12"/>
+      <c r="ES33" s="12"/>
+      <c r="ET33" s="12"/>
+      <c r="EU33" s="12"/>
+      <c r="EV33" s="12"/>
+      <c r="EW33" s="12"/>
+      <c r="EX33" s="12"/>
+      <c r="EY33" s="12"/>
+      <c r="EZ33" s="12"/>
+      <c r="FA33" s="12"/>
+      <c r="FB33" s="12"/>
+      <c r="FC33" s="12"/>
+      <c r="FD33" s="12"/>
+      <c r="FE33" s="12"/>
+      <c r="FF33" s="12"/>
+      <c r="FG33" s="12"/>
+      <c r="FH33" s="12"/>
+      <c r="FI33" s="12"/>
+      <c r="FJ33" s="12"/>
+      <c r="FK33" s="12"/>
+      <c r="FL33" s="12"/>
+      <c r="FM33" s="12"/>
+      <c r="FN33" s="12"/>
+      <c r="FO33" s="12"/>
+      <c r="FP33" s="12"/>
+      <c r="FQ33" s="12"/>
+      <c r="FR33" s="12"/>
+      <c r="FS33" s="12"/>
+      <c r="FT33" s="12"/>
+      <c r="FU33" s="12"/>
+      <c r="FV33" s="12"/>
+      <c r="FW33" s="12"/>
+      <c r="FX33" s="12"/>
+      <c r="FY33" s="12"/>
+      <c r="FZ33" s="12"/>
+      <c r="GA33" s="12"/>
+      <c r="GB33" s="12"/>
+      <c r="GC33" s="12"/>
+      <c r="GD33" s="12"/>
+      <c r="GE33" s="12"/>
+      <c r="GF33" s="12"/>
+      <c r="GG33" s="12"/>
+      <c r="GH33" s="12"/>
+      <c r="GI33" s="12"/>
+      <c r="GJ33" s="12"/>
+      <c r="GK33" s="12"/>
+      <c r="GL33" s="12"/>
+      <c r="GM33" s="12"/>
+      <c r="GN33" s="12"/>
+      <c r="GO33" s="12"/>
+      <c r="GP33" s="12"/>
+      <c r="GQ33" s="12"/>
+      <c r="GR33" s="12"/>
+      <c r="GS33" s="12"/>
+      <c r="GT33" s="12"/>
+      <c r="GU33" s="12"/>
+      <c r="GV33" s="12"/>
+      <c r="GW33" s="12"/>
+      <c r="GX33" s="12"/>
+      <c r="GY33" s="12"/>
+      <c r="GZ33" s="12"/>
+      <c r="HA33" s="12"/>
+      <c r="HB33" s="12"/>
+      <c r="HC33" s="12"/>
+      <c r="HD33" s="12"/>
+      <c r="HE33" s="12"/>
+      <c r="HF33" s="12"/>
+      <c r="HG33" s="12"/>
+      <c r="HH33" s="12"/>
+      <c r="HI33" s="12"/>
+      <c r="HJ33" s="12"/>
+      <c r="HK33" s="12"/>
+      <c r="HL33" s="12"/>
+      <c r="HM33" s="12"/>
+      <c r="HN33" s="12"/>
+      <c r="HO33" s="12"/>
+      <c r="HP33" s="12"/>
+      <c r="HQ33" s="12"/>
+      <c r="HR33" s="12"/>
+      <c r="HS33" s="12"/>
+      <c r="HT33" s="12"/>
+      <c r="HU33" s="12"/>
+      <c r="HV33" s="12"/>
+      <c r="HW33" s="12"/>
+      <c r="HX33" s="12"/>
+      <c r="HY33" s="12"/>
+      <c r="HZ33" s="12"/>
+      <c r="IA33" s="12"/>
+      <c r="IB33" s="12"/>
+      <c r="IC33" s="12"/>
+      <c r="ID33" s="12"/>
+      <c r="IE33" s="12"/>
+      <c r="IF33" s="12"/>
+      <c r="IG33" s="12"/>
+      <c r="IH33" s="12"/>
+      <c r="II33" s="12"/>
+      <c r="IJ33" s="12"/>
+      <c r="IK33" s="12"/>
+      <c r="IL33" s="12"/>
+      <c r="IM33" s="12"/>
+      <c r="IN33" s="12"/>
+      <c r="IO33" s="12"/>
+      <c r="IP33" s="12"/>
+      <c r="IQ33" s="12"/>
+      <c r="IR33" s="12"/>
+      <c r="IS33" s="12"/>
+      <c r="IT33" s="12"/>
+      <c r="IU33" s="12"/>
+      <c r="IV33" s="12"/>
+      <c r="IW33" s="12"/>
+      <c r="IX33" s="12"/>
+      <c r="IY33" s="12"/>
+      <c r="IZ33" s="12"/>
+      <c r="JA33" s="12"/>
+      <c r="JB33" s="12"/>
+      <c r="JC33" s="12"/>
+      <c r="JD33" s="12"/>
+      <c r="JE33" s="12"/>
+      <c r="JF33" s="12"/>
+      <c r="JG33" s="12"/>
+      <c r="JH33" s="12"/>
+      <c r="JI33" s="12"/>
+      <c r="JJ33" s="12"/>
+      <c r="JK33" s="12"/>
+      <c r="JL33" s="12"/>
+      <c r="JM33" s="12"/>
+      <c r="JN33" s="12"/>
+      <c r="JO33" s="12"/>
+      <c r="JP33" s="12"/>
+      <c r="JQ33" s="12"/>
+      <c r="JR33" s="12"/>
+      <c r="JS33" s="12"/>
+      <c r="JT33" s="12"/>
+      <c r="JU33" s="12"/>
+      <c r="JV33" s="12"/>
+      <c r="JW33" s="12"/>
+      <c r="JX33" s="12"/>
+      <c r="JY33" s="12"/>
+      <c r="JZ33" s="12"/>
+      <c r="KA33" s="12"/>
+      <c r="KB33" s="12"/>
+      <c r="KC33" s="12"/>
+      <c r="KD33" s="12"/>
+      <c r="KE33" s="12"/>
+      <c r="KF33" s="12"/>
+      <c r="KG33" s="12"/>
+      <c r="KH33" s="12"/>
+      <c r="KI33" s="12"/>
+      <c r="KJ33" s="12"/>
+      <c r="KK33" s="12"/>
+      <c r="KL33" s="12"/>
+      <c r="KM33" s="12"/>
+      <c r="KN33" s="12"/>
+      <c r="KO33" s="12"/>
+      <c r="KP33" s="12"/>
+      <c r="KQ33" s="12"/>
+      <c r="KR33" s="12"/>
+      <c r="KS33" s="12"/>
+      <c r="KT33" s="12"/>
+      <c r="KU33" s="12"/>
+      <c r="KV33" s="12"/>
+      <c r="KW33" s="12"/>
+      <c r="KX33" s="12"/>
+      <c r="KY33" s="12"/>
+      <c r="KZ33" s="12"/>
+      <c r="LA33" s="12"/>
+      <c r="LB33" s="12"/>
+      <c r="LC33" s="12"/>
+      <c r="LD33" s="12"/>
+      <c r="LE33" s="12"/>
+      <c r="LF33" s="12"/>
+      <c r="LG33" s="12"/>
+      <c r="LH33" s="12"/>
+      <c r="LI33" s="12"/>
+      <c r="LJ33" s="12"/>
+      <c r="LK33" s="12"/>
+      <c r="LL33" s="12"/>
+      <c r="LM33" s="12"/>
+      <c r="LN33" s="12"/>
+      <c r="LO33" s="12"/>
+      <c r="LP33" s="12"/>
+      <c r="LQ33" s="12"/>
+      <c r="LR33" s="12"/>
+      <c r="LS33" s="12"/>
+      <c r="LT33" s="12"/>
+      <c r="LU33" s="12"/>
+      <c r="LV33" s="12"/>
+      <c r="LW33" s="12"/>
+      <c r="LX33" s="12"/>
+      <c r="LY33" s="12"/>
+      <c r="LZ33" s="12"/>
+      <c r="MA33" s="12"/>
+      <c r="MB33" s="12"/>
+      <c r="MC33" s="12"/>
+      <c r="MD33" s="12"/>
+      <c r="ME33" s="12"/>
+      <c r="MF33" s="12"/>
+      <c r="MG33" s="12"/>
+      <c r="MH33" s="12"/>
+      <c r="MI33" s="12"/>
+      <c r="MJ33" s="12"/>
+      <c r="MK33" s="12"/>
+      <c r="ML33" s="12"/>
+      <c r="MM33" s="12"/>
+      <c r="MN33" s="12"/>
+      <c r="MO33" s="12"/>
+      <c r="MP33" s="12"/>
+      <c r="MQ33" s="12"/>
+      <c r="MR33" s="12"/>
+      <c r="MS33" s="12"/>
+      <c r="MT33" s="12"/>
+      <c r="MU33" s="12"/>
+      <c r="MV33" s="12"/>
+      <c r="MW33" s="12"/>
+      <c r="MX33" s="12"/>
+      <c r="MY33" s="12"/>
+      <c r="MZ33" s="12"/>
+      <c r="NA33" s="12"/>
+      <c r="NB33" s="12"/>
+      <c r="NC33" s="12"/>
+      <c r="ND33" s="12"/>
+      <c r="NE33" s="12"/>
+      <c r="NF33" s="12"/>
+      <c r="NG33" s="12"/>
+      <c r="NH33" s="12"/>
+      <c r="NI33" s="12"/>
+      <c r="NJ33" s="12"/>
+      <c r="NK33" s="12"/>
+      <c r="NL33" s="12"/>
+      <c r="NM33" s="12"/>
+      <c r="NN33" s="12"/>
+      <c r="NO33" s="12"/>
+      <c r="NP33" s="12"/>
+      <c r="NQ33" s="12"/>
+      <c r="NR33" s="12"/>
+      <c r="NS33" s="12"/>
+      <c r="NT33" s="12"/>
+      <c r="NU33" s="12"/>
+      <c r="NV33" s="12"/>
+      <c r="NW33" s="12"/>
+      <c r="NX33" s="12"/>
+      <c r="NY33" s="12"/>
+      <c r="NZ33" s="12"/>
+      <c r="OA33" s="12"/>
+      <c r="OB33" s="12"/>
+      <c r="OC33" s="12"/>
+      <c r="OD33" s="12"/>
+      <c r="OE33" s="12"/>
+      <c r="OF33" s="12"/>
+      <c r="OG33" s="12"/>
+      <c r="OH33" s="12"/>
+      <c r="OI33" s="12"/>
+      <c r="OJ33" s="12"/>
+      <c r="OK33" s="12"/>
+      <c r="OL33" s="12"/>
+      <c r="OM33" s="12"/>
+      <c r="ON33" s="12"/>
+      <c r="OO33" s="12"/>
+      <c r="OP33" s="12"/>
+      <c r="OQ33" s="12"/>
+      <c r="OR33" s="12"/>
+      <c r="OS33" s="12"/>
+      <c r="OT33" s="12"/>
+      <c r="OU33" s="12"/>
+      <c r="OV33" s="12"/>
+      <c r="OW33" s="12"/>
+      <c r="OX33" s="12"/>
+      <c r="OY33" s="12"/>
+      <c r="OZ33" s="12"/>
+      <c r="PA33" s="12"/>
+      <c r="PB33" s="12"/>
+      <c r="PC33" s="12"/>
+      <c r="PD33" s="12"/>
+      <c r="PE33" s="12"/>
+      <c r="PF33" s="12"/>
+      <c r="PG33" s="12"/>
+      <c r="PH33" s="12"/>
+      <c r="PI33" s="12"/>
+      <c r="PJ33" s="12"/>
+      <c r="PK33" s="12"/>
+      <c r="PL33" s="12"/>
+      <c r="PM33" s="12"/>
+      <c r="PN33" s="12"/>
+      <c r="PO33" s="12"/>
+      <c r="PP33" s="12"/>
+      <c r="PQ33" s="12"/>
+      <c r="PR33" s="12"/>
+      <c r="PS33" s="12"/>
+      <c r="PT33" s="12"/>
+      <c r="PU33" s="12"/>
+      <c r="PV33" s="12"/>
+      <c r="PW33" s="12"/>
+      <c r="PX33" s="12"/>
+      <c r="PY33" s="12"/>
+      <c r="PZ33" s="12"/>
+      <c r="QA33" s="12"/>
+      <c r="QB33" s="12"/>
+      <c r="QC33" s="12"/>
+      <c r="QD33" s="12"/>
+      <c r="QE33" s="12"/>
+      <c r="QF33" s="12"/>
+      <c r="QG33" s="12"/>
+      <c r="QH33" s="12"/>
+      <c r="QI33" s="12"/>
+      <c r="QJ33" s="12"/>
+      <c r="QK33" s="12"/>
+      <c r="QL33" s="12"/>
+      <c r="QM33" s="12"/>
+      <c r="QN33" s="12"/>
+      <c r="QO33" s="12"/>
+      <c r="QP33" s="12"/>
+      <c r="QQ33" s="12"/>
+      <c r="QR33" s="12"/>
+      <c r="QS33" s="12"/>
+      <c r="QT33" s="12"/>
+      <c r="QU33" s="12"/>
+      <c r="QV33" s="12"/>
+      <c r="QW33" s="12"/>
+      <c r="QX33" s="12"/>
+      <c r="QY33" s="12"/>
+      <c r="QZ33" s="12"/>
+      <c r="RA33" s="12"/>
+      <c r="RB33" s="12"/>
+      <c r="RC33" s="12"/>
+      <c r="RD33" s="12"/>
+      <c r="RE33" s="12"/>
+      <c r="RF33" s="12"/>
+      <c r="RG33" s="12"/>
+      <c r="RH33" s="12"/>
+      <c r="RI33" s="12"/>
+      <c r="RJ33" s="12"/>
+      <c r="RK33" s="12"/>
+      <c r="RL33" s="12"/>
+      <c r="RM33" s="12"/>
+      <c r="RN33" s="12"/>
+      <c r="RO33" s="12"/>
+      <c r="RP33" s="12"/>
+      <c r="RQ33" s="12"/>
+      <c r="RR33" s="12"/>
+      <c r="RS33" s="12"/>
+      <c r="RT33" s="12"/>
+      <c r="RU33" s="12"/>
+      <c r="RV33" s="12"/>
+      <c r="RW33" s="12"/>
+      <c r="RX33" s="12"/>
+      <c r="RY33" s="12"/>
+      <c r="RZ33" s="12"/>
+      <c r="SA33" s="12"/>
+      <c r="SB33" s="12"/>
+      <c r="SC33" s="12"/>
+      <c r="SD33" s="12"/>
+      <c r="SE33" s="12"/>
+      <c r="SF33" s="12"/>
+      <c r="SG33" s="12"/>
+      <c r="SH33" s="12"/>
+      <c r="SI33" s="12"/>
+      <c r="SJ33" s="12"/>
+      <c r="SK33" s="12"/>
+      <c r="SL33" s="12"/>
+      <c r="SM33" s="12"/>
+      <c r="SN33" s="12"/>
+      <c r="SO33" s="12"/>
+      <c r="SP33" s="12"/>
+      <c r="SQ33" s="12"/>
+      <c r="SR33" s="12"/>
+      <c r="SS33" s="12"/>
+      <c r="ST33" s="12"/>
+      <c r="SU33" s="12"/>
+      <c r="SV33" s="12"/>
+      <c r="SW33" s="12"/>
+      <c r="SX33" s="12"/>
+      <c r="SY33" s="12"/>
+      <c r="SZ33" s="12"/>
+      <c r="TA33" s="12"/>
+      <c r="TB33" s="12"/>
+      <c r="TC33" s="12"/>
+      <c r="TD33" s="12"/>
+      <c r="TE33" s="12"/>
+      <c r="TF33" s="12"/>
+      <c r="TG33" s="12"/>
+      <c r="TH33" s="12"/>
+      <c r="TI33" s="12"/>
+      <c r="TJ33" s="12"/>
+      <c r="TK33" s="12"/>
+      <c r="TL33" s="12"/>
+      <c r="TM33" s="12"/>
+      <c r="TN33" s="12"/>
+      <c r="TO33" s="12"/>
+      <c r="TP33" s="12"/>
+      <c r="TQ33" s="12"/>
+      <c r="TR33" s="12"/>
+      <c r="TS33" s="12"/>
+      <c r="TT33" s="12"/>
+      <c r="TU33" s="12"/>
+      <c r="TV33" s="12"/>
+      <c r="TW33" s="12"/>
+      <c r="TX33" s="12"/>
+      <c r="TY33" s="12"/>
+      <c r="TZ33" s="12"/>
+      <c r="UA33" s="12"/>
+      <c r="UB33" s="12"/>
+      <c r="UC33" s="12"/>
+      <c r="UD33" s="12"/>
+      <c r="UE33" s="12"/>
+      <c r="UF33" s="12"/>
+      <c r="UG33" s="12"/>
+      <c r="UH33" s="12"/>
+      <c r="UI33" s="12"/>
+      <c r="UJ33" s="12"/>
+      <c r="UK33" s="12"/>
+      <c r="UL33" s="12"/>
+      <c r="UM33" s="12"/>
+      <c r="UN33" s="12"/>
+      <c r="UO33" s="12"/>
+      <c r="UP33" s="12"/>
+      <c r="UQ33" s="12"/>
+      <c r="UR33" s="12"/>
+      <c r="US33" s="12"/>
+      <c r="UT33" s="12"/>
+      <c r="UU33" s="12"/>
+      <c r="UV33" s="12"/>
+      <c r="UW33" s="12"/>
+      <c r="UX33" s="12"/>
+      <c r="UY33" s="12"/>
+      <c r="UZ33" s="12"/>
+      <c r="VA33" s="12"/>
+      <c r="VB33" s="12"/>
+      <c r="VC33" s="12"/>
+      <c r="VD33" s="12"/>
+      <c r="VE33" s="12"/>
+      <c r="VF33" s="12"/>
+      <c r="VG33" s="12"/>
+      <c r="VH33" s="12"/>
+      <c r="VI33" s="12"/>
+      <c r="VJ33" s="12"/>
+      <c r="VK33" s="12"/>
+      <c r="VL33" s="12"/>
+      <c r="VM33" s="12"/>
+      <c r="VN33" s="12"/>
+      <c r="VO33" s="12"/>
+      <c r="VP33" s="12"/>
+      <c r="VQ33" s="12"/>
+      <c r="VR33" s="12"/>
+      <c r="VS33" s="12"/>
+      <c r="VT33" s="12"/>
+      <c r="VU33" s="12"/>
+      <c r="VV33" s="12"/>
+      <c r="VW33" s="12"/>
+      <c r="VX33" s="12"/>
+      <c r="VY33" s="12"/>
+      <c r="VZ33" s="12"/>
+      <c r="WA33" s="12"/>
+      <c r="WB33" s="12"/>
+      <c r="WC33" s="12"/>
+      <c r="WD33" s="12"/>
+      <c r="WE33" s="12"/>
+      <c r="WF33" s="12"/>
+      <c r="WG33" s="12"/>
+      <c r="WH33" s="12"/>
+      <c r="WI33" s="12"/>
+      <c r="WJ33" s="12"/>
+      <c r="WK33" s="12"/>
+      <c r="WL33" s="12"/>
+      <c r="WM33" s="12"/>
+      <c r="WN33" s="12"/>
+      <c r="WO33" s="12"/>
+      <c r="WP33" s="12"/>
+      <c r="WQ33" s="12"/>
+      <c r="WR33" s="12"/>
+      <c r="WS33" s="12"/>
+      <c r="WT33" s="12"/>
+      <c r="WU33" s="12"/>
+      <c r="WV33" s="12"/>
+      <c r="WW33" s="12"/>
+      <c r="WX33" s="12"/>
+      <c r="WY33" s="12"/>
+      <c r="WZ33" s="12"/>
+      <c r="XA33" s="12"/>
+      <c r="XB33" s="12"/>
+      <c r="XC33" s="12"/>
+      <c r="XD33" s="12"/>
+      <c r="XE33" s="12"/>
+      <c r="XF33" s="12"/>
+      <c r="XG33" s="12"/>
+      <c r="XH33" s="12"/>
+      <c r="XI33" s="12"/>
+      <c r="XJ33" s="12"/>
+      <c r="XK33" s="12"/>
+      <c r="XL33" s="12"/>
+      <c r="XM33" s="12"/>
+      <c r="XN33" s="12"/>
+      <c r="XO33" s="12"/>
+      <c r="XP33" s="12"/>
+      <c r="XQ33" s="12"/>
+      <c r="XR33" s="12"/>
+      <c r="XS33" s="12"/>
+      <c r="XT33" s="12"/>
+      <c r="XU33" s="12"/>
+      <c r="XV33" s="12"/>
+      <c r="XW33" s="12"/>
+      <c r="XX33" s="12"/>
+      <c r="XY33" s="12"/>
+      <c r="XZ33" s="12"/>
+      <c r="YA33" s="12"/>
+      <c r="YB33" s="12"/>
+      <c r="YC33" s="12"/>
+      <c r="YD33" s="12"/>
+      <c r="YE33" s="12"/>
+      <c r="YF33" s="12"/>
+      <c r="YG33" s="12"/>
+      <c r="YH33" s="12"/>
+      <c r="YI33" s="12"/>
+      <c r="YJ33" s="12"/>
+      <c r="YK33" s="12"/>
+      <c r="YL33" s="12"/>
+      <c r="YM33" s="12"/>
+      <c r="YN33" s="12"/>
+      <c r="YO33" s="12"/>
+      <c r="YP33" s="12"/>
+      <c r="YQ33" s="12"/>
+      <c r="YR33" s="12"/>
+      <c r="YS33" s="12"/>
+      <c r="YT33" s="12"/>
+      <c r="YU33" s="12"/>
+      <c r="YV33" s="12"/>
+      <c r="YW33" s="12"/>
+      <c r="YX33" s="12"/>
+      <c r="YY33" s="12"/>
+      <c r="YZ33" s="12"/>
+      <c r="ZA33" s="12"/>
+      <c r="ZB33" s="12"/>
+      <c r="ZC33" s="12"/>
+      <c r="ZD33" s="12"/>
+      <c r="ZE33" s="12"/>
+      <c r="ZF33" s="12"/>
+      <c r="ZG33" s="12"/>
+      <c r="ZH33" s="12"/>
+      <c r="ZI33" s="12"/>
+      <c r="ZJ33" s="12"/>
+      <c r="ZK33" s="12"/>
+      <c r="ZL33" s="12"/>
+      <c r="ZM33" s="12"/>
+      <c r="ZN33" s="12"/>
+      <c r="ZO33" s="12"/>
+      <c r="ZP33" s="12"/>
+      <c r="ZQ33" s="12"/>
+      <c r="ZR33" s="12"/>
+      <c r="ZS33" s="12"/>
+      <c r="ZT33" s="12"/>
+      <c r="ZU33" s="12"/>
+      <c r="ZV33" s="12"/>
+      <c r="ZW33" s="12"/>
+      <c r="ZX33" s="12"/>
+      <c r="ZY33" s="12"/>
+      <c r="ZZ33" s="12"/>
+      <c r="AAA33" s="12"/>
+      <c r="AAB33" s="12"/>
+      <c r="AAC33" s="12"/>
+      <c r="AAD33" s="12"/>
+      <c r="AAE33" s="12"/>
+      <c r="AAF33" s="12"/>
+      <c r="AAG33" s="12"/>
+      <c r="AAH33" s="12"/>
+      <c r="AAI33" s="12"/>
+      <c r="AAJ33" s="12"/>
+      <c r="AAK33" s="12"/>
+      <c r="AAL33" s="12"/>
+      <c r="AAM33" s="12"/>
+      <c r="AAN33" s="12"/>
+      <c r="AAO33" s="12"/>
+      <c r="AAP33" s="12"/>
+      <c r="AAQ33" s="12"/>
+      <c r="AAR33" s="12"/>
+      <c r="AAS33" s="12"/>
+      <c r="AAT33" s="12"/>
+      <c r="AAU33" s="12"/>
+      <c r="AAV33" s="12"/>
+      <c r="AAW33" s="12"/>
+      <c r="AAX33" s="12"/>
+      <c r="AAY33" s="12"/>
+      <c r="AAZ33" s="12"/>
+      <c r="ABA33" s="12"/>
+      <c r="ABB33" s="12"/>
+      <c r="ABC33" s="12"/>
+      <c r="ABD33" s="12"/>
+      <c r="ABE33" s="12"/>
+      <c r="ABF33" s="12"/>
+      <c r="ABG33" s="12"/>
+      <c r="ABH33" s="12"/>
+      <c r="ABI33" s="12"/>
+      <c r="ABJ33" s="12"/>
+      <c r="ABK33" s="12"/>
+      <c r="ABL33" s="12"/>
+      <c r="ABM33" s="12"/>
+      <c r="ABN33" s="12"/>
+      <c r="ABO33" s="12"/>
+      <c r="ABP33" s="12"/>
+      <c r="ABQ33" s="12"/>
+      <c r="ABR33" s="12"/>
+      <c r="ABS33" s="12"/>
+      <c r="ABT33" s="12"/>
+      <c r="ABU33" s="12"/>
+      <c r="ABV33" s="12"/>
+      <c r="ABW33" s="12"/>
+      <c r="ABX33" s="12"/>
+      <c r="ABY33" s="12"/>
+      <c r="ABZ33" s="12"/>
+      <c r="ACA33" s="12"/>
+      <c r="ACB33" s="12"/>
+      <c r="ACC33" s="12"/>
+      <c r="ACD33" s="12"/>
+      <c r="ACE33" s="12"/>
+      <c r="ACF33" s="12"/>
+      <c r="ACG33" s="12"/>
+      <c r="ACH33" s="12"/>
+      <c r="ACI33" s="12"/>
+      <c r="ACJ33" s="12"/>
+      <c r="ACK33" s="12"/>
+      <c r="ACL33" s="12"/>
+      <c r="ACM33" s="12"/>
+      <c r="ACN33" s="12"/>
+      <c r="ACO33" s="12"/>
+      <c r="ACP33" s="12"/>
+      <c r="ACQ33" s="12"/>
+      <c r="ACR33" s="12"/>
+      <c r="ACS33" s="12"/>
+      <c r="ACT33" s="12"/>
+      <c r="ACU33" s="12"/>
+      <c r="ACV33" s="12"/>
+      <c r="ACW33" s="12"/>
+      <c r="ACX33" s="12"/>
+      <c r="ACY33" s="12"/>
+      <c r="ACZ33" s="12"/>
+      <c r="ADA33" s="12"/>
+      <c r="ADB33" s="12"/>
+      <c r="ADC33" s="12"/>
+      <c r="ADD33" s="12"/>
+      <c r="ADE33" s="12"/>
+      <c r="ADF33" s="12"/>
+      <c r="ADG33" s="12"/>
+      <c r="ADH33" s="12"/>
+      <c r="ADI33" s="12"/>
+      <c r="ADJ33" s="12"/>
+      <c r="ADK33" s="12"/>
+      <c r="ADL33" s="12"/>
+      <c r="ADM33" s="12"/>
+      <c r="ADN33" s="12"/>
+      <c r="ADO33" s="12"/>
+      <c r="ADP33" s="12"/>
+      <c r="ADQ33" s="12"/>
+      <c r="ADR33" s="12"/>
+      <c r="ADS33" s="12"/>
+      <c r="ADT33" s="12"/>
+      <c r="ADU33" s="12"/>
+      <c r="ADV33" s="12"/>
+      <c r="ADW33" s="12"/>
+      <c r="ADX33" s="12"/>
+      <c r="ADY33" s="12"/>
+      <c r="ADZ33" s="12"/>
+      <c r="AEA33" s="12"/>
+      <c r="AEB33" s="12"/>
+      <c r="AEC33" s="12"/>
+      <c r="AED33" s="12"/>
+      <c r="AEE33" s="12"/>
+      <c r="AEF33" s="12"/>
+      <c r="AEG33" s="12"/>
+      <c r="AEH33" s="12"/>
+      <c r="AEI33" s="12"/>
+      <c r="AEJ33" s="12"/>
+      <c r="AEK33" s="12"/>
+      <c r="AEL33" s="12"/>
+      <c r="AEM33" s="12"/>
+      <c r="AEN33" s="12"/>
+      <c r="AEO33" s="12"/>
+      <c r="AEP33" s="12"/>
+      <c r="AEQ33" s="12"/>
+      <c r="AER33" s="12"/>
+      <c r="AES33" s="12"/>
+      <c r="AET33" s="12"/>
+      <c r="AEU33" s="12"/>
+      <c r="AEV33" s="12"/>
+      <c r="AEW33" s="12"/>
+      <c r="AEX33" s="12"/>
+      <c r="AEY33" s="12"/>
+      <c r="AEZ33" s="12"/>
+      <c r="AFA33" s="12"/>
+      <c r="AFB33" s="12"/>
+      <c r="AFC33" s="12"/>
+      <c r="AFD33" s="12"/>
+      <c r="AFE33" s="12"/>
+      <c r="AFF33" s="12"/>
+      <c r="AFG33" s="12"/>
+      <c r="AFH33" s="12"/>
+      <c r="AFI33" s="12"/>
+      <c r="AFJ33" s="12"/>
+      <c r="AFK33" s="12"/>
+      <c r="AFL33" s="12"/>
+      <c r="AFM33" s="12"/>
+      <c r="AFN33" s="12"/>
+      <c r="AFO33" s="12"/>
+      <c r="AFP33" s="12"/>
+      <c r="AFQ33" s="12"/>
+      <c r="AFR33" s="12"/>
+      <c r="AFS33" s="12"/>
+      <c r="AFT33" s="12"/>
+      <c r="AFU33" s="12"/>
+      <c r="AFV33" s="12"/>
+      <c r="AFW33" s="12"/>
+      <c r="AFX33" s="12"/>
+      <c r="AFY33" s="12"/>
+      <c r="AFZ33" s="12"/>
+      <c r="AGA33" s="12"/>
+      <c r="AGB33" s="12"/>
+      <c r="AGC33" s="12"/>
+      <c r="AGD33" s="12"/>
+      <c r="AGE33" s="12"/>
+      <c r="AGF33" s="12"/>
+      <c r="AGG33" s="12"/>
+      <c r="AGH33" s="12"/>
+      <c r="AGI33" s="12"/>
+      <c r="AGJ33" s="12"/>
+      <c r="AGK33" s="12"/>
+      <c r="AGL33" s="12"/>
+      <c r="AGM33" s="12"/>
+      <c r="AGN33" s="12"/>
+      <c r="AGO33" s="12"/>
+      <c r="AGP33" s="12"/>
+      <c r="AGQ33" s="12"/>
+      <c r="AGR33" s="12"/>
+      <c r="AGS33" s="12"/>
+      <c r="AGT33" s="12"/>
+      <c r="AGU33" s="12"/>
+      <c r="AGV33" s="12"/>
+      <c r="AGW33" s="12"/>
+      <c r="AGX33" s="12"/>
+      <c r="AGY33" s="12"/>
+      <c r="AGZ33" s="12"/>
+      <c r="AHA33" s="12"/>
+      <c r="AHB33" s="12"/>
+      <c r="AHC33" s="12"/>
+      <c r="AHD33" s="12"/>
+      <c r="AHE33" s="12"/>
+      <c r="AHF33" s="12"/>
+      <c r="AHG33" s="12"/>
+      <c r="AHH33" s="12"/>
+      <c r="AHI33" s="12"/>
+      <c r="AHJ33" s="12"/>
+      <c r="AHK33" s="12"/>
+      <c r="AHL33" s="12"/>
+      <c r="AHM33" s="12"/>
+      <c r="AHN33" s="12"/>
+      <c r="AHO33" s="12"/>
+      <c r="AHP33" s="12"/>
+      <c r="AHQ33" s="12"/>
+      <c r="AHR33" s="12"/>
+      <c r="AHS33" s="12"/>
+      <c r="AHT33" s="12"/>
+      <c r="AHU33" s="12"/>
+      <c r="AHV33" s="12"/>
+      <c r="AHW33" s="12"/>
+      <c r="AHX33" s="12"/>
+      <c r="AHY33" s="12"/>
+      <c r="AHZ33" s="12"/>
+      <c r="AIA33" s="12"/>
+      <c r="AIB33" s="12"/>
+      <c r="AIC33" s="12"/>
+      <c r="AID33" s="12"/>
+      <c r="AIE33" s="12"/>
+      <c r="AIF33" s="12"/>
+      <c r="AIG33" s="12"/>
+      <c r="AIH33" s="12"/>
+      <c r="AII33" s="12"/>
+      <c r="AIJ33" s="12"/>
+      <c r="AIK33" s="12"/>
+      <c r="AIL33" s="12"/>
+      <c r="AIM33" s="12"/>
+      <c r="AIN33" s="12"/>
+      <c r="AIO33" s="12"/>
+      <c r="AIP33" s="12"/>
+      <c r="AIQ33" s="12"/>
+      <c r="AIR33" s="12"/>
+      <c r="AIS33" s="12"/>
+      <c r="AIT33" s="12"/>
+      <c r="AIU33" s="12"/>
+      <c r="AIV33" s="12"/>
+      <c r="AIW33" s="12"/>
+      <c r="AIX33" s="12"/>
+      <c r="AIY33" s="12"/>
+      <c r="AIZ33" s="12"/>
+      <c r="AJA33" s="12"/>
+      <c r="AJB33" s="12"/>
+      <c r="AJC33" s="12"/>
+      <c r="AJD33" s="12"/>
+      <c r="AJE33" s="12"/>
+      <c r="AJF33" s="12"/>
+      <c r="AJG33" s="12"/>
+      <c r="AJH33" s="12"/>
+      <c r="AJI33" s="12"/>
+      <c r="AJJ33" s="12"/>
+      <c r="AJK33" s="12"/>
+      <c r="AJL33" s="12"/>
+      <c r="AJM33" s="12"/>
+      <c r="AJN33" s="12"/>
+      <c r="AJO33" s="12"/>
+      <c r="AJP33" s="12"/>
+      <c r="AJQ33" s="12"/>
+      <c r="AJR33" s="12"/>
+      <c r="AJS33" s="12"/>
+      <c r="AJT33" s="12"/>
+      <c r="AJU33" s="12"/>
+      <c r="AJV33" s="12"/>
+      <c r="AJW33" s="12"/>
+      <c r="AJX33" s="12"/>
+      <c r="AJY33" s="12"/>
+      <c r="AJZ33" s="12"/>
+      <c r="AKA33" s="12"/>
+      <c r="AKB33" s="12"/>
+      <c r="AKC33" s="12"/>
+      <c r="AKD33" s="12"/>
+      <c r="AKE33" s="12"/>
+      <c r="AKF33" s="12"/>
+      <c r="AKG33" s="12"/>
+      <c r="AKH33" s="12"/>
+      <c r="AKI33" s="12"/>
+      <c r="AKJ33" s="12"/>
+      <c r="AKK33" s="12"/>
+      <c r="AKL33" s="12"/>
+      <c r="AKM33" s="12"/>
+      <c r="AKN33" s="12"/>
+      <c r="AKO33" s="12"/>
+      <c r="AKP33" s="12"/>
+      <c r="AKQ33" s="12"/>
+      <c r="AKR33" s="12"/>
+      <c r="AKS33" s="12"/>
+      <c r="AKT33" s="12"/>
+      <c r="AKU33" s="12"/>
+      <c r="AKV33" s="12"/>
+      <c r="AKW33" s="12"/>
+      <c r="AKX33" s="12"/>
+      <c r="AKY33" s="12"/>
+      <c r="AKZ33" s="12"/>
+      <c r="ALA33" s="12"/>
+      <c r="ALB33" s="12"/>
+      <c r="ALC33" s="12"/>
+      <c r="ALD33" s="12"/>
+      <c r="ALE33" s="12"/>
+      <c r="ALF33" s="12"/>
+      <c r="ALG33" s="12"/>
+      <c r="ALH33" s="12"/>
+      <c r="ALI33" s="12"/>
+      <c r="ALJ33" s="12"/>
+      <c r="ALK33" s="12"/>
+      <c r="ALL33" s="12"/>
+      <c r="ALM33" s="12"/>
+      <c r="ALN33" s="12"/>
+      <c r="ALO33" s="12"/>
+      <c r="ALP33" s="12"/>
+      <c r="ALQ33" s="12"/>
+      <c r="ALR33" s="12"/>
+      <c r="ALS33" s="12"/>
+      <c r="ALT33" s="12"/>
+      <c r="ALU33" s="12"/>
+      <c r="ALV33" s="12"/>
+      <c r="ALW33" s="12"/>
+      <c r="ALX33" s="12"/>
+      <c r="ALY33" s="12"/>
+      <c r="ALZ33" s="12"/>
+      <c r="AMA33" s="12"/>
+      <c r="AMB33" s="12"/>
+      <c r="AMC33" s="12"/>
+      <c r="AMD33" s="12"/>
+      <c r="AME33" s="12"/>
+      <c r="AMF33" s="12"/>
+      <c r="AMG33" s="12"/>
+      <c r="AMH33" s="12"/>
+      <c r="AMI33" s="12"/>
+      <c r="AMJ33" s="12"/>
+    </row>
+    <row r="34" spans="1:1024" ht="15" customHeight="1">
+      <c r="A34" s="120" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="120"/>
+      <c r="C34" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="104"/>
-      <c r="E34" s="104"/>
-      <c r="F34" s="106" t="s">
-        <v>13</v>
-      </c>
+      <c r="D34" s="121"/>
+      <c r="E34" s="121"/>
+      <c r="F34" s="122"/>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="105"/>
-      <c r="B35" s="105"/>
-      <c r="C35" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="F35" s="106"/>
+    <row r="35" spans="1:1024" ht="15" customHeight="1">
+      <c r="A35" s="102"/>
+      <c r="B35" s="102"/>
+      <c r="C35" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="81" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="81" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="101"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:1024">
       <c r="A36" s="58">
         <v>1</v>
       </c>
-      <c r="B36" s="59" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
+      <c r="B36" s="77" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="77"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="77"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:1024">
       <c r="A37" s="58">
         <v>2</v>
       </c>
-      <c r="B37" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="C37" s="57"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
+      <c r="B37" s="77" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="77"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="77"/>
     </row>
-    <row r="38" spans="1:6" ht="30">
+    <row r="38" spans="1:1024">
       <c r="A38" s="58">
         <v>3</v>
       </c>
-      <c r="B38" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="C38" s="57"/>
-      <c r="D38" s="57"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="57"/>
+      <c r="B38" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="77"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="77"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:1024">
       <c r="A39" s="58">
         <v>4</v>
       </c>
       <c r="B39" s="59" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="57"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="57"/>
+        <v>98</v>
+      </c>
+      <c r="C39" s="77"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="77"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1">
-      <c r="A42" s="102" t="s">
-        <v>98</v>
-      </c>
-      <c r="B42" s="102"/>
-      <c r="C42" s="103" t="s">
+    <row r="40" spans="1:1024">
+      <c r="A40" s="58">
+        <v>5</v>
+      </c>
+      <c r="B40" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" s="77"/>
+      <c r="D40" s="77"/>
+      <c r="E40" s="77"/>
+      <c r="F40" s="77"/>
+    </row>
+    <row r="41" spans="1:1024">
+      <c r="A41" s="58">
+        <v>6</v>
+      </c>
+      <c r="B41" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" s="77"/>
+      <c r="D41" s="77"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="77"/>
+    </row>
+    <row r="42" spans="1:1024">
+      <c r="A42" s="58">
+        <v>7</v>
+      </c>
+      <c r="B42" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" s="77"/>
+      <c r="D42" s="77"/>
+      <c r="E42" s="77"/>
+      <c r="F42" s="77"/>
+    </row>
+    <row r="43" spans="1:1024">
+      <c r="A43" s="58">
+        <v>8</v>
+      </c>
+      <c r="B43" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+    </row>
+    <row r="44" spans="1:1024">
+      <c r="A44" s="58">
+        <v>9</v>
+      </c>
+      <c r="B44" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="57"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="57"/>
+    </row>
+    <row r="46" spans="1:1024">
+      <c r="A46" s="106" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="106"/>
+      <c r="C46" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="D42" s="103"/>
-      <c r="E42" s="103"/>
-      <c r="F42" s="101"/>
+      <c r="D46" s="105"/>
+      <c r="E46" s="105"/>
+      <c r="F46" s="107" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1">
-      <c r="A43" s="102"/>
-      <c r="B43" s="102"/>
-      <c r="C43" s="77" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="77" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="101"/>
+    <row r="47" spans="1:1024">
+      <c r="A47" s="106"/>
+      <c r="B47" s="106"/>
+      <c r="C47" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="F47" s="107"/>
     </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="58">
+    <row r="48" spans="1:1024">
+      <c r="A48" s="58">
         <v>1</v>
       </c>
-      <c r="B44" s="78" t="s">
-        <v>100</v>
-      </c>
-      <c r="C44" s="78"/>
-      <c r="D44" s="78"/>
-      <c r="E44" s="78"/>
-      <c r="F44" s="78"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="58">
-        <v>2</v>
-      </c>
-      <c r="B45" s="78" t="s">
-        <v>101</v>
-      </c>
-      <c r="C45" s="78"/>
-      <c r="D45" s="78"/>
-      <c r="E45" s="78"/>
-      <c r="F45" s="78"/>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="58">
-        <v>3</v>
-      </c>
-      <c r="B46" s="78" t="s">
-        <v>102</v>
-      </c>
-      <c r="C46" s="78"/>
-      <c r="D46" s="78"/>
-      <c r="E46" s="78"/>
-      <c r="F46" s="78"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="58">
-        <v>4</v>
-      </c>
-      <c r="B47" s="59" t="s">
-        <v>99</v>
-      </c>
-      <c r="C47" s="78"/>
-      <c r="D47" s="78"/>
-      <c r="E47" s="78"/>
-      <c r="F47" s="78"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="58">
-        <v>5</v>
-      </c>
       <c r="B48" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48" s="78"/>
-      <c r="D48" s="78"/>
-      <c r="E48" s="78"/>
-      <c r="F48" s="78"/>
+        <v>79</v>
+      </c>
+      <c r="C48" s="57"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="57"/>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="58">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B49" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" s="78"/>
-      <c r="D49" s="78"/>
-      <c r="E49" s="78"/>
-      <c r="F49" s="78"/>
+        <v>83</v>
+      </c>
+      <c r="C49" s="57"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="57"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" ht="30">
       <c r="A50" s="58">
-        <v>7</v>
-      </c>
-      <c r="B50" s="78" t="s">
-        <v>105</v>
-      </c>
-      <c r="C50" s="78"/>
-      <c r="D50" s="78"/>
-      <c r="E50" s="78"/>
-      <c r="F50" s="78"/>
+        <v>3</v>
+      </c>
+      <c r="B50" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="58">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B51" s="59" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="C51" s="57"/>
       <c r="D51" s="57"/>
       <c r="E51" s="57"/>
       <c r="F51" s="57"/>
     </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="58">
+    <row r="54" spans="1:6">
+      <c r="A54" s="95" t="s">
+        <v>109</v>
+      </c>
+      <c r="B54" s="95"/>
+      <c r="C54" s="96" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="96"/>
+      <c r="E54" s="97"/>
+      <c r="F54" s="98" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="95"/>
+      <c r="B55" s="95"/>
+      <c r="C55" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B52" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="C52" s="57"/>
-      <c r="D52" s="57"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="57"/>
+      <c r="D55" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="99"/>
+    </row>
+    <row r="56" spans="1:6" ht="26.25">
+      <c r="A56" s="24">
+        <v>1</v>
+      </c>
+      <c r="B56" s="124" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="25"/>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="24">
+        <v>2</v>
+      </c>
+      <c r="B57" s="124" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="25"/>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="24">
+        <v>3</v>
+      </c>
+      <c r="B58" s="124" t="s">
+        <v>112</v>
+      </c>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="25"/>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="24">
+        <v>4</v>
+      </c>
+      <c r="B59" s="124" t="s">
+        <v>113</v>
+      </c>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="25"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="125">
+        <v>5</v>
+      </c>
+      <c r="B60" s="124" t="s">
+        <v>114</v>
+      </c>
+      <c r="C60" s="126"/>
+      <c r="D60" s="126"/>
+      <c r="E60" s="126"/>
+      <c r="F60" s="127"/>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="24">
+        <v>6</v>
+      </c>
+      <c r="B61" s="124" t="s">
+        <v>115</v>
+      </c>
+      <c r="C61" s="128"/>
+      <c r="D61" s="128"/>
+      <c r="E61" s="128"/>
+      <c r="F61" s="128"/>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="24">
+        <v>7</v>
+      </c>
+      <c r="B62" s="124" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" s="128"/>
+      <c r="D62" s="128"/>
+      <c r="E62" s="128"/>
+      <c r="F62" s="128"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="A42:B43"/>
-    <mergeCell ref="C42:E42"/>
+  <mergeCells count="18">
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="A54:B55"/>
+    <mergeCell ref="C54:E54"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A9:B10"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="A34:B35"/>
-    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="A46:B47"/>
+    <mergeCell ref="F46:F47"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="A14:B15"/>
     <mergeCell ref="C14:E14"/>
+    <mergeCell ref="A34:B35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -22553,10 +23779,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -22567,22 +23793,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="109" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="111" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="112"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="93" t="s">
+      <c r="D1" s="113"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="89" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="109"/>
-      <c r="B2" s="110"/>
+      <c r="A2" s="110"/>
+      <c r="B2" s="111"/>
       <c r="C2" s="73" t="s">
         <v>14</v>
       </c>
@@ -22592,13 +23818,13 @@
       <c r="E2" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="93"/>
+      <c r="F2" s="89"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="108" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="107"/>
+      <c r="B3" s="108"/>
       <c r="C3" s="74"/>
       <c r="D3" s="74"/>
       <c r="E3" s="75"/>
@@ -22633,41 +23859,41 @@
         <v>3</v>
       </c>
       <c r="B6" s="70" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="71"/>
       <c r="D6" s="71"/>
       <c r="E6" s="71"/>
       <c r="F6" s="72"/>
     </row>
-    <row r="7" spans="1:6" ht="26.25">
-      <c r="A7" s="69">
-        <v>4</v>
-      </c>
-      <c r="B7" s="70" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="72"/>
+    <row r="7" spans="1:6">
+      <c r="A7" s="108" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="108"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="74"/>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="107" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" s="107"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="74"/>
+    <row r="8" spans="1:6" ht="26.25">
+      <c r="A8" s="69">
+        <v>1</v>
+      </c>
+      <c r="B8" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="72"/>
     </row>
     <row r="9" spans="1:6" ht="26.25">
       <c r="A9" s="69">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" s="70" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C9" s="71"/>
       <c r="D9" s="71"/>
@@ -22676,71 +23902,59 @@
     </row>
     <row r="10" spans="1:6" ht="26.25">
       <c r="A10" s="69">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C10" s="71"/>
       <c r="D10" s="71"/>
       <c r="E10" s="71"/>
       <c r="F10" s="72"/>
     </row>
-    <row r="11" spans="1:6" ht="26.25">
+    <row r="11" spans="1:6" ht="39">
       <c r="A11" s="69">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B11" s="70" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C11" s="71"/>
       <c r="D11" s="71"/>
       <c r="E11" s="71"/>
       <c r="F11" s="72"/>
     </row>
-    <row r="12" spans="1:6" ht="39">
-      <c r="A12" s="69">
-        <v>7</v>
-      </c>
-      <c r="B12" s="70" t="s">
-        <v>96</v>
-      </c>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="72"/>
+    <row r="12" spans="1:6">
+      <c r="A12" s="108" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="108"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="74"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="107" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="107"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="74"/>
+      <c r="A13" s="69">
+        <v>8</v>
+      </c>
+      <c r="B13" s="72"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="72"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="69">
-        <v>8</v>
-      </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="72"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="B15" s="76"/>
+      <c r="B14" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Auditorias fisicas , incorporacion
</commit_message>
<xml_diff>
--- a/Organización/Calidad/PTL_Checklist_Calidad_aammdd.xlsx
+++ b/Organización/Calidad/PTL_Checklist_Calidad_aammdd.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095" activeTab="2"/>
+    <workbookView xWindow="420" yWindow="585" windowWidth="15615" windowHeight="7095"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
     <sheet name="procesos" sheetId="5" r:id="rId2"/>
     <sheet name="Productos" sheetId="7" r:id="rId3"/>
     <sheet name="Física" sheetId="8" r:id="rId4"/>
+    <sheet name="Funcional" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="134">
   <si>
     <t>DATOS GENERALES</t>
   </si>
@@ -143,9 +144,6 @@
   </si>
   <si>
     <t>¿Se encuentran estimadas las compras de materiales requeridas para la elaboración del proyecto?</t>
-  </si>
-  <si>
-    <t>¿El artefacto de analisís de requerimientos contempla todos los servicios que la empresa genera?</t>
   </si>
   <si>
     <t>Estimación</t>
@@ -343,9 +341,6 @@
     <t>Tickets de Servicio</t>
   </si>
   <si>
-    <t>¿Se identificó el producto a vender dentro de todas las opciones?</t>
-  </si>
-  <si>
     <t>Reporte de Monitoreo</t>
   </si>
   <si>
@@ -368,6 +363,63 @@
   </si>
   <si>
     <t>¿Se agregarón comentarios para el seguimiento de los riesgos ?</t>
+  </si>
+  <si>
+    <t>Líneas Base</t>
+  </si>
+  <si>
+    <t>Entregables</t>
+  </si>
+  <si>
+    <t>¿Se ha comunicado la creación/modificación de las líneas base?</t>
+  </si>
+  <si>
+    <t>¿El contenido de la linea base se ha generado de acuerdo a las plantillas de planeación?</t>
+  </si>
+  <si>
+    <t>¿Se tienen almacenados todos los elementos pertenecientes a la linea base?</t>
+  </si>
+  <si>
+    <t>¿Los documentos almacenados como linea bae se encuentran actualizados?</t>
+  </si>
+  <si>
+    <t>¿Se actualizaron todos los documentos que fueron involucrados en el documento control de cambios?</t>
+  </si>
+  <si>
+    <t>¿Se autorizo la solicitud de cambios por parte del CCC?</t>
+  </si>
+  <si>
+    <t>¿Se actualizó  la línea base de los productos afectadados?</t>
+  </si>
+  <si>
+    <t>¿El cliente aprobó el cambio solicitado?</t>
+  </si>
+  <si>
+    <t>¿Se cuenta con la documentación necesaria para ejecutar el cambio solicitado?</t>
+  </si>
+  <si>
+    <t>Funcional</t>
+  </si>
+  <si>
+    <t>¿El entregable cubre con la lista de los servicios/productos definidos al arranque del proyecto?</t>
+  </si>
+  <si>
+    <t>¿Todos los elementos a entregar fuerón contemplados en la estimación del proyecto?</t>
+  </si>
+  <si>
+    <t>¿Se encuentran registrados todos los tickets para aquellas actividades que no generan un documento físico?</t>
+  </si>
+  <si>
+    <t>¿La entrega del producto/servicio se encuentra planeada?</t>
+  </si>
+  <si>
+    <t>¿Se tiene identificado el producto/servicio(s) dentro del documento?</t>
+  </si>
+  <si>
+    <t>¿El documento cuenta con información que permita a los nuevos empleados saber algo acerca del producto, es decir cuenta con una pequeña descripción o funciones del producto?</t>
+  </si>
+  <si>
+    <t>¿Se tienen contemplados todos los productos que maneja la empresa en la actualidad?</t>
   </si>
 </sst>
 </file>
@@ -633,7 +685,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -857,6 +909,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0"/>
@@ -873,7 +934,7 @@
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="128">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1059,18 +1120,6 @@
     <xf numFmtId="165" fontId="8" fillId="14" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1079,9 +1128,6 @@
     </xf>
     <xf numFmtId="165" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="22" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1092,6 +1138,40 @@
     <xf numFmtId="165" fontId="0" fillId="21" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="15" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1101,6 +1181,16 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="8" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1126,16 +1216,6 @@
     <xf numFmtId="165" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1145,11 +1225,14 @@
     <xf numFmtId="165" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="21" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="20" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="20" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1164,6 +1247,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="10" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1187,47 +1276,15 @@
     <xf numFmtId="165" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="21" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="20" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="ConditionalStyle_1" xfId="1"/>
@@ -1545,10 +1602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ36"/>
+  <dimension ref="A1:AMJ44"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1567,66 +1624,66 @@
     <row r="1" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="2"/>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
     </row>
     <row r="4" spans="1:6" ht="15.75">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
     </row>
     <row r="6" spans="1:6" ht="13.9" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
+      <c r="C8" s="92"/>
+      <c r="D8" s="92"/>
+      <c r="E8" s="92"/>
+      <c r="F8" s="92"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="10" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="11" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="12" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="83"/>
-      <c r="D12" s="83"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
       <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1">
@@ -1725,11 +1782,11 @@
     <row r="21" spans="2:4" s="5" customFormat="1" ht="12.75"/>
     <row r="22" spans="2:4" s="5" customFormat="1" ht="12.75"/>
     <row r="23" spans="2:4" ht="15.75">
-      <c r="B23" s="83" t="s">
+      <c r="B23" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="90"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="6" t="s">
@@ -1762,74 +1819,74 @@
         <v>Requerimientos</v>
       </c>
       <c r="C26" s="66">
-        <f>COUNTA(Productos!C11:C12)</f>
+        <f>COUNTA(Productos!C11:C13)</f>
         <v>0</v>
       </c>
       <c r="D26" s="64" t="e">
-        <f>COUNTIF(Productos!C11:C12,"x")/(COUNTIF((Productos!C11:C12),"x")+COUNTIF((Productos!D11:D12),"x"))</f>
+        <f>COUNTIF(Productos!C11:C13,"x")/(COUNTIF((Productos!C11:C13),"x")+COUNTIF((Productos!D11:D13),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="67" t="str">
-        <f>Productos!A14</f>
+        <f>Productos!A15</f>
         <v>Plan de proyecto</v>
       </c>
       <c r="C27" s="68">
-        <f>COUNTA(Productos!C16:C32)</f>
+        <f>COUNTA(Productos!C17:C33)</f>
         <v>0</v>
       </c>
       <c r="D27" s="64" t="e">
-        <f>COUNTIF(Productos!C16:C32,"x")/(COUNTIF((Productos!C16:C32),"x")+COUNTIF((Productos!D16:D32),"x"))</f>
+        <f>COUNTIF(Productos!C17:C33,"x")/(COUNTIF((Productos!C17:C33),"x")+COUNTIF((Productos!D17:D33),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="61" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" s="68">
-        <f>COUNTA(Productos!C48:C51)</f>
+        <f>COUNTA(Productos!C49:C52)</f>
         <v>0</v>
       </c>
       <c r="D28" s="64" t="e">
-        <f>COUNTIF(Productos!C48:C51,"x")/(COUNTIF((Productos!C48:C51),"x")+COUNTIF((Productos!D48:D51),"x"))</f>
+        <f>COUNTIF(Productos!C49:C52,"x")/(COUNTIF((Productos!C49:C52),"x")+COUNTIF((Productos!D49:D52),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="61" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C29" s="68">
-        <f>COUNTA(Productos!C36:C44)</f>
+        <f>COUNTA(Productos!C37:C45)</f>
         <v>0</v>
       </c>
       <c r="D29" s="64" t="e">
-        <f>COUNTIF(Productos!C36:C44,"x")/(COUNTIF((Productos!C36:C44),"x")+COUNTIF((Productos!D36:D44),"x"))</f>
+        <f>COUNTIF(Productos!C37:C45,"x")/(COUNTIF((Productos!C37:C45),"x")+COUNTIF((Productos!D37:D45),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="30" spans="2:4">
-      <c r="B30" s="129" t="str">
-        <f>Productos!A54</f>
+      <c r="B30" s="61" t="str">
+        <f>Productos!A55</f>
         <v>Reporte de Monitoreo</v>
       </c>
       <c r="C30" s="68">
-        <f>COUNTA(Productos!C56:C62)</f>
+        <f>COUNTA(Productos!C57:C63)</f>
         <v>0</v>
       </c>
       <c r="D30" s="64" t="e">
-        <f>COUNTIF(Productos!C56:C62,"x")/(COUNTIF((Productos!C56:C62),"x")+COUNTIF((Productos!D56:D62),"x"))</f>
+        <f>COUNTIF(Productos!C57:C63,"x")/(COUNTIF((Productos!C57:C63),"x")+COUNTIF((Productos!D57:D63),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="18">
-      <c r="B32" s="82" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="82"/>
-      <c r="D32" s="82"/>
+      <c r="B32" s="89" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="89"/>
+      <c r="D32" s="89"/>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="6" t="s">
@@ -1843,49 +1900,110 @@
       </c>
     </row>
     <row r="34" spans="2:4">
-      <c r="B34" s="78" t="str">
+      <c r="B34" s="73" t="str">
         <f>Física!A3</f>
         <v>Elementos de Configuración</v>
       </c>
-      <c r="C34" s="79">
+      <c r="C34" s="74">
         <f>COUNTA(Física!C4:C6)</f>
         <v>0</v>
       </c>
-      <c r="D34" s="80" t="e">
+      <c r="D34" s="75" t="e">
         <f>COUNTIF(Física!C4:C6,"x")/(COUNTIF((Física!C4:C6),"x")+COUNTIF((Física!D4:D6),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="35" spans="2:4">
-      <c r="B35" s="78" t="str">
+      <c r="B35" s="73" t="str">
         <f>Física!A7</f>
         <v>Línea Base</v>
       </c>
-      <c r="C35" s="79">
+      <c r="C35" s="74">
         <f>COUNTA(Física!C8:C11)</f>
         <v>0</v>
       </c>
-      <c r="D35" s="80" t="e">
+      <c r="D35" s="75" t="e">
         <f>COUNTIF(Física!C8:C11,"x")/(COUNTIF((Física!C8:C11),"x")+COUNTIF((Física!D8:D11),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="36" spans="2:4">
-      <c r="B36" s="78" t="str">
+      <c r="B36" s="73" t="str">
         <f>Física!A12</f>
         <v>Control de Cambios</v>
       </c>
-      <c r="C36" s="79">
+      <c r="C36" s="74">
         <f>COUNTA(Física!C13:C13)</f>
         <v>0</v>
       </c>
-      <c r="D36" s="80" t="e">
+      <c r="D36" s="75" t="e">
         <f>COUNTIF(Física!C13:C13,"x")/(COUNTIF((Física!C13:C13),"x")+COUNTIF((Física!D13:D13),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
+    <row r="40" spans="2:4" ht="18">
+      <c r="B40" s="89" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" s="89"/>
+      <c r="D40" s="89"/>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="B42" s="73" t="str">
+        <f>Funcional!A4</f>
+        <v>Líneas Base</v>
+      </c>
+      <c r="C42" s="74">
+        <f>COUNTA(Funcional!C5:C8)</f>
+        <v>0</v>
+      </c>
+      <c r="D42" s="75" t="e">
+        <f>COUNTIF(Funcional!C5:C8,"x")/(COUNTIF((Funcional!C5:C8),"x")+COUNTIF((Funcional!D5:D8),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43" s="73" t="str">
+        <f>Funcional!A9</f>
+        <v>Control de Cambios</v>
+      </c>
+      <c r="C43" s="74">
+        <f>COUNTA(Funcional!C10:C13)</f>
+        <v>0</v>
+      </c>
+      <c r="D43" s="75" t="e">
+        <f>COUNTIF(Funcional!C10:C13,"x")/(COUNTIF((Funcional!C10:C13),"x")+COUNTIF((Funcional!D10:D13),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" s="73" t="str">
+        <f>Funcional!A14</f>
+        <v>Entregables</v>
+      </c>
+      <c r="C44" s="74">
+        <f>COUNTA(Funcional!C15:C18)</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="75" t="e">
+        <f>COUNTIF(Funcional!C15:C18,"x")/(COUNTIF((Funcional!C15:C18),"x")+COUNTIF((Funcional!D15:D18),"x"))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="B40:D40"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B12:D12"/>
@@ -1906,7 +2024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMI191"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
@@ -1920,22 +2038,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="86" t="s">
+      <c r="B1" s="102"/>
+      <c r="C1" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="87"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="89" t="s">
+      <c r="D1" s="98"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="100" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="92"/>
-      <c r="B2" s="93"/>
+      <c r="A2" s="103"/>
+      <c r="B2" s="104"/>
       <c r="C2" s="14" t="s">
         <v>14</v>
       </c>
@@ -1945,7 +2063,7 @@
       <c r="E2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="89"/>
+      <c r="F2" s="100"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="37">
@@ -1964,7 +2082,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -1998,22 +2116,22 @@
     <row r="7" spans="1:6" s="15" customFormat="1"/>
     <row r="8" spans="1:6" s="15" customFormat="1"/>
     <row r="9" spans="1:6" s="15" customFormat="1">
-      <c r="A9" s="95" t="s">
+      <c r="A9" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="95"/>
-      <c r="C9" s="96" t="s">
+      <c r="B9" s="94"/>
+      <c r="C9" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="96"/>
-      <c r="E9" s="97"/>
-      <c r="F9" s="98" t="s">
+      <c r="D9" s="95"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="105" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="15" customFormat="1">
-      <c r="A10" s="95"/>
-      <c r="B10" s="95"/>
+      <c r="A10" s="94"/>
+      <c r="B10" s="94"/>
       <c r="C10" s="36" t="s">
         <v>9</v>
       </c>
@@ -2023,14 +2141,14 @@
       <c r="E10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="99"/>
+      <c r="F10" s="106"/>
     </row>
     <row r="11" spans="1:6" s="15" customFormat="1">
       <c r="A11" s="24">
         <v>1</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="26"/>
       <c r="D11" s="26"/>
@@ -2054,7 +2172,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
@@ -2078,7 +2196,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="26"/>
       <c r="D15" s="26"/>
@@ -2114,7 +2232,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
@@ -2124,22 +2242,22 @@
     <row r="19" spans="1:6" s="15" customFormat="1"/>
     <row r="20" spans="1:6" s="15" customFormat="1"/>
     <row r="21" spans="1:6" s="15" customFormat="1">
-      <c r="A21" s="95" t="s">
+      <c r="A21" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="95"/>
-      <c r="C21" s="96" t="s">
+      <c r="B21" s="94"/>
+      <c r="C21" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="96"/>
-      <c r="E21" s="97"/>
-      <c r="F21" s="98" t="s">
+      <c r="D21" s="95"/>
+      <c r="E21" s="96"/>
+      <c r="F21" s="105" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="15" customFormat="1">
-      <c r="A22" s="95"/>
-      <c r="B22" s="95"/>
+      <c r="A22" s="94"/>
+      <c r="B22" s="94"/>
       <c r="C22" s="31" t="s">
         <v>9</v>
       </c>
@@ -2149,14 +2267,14 @@
       <c r="E22" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="100"/>
+      <c r="F22" s="107"/>
     </row>
     <row r="23" spans="1:6" s="15" customFormat="1">
       <c r="A23" s="47">
         <v>1</v>
       </c>
       <c r="B23" s="43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="44"/>
       <c r="D23" s="44"/>
@@ -2180,7 +2298,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="44"/>
       <c r="D25" s="44"/>
@@ -2214,22 +2332,22 @@
     <row r="28" spans="1:6" s="15" customFormat="1"/>
     <row r="29" spans="1:6" s="15" customFormat="1"/>
     <row r="30" spans="1:6" s="15" customFormat="1">
-      <c r="A30" s="95" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" s="95"/>
-      <c r="C30" s="96" t="s">
+      <c r="A30" s="94" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="94"/>
+      <c r="C30" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="96"/>
-      <c r="E30" s="97"/>
-      <c r="F30" s="98" t="s">
+      <c r="D30" s="95"/>
+      <c r="E30" s="96"/>
+      <c r="F30" s="105" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="15" customFormat="1">
-      <c r="A31" s="95"/>
-      <c r="B31" s="95"/>
+      <c r="A31" s="94"/>
+      <c r="B31" s="94"/>
       <c r="C31" s="32" t="s">
         <v>9</v>
       </c>
@@ -2239,14 +2357,14 @@
       <c r="E31" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="100"/>
+      <c r="F31" s="107"/>
     </row>
     <row r="32" spans="1:6" s="15" customFormat="1">
       <c r="A32" s="47">
         <v>1</v>
       </c>
       <c r="B32" s="43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" s="44"/>
       <c r="D32" s="44"/>
@@ -2258,7 +2376,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" s="44"/>
       <c r="D33" s="44"/>
@@ -2270,7 +2388,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C34" s="44"/>
       <c r="D34" s="44"/>
@@ -2282,7 +2400,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" s="44"/>
       <c r="D35" s="44"/>
@@ -2293,22 +2411,22 @@
     <row r="37" spans="1:6" s="15" customFormat="1"/>
     <row r="38" spans="1:6" s="15" customFormat="1"/>
     <row r="39" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A39" s="95" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="95"/>
-      <c r="C39" s="96" t="s">
+      <c r="A39" s="94" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="94"/>
+      <c r="C39" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="96"/>
-      <c r="E39" s="97"/>
-      <c r="F39" s="98" t="s">
+      <c r="D39" s="95"/>
+      <c r="E39" s="96"/>
+      <c r="F39" s="105" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A40" s="95"/>
-      <c r="B40" s="95"/>
+      <c r="A40" s="94"/>
+      <c r="B40" s="94"/>
       <c r="C40" s="36" t="s">
         <v>9</v>
       </c>
@@ -2318,14 +2436,14 @@
       <c r="E40" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F40" s="99"/>
+      <c r="F40" s="106"/>
     </row>
     <row r="41" spans="1:6" s="15" customFormat="1">
       <c r="A41" s="24">
         <v>1</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C41" s="26"/>
       <c r="D41" s="26"/>
@@ -2337,7 +2455,7 @@
         <v>2</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
@@ -2349,7 +2467,7 @@
         <v>3</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
@@ -2361,7 +2479,7 @@
         <v>4</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
@@ -2370,28 +2488,28 @@
     </row>
     <row r="45" spans="1:6" s="15" customFormat="1"/>
     <row r="46" spans="1:6" s="15" customFormat="1">
-      <c r="B46" s="94"/>
-      <c r="C46" s="94"/>
-      <c r="D46" s="94"/>
-      <c r="E46" s="94"/>
+      <c r="B46" s="93"/>
+      <c r="C46" s="93"/>
+      <c r="D46" s="93"/>
+      <c r="E46" s="93"/>
     </row>
     <row r="47" spans="1:6" s="15" customFormat="1">
-      <c r="A47" s="95" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" s="95"/>
-      <c r="C47" s="96" t="s">
+      <c r="A47" s="94" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" s="94"/>
+      <c r="C47" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="96"/>
-      <c r="E47" s="97"/>
-      <c r="F47" s="98" t="s">
+      <c r="D47" s="95"/>
+      <c r="E47" s="96"/>
+      <c r="F47" s="105" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="15" customFormat="1">
-      <c r="A48" s="95"/>
-      <c r="B48" s="95"/>
+      <c r="A48" s="94"/>
+      <c r="B48" s="94"/>
       <c r="C48" s="36" t="s">
         <v>9</v>
       </c>
@@ -2401,14 +2519,14 @@
       <c r="E48" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F48" s="99"/>
+      <c r="F48" s="106"/>
     </row>
     <row r="49" spans="1:6" s="15" customFormat="1">
       <c r="A49" s="24">
         <v>2</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C49" s="26"/>
       <c r="D49" s="26"/>
@@ -2420,7 +2538,7 @@
         <v>3</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C50" s="26"/>
       <c r="D50" s="26"/>
@@ -2432,7 +2550,7 @@
         <v>4</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C51" s="26"/>
       <c r="D51" s="26"/>
@@ -2444,7 +2562,7 @@
         <v>5</v>
       </c>
       <c r="B52" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C52" s="26"/>
       <c r="D52" s="26"/>
@@ -2456,7 +2574,7 @@
         <v>6</v>
       </c>
       <c r="B53" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C53" s="26"/>
       <c r="D53" s="26"/>
@@ -2478,10 +2596,10 @@
     <row r="66" spans="2:5" s="15" customFormat="1"/>
     <row r="67" spans="2:5" s="15" customFormat="1"/>
     <row r="68" spans="2:5" s="15" customFormat="1">
-      <c r="B68" s="94"/>
-      <c r="C68" s="94"/>
-      <c r="D68" s="94"/>
-      <c r="E68" s="94"/>
+      <c r="B68" s="93"/>
+      <c r="C68" s="93"/>
+      <c r="D68" s="93"/>
+      <c r="E68" s="93"/>
     </row>
     <row r="69" spans="2:5" s="15" customFormat="1"/>
     <row r="70" spans="2:5" s="15" customFormat="1">
@@ -2499,10 +2617,10 @@
     <row r="78" spans="2:5" s="15" customFormat="1"/>
     <row r="79" spans="2:5" s="15" customFormat="1"/>
     <row r="80" spans="2:5" s="15" customFormat="1">
-      <c r="B80" s="94"/>
-      <c r="C80" s="94"/>
-      <c r="D80" s="94"/>
-      <c r="E80" s="94"/>
+      <c r="B80" s="93"/>
+      <c r="C80" s="93"/>
+      <c r="D80" s="93"/>
+      <c r="E80" s="93"/>
     </row>
     <row r="81" spans="2:5" s="15" customFormat="1"/>
     <row r="82" spans="2:5" s="15" customFormat="1">
@@ -2524,10 +2642,10 @@
     <row r="94" spans="2:5" s="15" customFormat="1"/>
     <row r="95" spans="2:5" s="15" customFormat="1"/>
     <row r="96" spans="2:5" s="15" customFormat="1">
-      <c r="B96" s="94"/>
-      <c r="C96" s="94"/>
-      <c r="D96" s="94"/>
-      <c r="E96" s="94"/>
+      <c r="B96" s="93"/>
+      <c r="C96" s="93"/>
+      <c r="D96" s="93"/>
+      <c r="E96" s="93"/>
     </row>
     <row r="97" spans="3:5" s="15" customFormat="1"/>
     <row r="98" spans="3:5" s="15" customFormat="1">
@@ -2630,12 +2748,6 @@
     <row r="191" s="15" customFormat="1"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B96:E96"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="A9:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="C21:E21"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:B2"/>
@@ -2652,6 +2764,12 @@
     <mergeCell ref="A47:B48"/>
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="F47:F48"/>
+    <mergeCell ref="B96:E96"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="A9:B10"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="C21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
   <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2661,10 +2779,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ62"/>
+  <dimension ref="A1:AMJ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2674,22 +2792,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024">
-      <c r="A1" s="95" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="96" t="s">
+      <c r="A1" s="94" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="94"/>
+      <c r="C1" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="96"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="98" t="s">
+      <c r="D1" s="95"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="105" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1024">
-      <c r="A2" s="95"/>
-      <c r="B2" s="95"/>
+      <c r="A2" s="94"/>
+      <c r="B2" s="94"/>
       <c r="C2" s="31" t="s">
         <v>9</v>
       </c>
@@ -2699,7 +2817,7 @@
       <c r="E2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="100"/>
+      <c r="F2" s="107"/>
     </row>
     <row r="3" spans="1:1024" ht="30">
       <c r="A3" s="50">
@@ -2718,7 +2836,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="55"/>
       <c r="D4" s="55"/>
@@ -2742,7 +2860,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="57"/>
       <c r="D6" s="57"/>
@@ -2754,7 +2872,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="54" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="57"/>
       <c r="D7" s="57"/>
@@ -2770,22 +2888,22 @@
       <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:1024" ht="15" customHeight="1">
-      <c r="A9" s="95" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="95"/>
-      <c r="C9" s="96" t="s">
+      <c r="A9" s="94" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="94"/>
+      <c r="C9" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="96"/>
-      <c r="E9" s="97"/>
-      <c r="F9" s="98" t="s">
+      <c r="D9" s="95"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="105" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:1024" ht="15" customHeight="1">
-      <c r="A10" s="103"/>
-      <c r="B10" s="103"/>
+      <c r="A10" s="111"/>
+      <c r="B10" s="111"/>
       <c r="C10" s="36" t="s">
         <v>9</v>
       </c>
@@ -2795,26 +2913,26 @@
       <c r="E10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="104"/>
+      <c r="F10" s="112"/>
     </row>
-    <row r="11" spans="1:1024" ht="30">
+    <row r="11" spans="1:1024">
       <c r="A11" s="48">
         <v>1</v>
       </c>
       <c r="B11" s="54" t="s">
-        <v>42</v>
+        <v>131</v>
       </c>
       <c r="C11" s="55"/>
       <c r="D11" s="55"/>
       <c r="E11" s="55"/>
       <c r="F11" s="56"/>
     </row>
-    <row r="12" spans="1:1024">
+    <row r="12" spans="1:1024" ht="45">
       <c r="A12" s="48">
         <v>2</v>
       </c>
       <c r="B12" s="54" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="C12" s="55"/>
       <c r="D12" s="55"/>
@@ -2822,1058 +2940,38 @@
       <c r="F12" s="56"/>
     </row>
     <row r="13" spans="1:1024">
-      <c r="A13" s="35"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
+      <c r="A13" s="48">
+        <v>3</v>
+      </c>
+      <c r="B13" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="56"/>
     </row>
-    <row r="14" spans="1:1024" ht="15" customHeight="1">
-      <c r="A14" s="95" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="95"/>
-      <c r="C14" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="96"/>
-      <c r="E14" s="97"/>
-      <c r="F14" s="98" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="12"/>
-      <c r="V14" s="12"/>
-      <c r="W14" s="12"/>
-      <c r="X14" s="12"/>
-      <c r="Y14" s="12"/>
-      <c r="Z14" s="12"/>
-      <c r="AA14" s="12"/>
-      <c r="AB14" s="12"/>
-      <c r="AC14" s="12"/>
-      <c r="AD14" s="12"/>
-      <c r="AE14" s="12"/>
-      <c r="AF14" s="12"/>
-      <c r="AG14" s="12"/>
-      <c r="AH14" s="12"/>
-      <c r="AI14" s="12"/>
-      <c r="AJ14" s="12"/>
-      <c r="AK14" s="12"/>
-      <c r="AL14" s="12"/>
-      <c r="AM14" s="12"/>
-      <c r="AN14" s="12"/>
-      <c r="AO14" s="12"/>
-      <c r="AP14" s="12"/>
-      <c r="AQ14" s="12"/>
-      <c r="AR14" s="12"/>
-      <c r="AS14" s="12"/>
-      <c r="AT14" s="12"/>
-      <c r="AU14" s="12"/>
-      <c r="AV14" s="12"/>
-      <c r="AW14" s="12"/>
-      <c r="AX14" s="12"/>
-      <c r="AY14" s="12"/>
-      <c r="AZ14" s="12"/>
-      <c r="BA14" s="12"/>
-      <c r="BB14" s="12"/>
-      <c r="BC14" s="12"/>
-      <c r="BD14" s="12"/>
-      <c r="BE14" s="12"/>
-      <c r="BF14" s="12"/>
-      <c r="BG14" s="12"/>
-      <c r="BH14" s="12"/>
-      <c r="BI14" s="12"/>
-      <c r="BJ14" s="12"/>
-      <c r="BK14" s="12"/>
-      <c r="BL14" s="12"/>
-      <c r="BM14" s="12"/>
-      <c r="BN14" s="12"/>
-      <c r="BO14" s="12"/>
-      <c r="BP14" s="12"/>
-      <c r="BQ14" s="12"/>
-      <c r="BR14" s="12"/>
-      <c r="BS14" s="12"/>
-      <c r="BT14" s="12"/>
-      <c r="BU14" s="12"/>
-      <c r="BV14" s="12"/>
-      <c r="BW14" s="12"/>
-      <c r="BX14" s="12"/>
-      <c r="BY14" s="12"/>
-      <c r="BZ14" s="12"/>
-      <c r="CA14" s="12"/>
-      <c r="CB14" s="12"/>
-      <c r="CC14" s="12"/>
-      <c r="CD14" s="12"/>
-      <c r="CE14" s="12"/>
-      <c r="CF14" s="12"/>
-      <c r="CG14" s="12"/>
-      <c r="CH14" s="12"/>
-      <c r="CI14" s="12"/>
-      <c r="CJ14" s="12"/>
-      <c r="CK14" s="12"/>
-      <c r="CL14" s="12"/>
-      <c r="CM14" s="12"/>
-      <c r="CN14" s="12"/>
-      <c r="CO14" s="12"/>
-      <c r="CP14" s="12"/>
-      <c r="CQ14" s="12"/>
-      <c r="CR14" s="12"/>
-      <c r="CS14" s="12"/>
-      <c r="CT14" s="12"/>
-      <c r="CU14" s="12"/>
-      <c r="CV14" s="12"/>
-      <c r="CW14" s="12"/>
-      <c r="CX14" s="12"/>
-      <c r="CY14" s="12"/>
-      <c r="CZ14" s="12"/>
-      <c r="DA14" s="12"/>
-      <c r="DB14" s="12"/>
-      <c r="DC14" s="12"/>
-      <c r="DD14" s="12"/>
-      <c r="DE14" s="12"/>
-      <c r="DF14" s="12"/>
-      <c r="DG14" s="12"/>
-      <c r="DH14" s="12"/>
-      <c r="DI14" s="12"/>
-      <c r="DJ14" s="12"/>
-      <c r="DK14" s="12"/>
-      <c r="DL14" s="12"/>
-      <c r="DM14" s="12"/>
-      <c r="DN14" s="12"/>
-      <c r="DO14" s="12"/>
-      <c r="DP14" s="12"/>
-      <c r="DQ14" s="12"/>
-      <c r="DR14" s="12"/>
-      <c r="DS14" s="12"/>
-      <c r="DT14" s="12"/>
-      <c r="DU14" s="12"/>
-      <c r="DV14" s="12"/>
-      <c r="DW14" s="12"/>
-      <c r="DX14" s="12"/>
-      <c r="DY14" s="12"/>
-      <c r="DZ14" s="12"/>
-      <c r="EA14" s="12"/>
-      <c r="EB14" s="12"/>
-      <c r="EC14" s="12"/>
-      <c r="ED14" s="12"/>
-      <c r="EE14" s="12"/>
-      <c r="EF14" s="12"/>
-      <c r="EG14" s="12"/>
-      <c r="EH14" s="12"/>
-      <c r="EI14" s="12"/>
-      <c r="EJ14" s="12"/>
-      <c r="EK14" s="12"/>
-      <c r="EL14" s="12"/>
-      <c r="EM14" s="12"/>
-      <c r="EN14" s="12"/>
-      <c r="EO14" s="12"/>
-      <c r="EP14" s="12"/>
-      <c r="EQ14" s="12"/>
-      <c r="ER14" s="12"/>
-      <c r="ES14" s="12"/>
-      <c r="ET14" s="12"/>
-      <c r="EU14" s="12"/>
-      <c r="EV14" s="12"/>
-      <c r="EW14" s="12"/>
-      <c r="EX14" s="12"/>
-      <c r="EY14" s="12"/>
-      <c r="EZ14" s="12"/>
-      <c r="FA14" s="12"/>
-      <c r="FB14" s="12"/>
-      <c r="FC14" s="12"/>
-      <c r="FD14" s="12"/>
-      <c r="FE14" s="12"/>
-      <c r="FF14" s="12"/>
-      <c r="FG14" s="12"/>
-      <c r="FH14" s="12"/>
-      <c r="FI14" s="12"/>
-      <c r="FJ14" s="12"/>
-      <c r="FK14" s="12"/>
-      <c r="FL14" s="12"/>
-      <c r="FM14" s="12"/>
-      <c r="FN14" s="12"/>
-      <c r="FO14" s="12"/>
-      <c r="FP14" s="12"/>
-      <c r="FQ14" s="12"/>
-      <c r="FR14" s="12"/>
-      <c r="FS14" s="12"/>
-      <c r="FT14" s="12"/>
-      <c r="FU14" s="12"/>
-      <c r="FV14" s="12"/>
-      <c r="FW14" s="12"/>
-      <c r="FX14" s="12"/>
-      <c r="FY14" s="12"/>
-      <c r="FZ14" s="12"/>
-      <c r="GA14" s="12"/>
-      <c r="GB14" s="12"/>
-      <c r="GC14" s="12"/>
-      <c r="GD14" s="12"/>
-      <c r="GE14" s="12"/>
-      <c r="GF14" s="12"/>
-      <c r="GG14" s="12"/>
-      <c r="GH14" s="12"/>
-      <c r="GI14" s="12"/>
-      <c r="GJ14" s="12"/>
-      <c r="GK14" s="12"/>
-      <c r="GL14" s="12"/>
-      <c r="GM14" s="12"/>
-      <c r="GN14" s="12"/>
-      <c r="GO14" s="12"/>
-      <c r="GP14" s="12"/>
-      <c r="GQ14" s="12"/>
-      <c r="GR14" s="12"/>
-      <c r="GS14" s="12"/>
-      <c r="GT14" s="12"/>
-      <c r="GU14" s="12"/>
-      <c r="GV14" s="12"/>
-      <c r="GW14" s="12"/>
-      <c r="GX14" s="12"/>
-      <c r="GY14" s="12"/>
-      <c r="GZ14" s="12"/>
-      <c r="HA14" s="12"/>
-      <c r="HB14" s="12"/>
-      <c r="HC14" s="12"/>
-      <c r="HD14" s="12"/>
-      <c r="HE14" s="12"/>
-      <c r="HF14" s="12"/>
-      <c r="HG14" s="12"/>
-      <c r="HH14" s="12"/>
-      <c r="HI14" s="12"/>
-      <c r="HJ14" s="12"/>
-      <c r="HK14" s="12"/>
-      <c r="HL14" s="12"/>
-      <c r="HM14" s="12"/>
-      <c r="HN14" s="12"/>
-      <c r="HO14" s="12"/>
-      <c r="HP14" s="12"/>
-      <c r="HQ14" s="12"/>
-      <c r="HR14" s="12"/>
-      <c r="HS14" s="12"/>
-      <c r="HT14" s="12"/>
-      <c r="HU14" s="12"/>
-      <c r="HV14" s="12"/>
-      <c r="HW14" s="12"/>
-      <c r="HX14" s="12"/>
-      <c r="HY14" s="12"/>
-      <c r="HZ14" s="12"/>
-      <c r="IA14" s="12"/>
-      <c r="IB14" s="12"/>
-      <c r="IC14" s="12"/>
-      <c r="ID14" s="12"/>
-      <c r="IE14" s="12"/>
-      <c r="IF14" s="12"/>
-      <c r="IG14" s="12"/>
-      <c r="IH14" s="12"/>
-      <c r="II14" s="12"/>
-      <c r="IJ14" s="12"/>
-      <c r="IK14" s="12"/>
-      <c r="IL14" s="12"/>
-      <c r="IM14" s="12"/>
-      <c r="IN14" s="12"/>
-      <c r="IO14" s="12"/>
-      <c r="IP14" s="12"/>
-      <c r="IQ14" s="12"/>
-      <c r="IR14" s="12"/>
-      <c r="IS14" s="12"/>
-      <c r="IT14" s="12"/>
-      <c r="IU14" s="12"/>
-      <c r="IV14" s="12"/>
-      <c r="IW14" s="12"/>
-      <c r="IX14" s="12"/>
-      <c r="IY14" s="12"/>
-      <c r="IZ14" s="12"/>
-      <c r="JA14" s="12"/>
-      <c r="JB14" s="12"/>
-      <c r="JC14" s="12"/>
-      <c r="JD14" s="12"/>
-      <c r="JE14" s="12"/>
-      <c r="JF14" s="12"/>
-      <c r="JG14" s="12"/>
-      <c r="JH14" s="12"/>
-      <c r="JI14" s="12"/>
-      <c r="JJ14" s="12"/>
-      <c r="JK14" s="12"/>
-      <c r="JL14" s="12"/>
-      <c r="JM14" s="12"/>
-      <c r="JN14" s="12"/>
-      <c r="JO14" s="12"/>
-      <c r="JP14" s="12"/>
-      <c r="JQ14" s="12"/>
-      <c r="JR14" s="12"/>
-      <c r="JS14" s="12"/>
-      <c r="JT14" s="12"/>
-      <c r="JU14" s="12"/>
-      <c r="JV14" s="12"/>
-      <c r="JW14" s="12"/>
-      <c r="JX14" s="12"/>
-      <c r="JY14" s="12"/>
-      <c r="JZ14" s="12"/>
-      <c r="KA14" s="12"/>
-      <c r="KB14" s="12"/>
-      <c r="KC14" s="12"/>
-      <c r="KD14" s="12"/>
-      <c r="KE14" s="12"/>
-      <c r="KF14" s="12"/>
-      <c r="KG14" s="12"/>
-      <c r="KH14" s="12"/>
-      <c r="KI14" s="12"/>
-      <c r="KJ14" s="12"/>
-      <c r="KK14" s="12"/>
-      <c r="KL14" s="12"/>
-      <c r="KM14" s="12"/>
-      <c r="KN14" s="12"/>
-      <c r="KO14" s="12"/>
-      <c r="KP14" s="12"/>
-      <c r="KQ14" s="12"/>
-      <c r="KR14" s="12"/>
-      <c r="KS14" s="12"/>
-      <c r="KT14" s="12"/>
-      <c r="KU14" s="12"/>
-      <c r="KV14" s="12"/>
-      <c r="KW14" s="12"/>
-      <c r="KX14" s="12"/>
-      <c r="KY14" s="12"/>
-      <c r="KZ14" s="12"/>
-      <c r="LA14" s="12"/>
-      <c r="LB14" s="12"/>
-      <c r="LC14" s="12"/>
-      <c r="LD14" s="12"/>
-      <c r="LE14" s="12"/>
-      <c r="LF14" s="12"/>
-      <c r="LG14" s="12"/>
-      <c r="LH14" s="12"/>
-      <c r="LI14" s="12"/>
-      <c r="LJ14" s="12"/>
-      <c r="LK14" s="12"/>
-      <c r="LL14" s="12"/>
-      <c r="LM14" s="12"/>
-      <c r="LN14" s="12"/>
-      <c r="LO14" s="12"/>
-      <c r="LP14" s="12"/>
-      <c r="LQ14" s="12"/>
-      <c r="LR14" s="12"/>
-      <c r="LS14" s="12"/>
-      <c r="LT14" s="12"/>
-      <c r="LU14" s="12"/>
-      <c r="LV14" s="12"/>
-      <c r="LW14" s="12"/>
-      <c r="LX14" s="12"/>
-      <c r="LY14" s="12"/>
-      <c r="LZ14" s="12"/>
-      <c r="MA14" s="12"/>
-      <c r="MB14" s="12"/>
-      <c r="MC14" s="12"/>
-      <c r="MD14" s="12"/>
-      <c r="ME14" s="12"/>
-      <c r="MF14" s="12"/>
-      <c r="MG14" s="12"/>
-      <c r="MH14" s="12"/>
-      <c r="MI14" s="12"/>
-      <c r="MJ14" s="12"/>
-      <c r="MK14" s="12"/>
-      <c r="ML14" s="12"/>
-      <c r="MM14" s="12"/>
-      <c r="MN14" s="12"/>
-      <c r="MO14" s="12"/>
-      <c r="MP14" s="12"/>
-      <c r="MQ14" s="12"/>
-      <c r="MR14" s="12"/>
-      <c r="MS14" s="12"/>
-      <c r="MT14" s="12"/>
-      <c r="MU14" s="12"/>
-      <c r="MV14" s="12"/>
-      <c r="MW14" s="12"/>
-      <c r="MX14" s="12"/>
-      <c r="MY14" s="12"/>
-      <c r="MZ14" s="12"/>
-      <c r="NA14" s="12"/>
-      <c r="NB14" s="12"/>
-      <c r="NC14" s="12"/>
-      <c r="ND14" s="12"/>
-      <c r="NE14" s="12"/>
-      <c r="NF14" s="12"/>
-      <c r="NG14" s="12"/>
-      <c r="NH14" s="12"/>
-      <c r="NI14" s="12"/>
-      <c r="NJ14" s="12"/>
-      <c r="NK14" s="12"/>
-      <c r="NL14" s="12"/>
-      <c r="NM14" s="12"/>
-      <c r="NN14" s="12"/>
-      <c r="NO14" s="12"/>
-      <c r="NP14" s="12"/>
-      <c r="NQ14" s="12"/>
-      <c r="NR14" s="12"/>
-      <c r="NS14" s="12"/>
-      <c r="NT14" s="12"/>
-      <c r="NU14" s="12"/>
-      <c r="NV14" s="12"/>
-      <c r="NW14" s="12"/>
-      <c r="NX14" s="12"/>
-      <c r="NY14" s="12"/>
-      <c r="NZ14" s="12"/>
-      <c r="OA14" s="12"/>
-      <c r="OB14" s="12"/>
-      <c r="OC14" s="12"/>
-      <c r="OD14" s="12"/>
-      <c r="OE14" s="12"/>
-      <c r="OF14" s="12"/>
-      <c r="OG14" s="12"/>
-      <c r="OH14" s="12"/>
-      <c r="OI14" s="12"/>
-      <c r="OJ14" s="12"/>
-      <c r="OK14" s="12"/>
-      <c r="OL14" s="12"/>
-      <c r="OM14" s="12"/>
-      <c r="ON14" s="12"/>
-      <c r="OO14" s="12"/>
-      <c r="OP14" s="12"/>
-      <c r="OQ14" s="12"/>
-      <c r="OR14" s="12"/>
-      <c r="OS14" s="12"/>
-      <c r="OT14" s="12"/>
-      <c r="OU14" s="12"/>
-      <c r="OV14" s="12"/>
-      <c r="OW14" s="12"/>
-      <c r="OX14" s="12"/>
-      <c r="OY14" s="12"/>
-      <c r="OZ14" s="12"/>
-      <c r="PA14" s="12"/>
-      <c r="PB14" s="12"/>
-      <c r="PC14" s="12"/>
-      <c r="PD14" s="12"/>
-      <c r="PE14" s="12"/>
-      <c r="PF14" s="12"/>
-      <c r="PG14" s="12"/>
-      <c r="PH14" s="12"/>
-      <c r="PI14" s="12"/>
-      <c r="PJ14" s="12"/>
-      <c r="PK14" s="12"/>
-      <c r="PL14" s="12"/>
-      <c r="PM14" s="12"/>
-      <c r="PN14" s="12"/>
-      <c r="PO14" s="12"/>
-      <c r="PP14" s="12"/>
-      <c r="PQ14" s="12"/>
-      <c r="PR14" s="12"/>
-      <c r="PS14" s="12"/>
-      <c r="PT14" s="12"/>
-      <c r="PU14" s="12"/>
-      <c r="PV14" s="12"/>
-      <c r="PW14" s="12"/>
-      <c r="PX14" s="12"/>
-      <c r="PY14" s="12"/>
-      <c r="PZ14" s="12"/>
-      <c r="QA14" s="12"/>
-      <c r="QB14" s="12"/>
-      <c r="QC14" s="12"/>
-      <c r="QD14" s="12"/>
-      <c r="QE14" s="12"/>
-      <c r="QF14" s="12"/>
-      <c r="QG14" s="12"/>
-      <c r="QH14" s="12"/>
-      <c r="QI14" s="12"/>
-      <c r="QJ14" s="12"/>
-      <c r="QK14" s="12"/>
-      <c r="QL14" s="12"/>
-      <c r="QM14" s="12"/>
-      <c r="QN14" s="12"/>
-      <c r="QO14" s="12"/>
-      <c r="QP14" s="12"/>
-      <c r="QQ14" s="12"/>
-      <c r="QR14" s="12"/>
-      <c r="QS14" s="12"/>
-      <c r="QT14" s="12"/>
-      <c r="QU14" s="12"/>
-      <c r="QV14" s="12"/>
-      <c r="QW14" s="12"/>
-      <c r="QX14" s="12"/>
-      <c r="QY14" s="12"/>
-      <c r="QZ14" s="12"/>
-      <c r="RA14" s="12"/>
-      <c r="RB14" s="12"/>
-      <c r="RC14" s="12"/>
-      <c r="RD14" s="12"/>
-      <c r="RE14" s="12"/>
-      <c r="RF14" s="12"/>
-      <c r="RG14" s="12"/>
-      <c r="RH14" s="12"/>
-      <c r="RI14" s="12"/>
-      <c r="RJ14" s="12"/>
-      <c r="RK14" s="12"/>
-      <c r="RL14" s="12"/>
-      <c r="RM14" s="12"/>
-      <c r="RN14" s="12"/>
-      <c r="RO14" s="12"/>
-      <c r="RP14" s="12"/>
-      <c r="RQ14" s="12"/>
-      <c r="RR14" s="12"/>
-      <c r="RS14" s="12"/>
-      <c r="RT14" s="12"/>
-      <c r="RU14" s="12"/>
-      <c r="RV14" s="12"/>
-      <c r="RW14" s="12"/>
-      <c r="RX14" s="12"/>
-      <c r="RY14" s="12"/>
-      <c r="RZ14" s="12"/>
-      <c r="SA14" s="12"/>
-      <c r="SB14" s="12"/>
-      <c r="SC14" s="12"/>
-      <c r="SD14" s="12"/>
-      <c r="SE14" s="12"/>
-      <c r="SF14" s="12"/>
-      <c r="SG14" s="12"/>
-      <c r="SH14" s="12"/>
-      <c r="SI14" s="12"/>
-      <c r="SJ14" s="12"/>
-      <c r="SK14" s="12"/>
-      <c r="SL14" s="12"/>
-      <c r="SM14" s="12"/>
-      <c r="SN14" s="12"/>
-      <c r="SO14" s="12"/>
-      <c r="SP14" s="12"/>
-      <c r="SQ14" s="12"/>
-      <c r="SR14" s="12"/>
-      <c r="SS14" s="12"/>
-      <c r="ST14" s="12"/>
-      <c r="SU14" s="12"/>
-      <c r="SV14" s="12"/>
-      <c r="SW14" s="12"/>
-      <c r="SX14" s="12"/>
-      <c r="SY14" s="12"/>
-      <c r="SZ14" s="12"/>
-      <c r="TA14" s="12"/>
-      <c r="TB14" s="12"/>
-      <c r="TC14" s="12"/>
-      <c r="TD14" s="12"/>
-      <c r="TE14" s="12"/>
-      <c r="TF14" s="12"/>
-      <c r="TG14" s="12"/>
-      <c r="TH14" s="12"/>
-      <c r="TI14" s="12"/>
-      <c r="TJ14" s="12"/>
-      <c r="TK14" s="12"/>
-      <c r="TL14" s="12"/>
-      <c r="TM14" s="12"/>
-      <c r="TN14" s="12"/>
-      <c r="TO14" s="12"/>
-      <c r="TP14" s="12"/>
-      <c r="TQ14" s="12"/>
-      <c r="TR14" s="12"/>
-      <c r="TS14" s="12"/>
-      <c r="TT14" s="12"/>
-      <c r="TU14" s="12"/>
-      <c r="TV14" s="12"/>
-      <c r="TW14" s="12"/>
-      <c r="TX14" s="12"/>
-      <c r="TY14" s="12"/>
-      <c r="TZ14" s="12"/>
-      <c r="UA14" s="12"/>
-      <c r="UB14" s="12"/>
-      <c r="UC14" s="12"/>
-      <c r="UD14" s="12"/>
-      <c r="UE14" s="12"/>
-      <c r="UF14" s="12"/>
-      <c r="UG14" s="12"/>
-      <c r="UH14" s="12"/>
-      <c r="UI14" s="12"/>
-      <c r="UJ14" s="12"/>
-      <c r="UK14" s="12"/>
-      <c r="UL14" s="12"/>
-      <c r="UM14" s="12"/>
-      <c r="UN14" s="12"/>
-      <c r="UO14" s="12"/>
-      <c r="UP14" s="12"/>
-      <c r="UQ14" s="12"/>
-      <c r="UR14" s="12"/>
-      <c r="US14" s="12"/>
-      <c r="UT14" s="12"/>
-      <c r="UU14" s="12"/>
-      <c r="UV14" s="12"/>
-      <c r="UW14" s="12"/>
-      <c r="UX14" s="12"/>
-      <c r="UY14" s="12"/>
-      <c r="UZ14" s="12"/>
-      <c r="VA14" s="12"/>
-      <c r="VB14" s="12"/>
-      <c r="VC14" s="12"/>
-      <c r="VD14" s="12"/>
-      <c r="VE14" s="12"/>
-      <c r="VF14" s="12"/>
-      <c r="VG14" s="12"/>
-      <c r="VH14" s="12"/>
-      <c r="VI14" s="12"/>
-      <c r="VJ14" s="12"/>
-      <c r="VK14" s="12"/>
-      <c r="VL14" s="12"/>
-      <c r="VM14" s="12"/>
-      <c r="VN14" s="12"/>
-      <c r="VO14" s="12"/>
-      <c r="VP14" s="12"/>
-      <c r="VQ14" s="12"/>
-      <c r="VR14" s="12"/>
-      <c r="VS14" s="12"/>
-      <c r="VT14" s="12"/>
-      <c r="VU14" s="12"/>
-      <c r="VV14" s="12"/>
-      <c r="VW14" s="12"/>
-      <c r="VX14" s="12"/>
-      <c r="VY14" s="12"/>
-      <c r="VZ14" s="12"/>
-      <c r="WA14" s="12"/>
-      <c r="WB14" s="12"/>
-      <c r="WC14" s="12"/>
-      <c r="WD14" s="12"/>
-      <c r="WE14" s="12"/>
-      <c r="WF14" s="12"/>
-      <c r="WG14" s="12"/>
-      <c r="WH14" s="12"/>
-      <c r="WI14" s="12"/>
-      <c r="WJ14" s="12"/>
-      <c r="WK14" s="12"/>
-      <c r="WL14" s="12"/>
-      <c r="WM14" s="12"/>
-      <c r="WN14" s="12"/>
-      <c r="WO14" s="12"/>
-      <c r="WP14" s="12"/>
-      <c r="WQ14" s="12"/>
-      <c r="WR14" s="12"/>
-      <c r="WS14" s="12"/>
-      <c r="WT14" s="12"/>
-      <c r="WU14" s="12"/>
-      <c r="WV14" s="12"/>
-      <c r="WW14" s="12"/>
-      <c r="WX14" s="12"/>
-      <c r="WY14" s="12"/>
-      <c r="WZ14" s="12"/>
-      <c r="XA14" s="12"/>
-      <c r="XB14" s="12"/>
-      <c r="XC14" s="12"/>
-      <c r="XD14" s="12"/>
-      <c r="XE14" s="12"/>
-      <c r="XF14" s="12"/>
-      <c r="XG14" s="12"/>
-      <c r="XH14" s="12"/>
-      <c r="XI14" s="12"/>
-      <c r="XJ14" s="12"/>
-      <c r="XK14" s="12"/>
-      <c r="XL14" s="12"/>
-      <c r="XM14" s="12"/>
-      <c r="XN14" s="12"/>
-      <c r="XO14" s="12"/>
-      <c r="XP14" s="12"/>
-      <c r="XQ14" s="12"/>
-      <c r="XR14" s="12"/>
-      <c r="XS14" s="12"/>
-      <c r="XT14" s="12"/>
-      <c r="XU14" s="12"/>
-      <c r="XV14" s="12"/>
-      <c r="XW14" s="12"/>
-      <c r="XX14" s="12"/>
-      <c r="XY14" s="12"/>
-      <c r="XZ14" s="12"/>
-      <c r="YA14" s="12"/>
-      <c r="YB14" s="12"/>
-      <c r="YC14" s="12"/>
-      <c r="YD14" s="12"/>
-      <c r="YE14" s="12"/>
-      <c r="YF14" s="12"/>
-      <c r="YG14" s="12"/>
-      <c r="YH14" s="12"/>
-      <c r="YI14" s="12"/>
-      <c r="YJ14" s="12"/>
-      <c r="YK14" s="12"/>
-      <c r="YL14" s="12"/>
-      <c r="YM14" s="12"/>
-      <c r="YN14" s="12"/>
-      <c r="YO14" s="12"/>
-      <c r="YP14" s="12"/>
-      <c r="YQ14" s="12"/>
-      <c r="YR14" s="12"/>
-      <c r="YS14" s="12"/>
-      <c r="YT14" s="12"/>
-      <c r="YU14" s="12"/>
-      <c r="YV14" s="12"/>
-      <c r="YW14" s="12"/>
-      <c r="YX14" s="12"/>
-      <c r="YY14" s="12"/>
-      <c r="YZ14" s="12"/>
-      <c r="ZA14" s="12"/>
-      <c r="ZB14" s="12"/>
-      <c r="ZC14" s="12"/>
-      <c r="ZD14" s="12"/>
-      <c r="ZE14" s="12"/>
-      <c r="ZF14" s="12"/>
-      <c r="ZG14" s="12"/>
-      <c r="ZH14" s="12"/>
-      <c r="ZI14" s="12"/>
-      <c r="ZJ14" s="12"/>
-      <c r="ZK14" s="12"/>
-      <c r="ZL14" s="12"/>
-      <c r="ZM14" s="12"/>
-      <c r="ZN14" s="12"/>
-      <c r="ZO14" s="12"/>
-      <c r="ZP14" s="12"/>
-      <c r="ZQ14" s="12"/>
-      <c r="ZR14" s="12"/>
-      <c r="ZS14" s="12"/>
-      <c r="ZT14" s="12"/>
-      <c r="ZU14" s="12"/>
-      <c r="ZV14" s="12"/>
-      <c r="ZW14" s="12"/>
-      <c r="ZX14" s="12"/>
-      <c r="ZY14" s="12"/>
-      <c r="ZZ14" s="12"/>
-      <c r="AAA14" s="12"/>
-      <c r="AAB14" s="12"/>
-      <c r="AAC14" s="12"/>
-      <c r="AAD14" s="12"/>
-      <c r="AAE14" s="12"/>
-      <c r="AAF14" s="12"/>
-      <c r="AAG14" s="12"/>
-      <c r="AAH14" s="12"/>
-      <c r="AAI14" s="12"/>
-      <c r="AAJ14" s="12"/>
-      <c r="AAK14" s="12"/>
-      <c r="AAL14" s="12"/>
-      <c r="AAM14" s="12"/>
-      <c r="AAN14" s="12"/>
-      <c r="AAO14" s="12"/>
-      <c r="AAP14" s="12"/>
-      <c r="AAQ14" s="12"/>
-      <c r="AAR14" s="12"/>
-      <c r="AAS14" s="12"/>
-      <c r="AAT14" s="12"/>
-      <c r="AAU14" s="12"/>
-      <c r="AAV14" s="12"/>
-      <c r="AAW14" s="12"/>
-      <c r="AAX14" s="12"/>
-      <c r="AAY14" s="12"/>
-      <c r="AAZ14" s="12"/>
-      <c r="ABA14" s="12"/>
-      <c r="ABB14" s="12"/>
-      <c r="ABC14" s="12"/>
-      <c r="ABD14" s="12"/>
-      <c r="ABE14" s="12"/>
-      <c r="ABF14" s="12"/>
-      <c r="ABG14" s="12"/>
-      <c r="ABH14" s="12"/>
-      <c r="ABI14" s="12"/>
-      <c r="ABJ14" s="12"/>
-      <c r="ABK14" s="12"/>
-      <c r="ABL14" s="12"/>
-      <c r="ABM14" s="12"/>
-      <c r="ABN14" s="12"/>
-      <c r="ABO14" s="12"/>
-      <c r="ABP14" s="12"/>
-      <c r="ABQ14" s="12"/>
-      <c r="ABR14" s="12"/>
-      <c r="ABS14" s="12"/>
-      <c r="ABT14" s="12"/>
-      <c r="ABU14" s="12"/>
-      <c r="ABV14" s="12"/>
-      <c r="ABW14" s="12"/>
-      <c r="ABX14" s="12"/>
-      <c r="ABY14" s="12"/>
-      <c r="ABZ14" s="12"/>
-      <c r="ACA14" s="12"/>
-      <c r="ACB14" s="12"/>
-      <c r="ACC14" s="12"/>
-      <c r="ACD14" s="12"/>
-      <c r="ACE14" s="12"/>
-      <c r="ACF14" s="12"/>
-      <c r="ACG14" s="12"/>
-      <c r="ACH14" s="12"/>
-      <c r="ACI14" s="12"/>
-      <c r="ACJ14" s="12"/>
-      <c r="ACK14" s="12"/>
-      <c r="ACL14" s="12"/>
-      <c r="ACM14" s="12"/>
-      <c r="ACN14" s="12"/>
-      <c r="ACO14" s="12"/>
-      <c r="ACP14" s="12"/>
-      <c r="ACQ14" s="12"/>
-      <c r="ACR14" s="12"/>
-      <c r="ACS14" s="12"/>
-      <c r="ACT14" s="12"/>
-      <c r="ACU14" s="12"/>
-      <c r="ACV14" s="12"/>
-      <c r="ACW14" s="12"/>
-      <c r="ACX14" s="12"/>
-      <c r="ACY14" s="12"/>
-      <c r="ACZ14" s="12"/>
-      <c r="ADA14" s="12"/>
-      <c r="ADB14" s="12"/>
-      <c r="ADC14" s="12"/>
-      <c r="ADD14" s="12"/>
-      <c r="ADE14" s="12"/>
-      <c r="ADF14" s="12"/>
-      <c r="ADG14" s="12"/>
-      <c r="ADH14" s="12"/>
-      <c r="ADI14" s="12"/>
-      <c r="ADJ14" s="12"/>
-      <c r="ADK14" s="12"/>
-      <c r="ADL14" s="12"/>
-      <c r="ADM14" s="12"/>
-      <c r="ADN14" s="12"/>
-      <c r="ADO14" s="12"/>
-      <c r="ADP14" s="12"/>
-      <c r="ADQ14" s="12"/>
-      <c r="ADR14" s="12"/>
-      <c r="ADS14" s="12"/>
-      <c r="ADT14" s="12"/>
-      <c r="ADU14" s="12"/>
-      <c r="ADV14" s="12"/>
-      <c r="ADW14" s="12"/>
-      <c r="ADX14" s="12"/>
-      <c r="ADY14" s="12"/>
-      <c r="ADZ14" s="12"/>
-      <c r="AEA14" s="12"/>
-      <c r="AEB14" s="12"/>
-      <c r="AEC14" s="12"/>
-      <c r="AED14" s="12"/>
-      <c r="AEE14" s="12"/>
-      <c r="AEF14" s="12"/>
-      <c r="AEG14" s="12"/>
-      <c r="AEH14" s="12"/>
-      <c r="AEI14" s="12"/>
-      <c r="AEJ14" s="12"/>
-      <c r="AEK14" s="12"/>
-      <c r="AEL14" s="12"/>
-      <c r="AEM14" s="12"/>
-      <c r="AEN14" s="12"/>
-      <c r="AEO14" s="12"/>
-      <c r="AEP14" s="12"/>
-      <c r="AEQ14" s="12"/>
-      <c r="AER14" s="12"/>
-      <c r="AES14" s="12"/>
-      <c r="AET14" s="12"/>
-      <c r="AEU14" s="12"/>
-      <c r="AEV14" s="12"/>
-      <c r="AEW14" s="12"/>
-      <c r="AEX14" s="12"/>
-      <c r="AEY14" s="12"/>
-      <c r="AEZ14" s="12"/>
-      <c r="AFA14" s="12"/>
-      <c r="AFB14" s="12"/>
-      <c r="AFC14" s="12"/>
-      <c r="AFD14" s="12"/>
-      <c r="AFE14" s="12"/>
-      <c r="AFF14" s="12"/>
-      <c r="AFG14" s="12"/>
-      <c r="AFH14" s="12"/>
-      <c r="AFI14" s="12"/>
-      <c r="AFJ14" s="12"/>
-      <c r="AFK14" s="12"/>
-      <c r="AFL14" s="12"/>
-      <c r="AFM14" s="12"/>
-      <c r="AFN14" s="12"/>
-      <c r="AFO14" s="12"/>
-      <c r="AFP14" s="12"/>
-      <c r="AFQ14" s="12"/>
-      <c r="AFR14" s="12"/>
-      <c r="AFS14" s="12"/>
-      <c r="AFT14" s="12"/>
-      <c r="AFU14" s="12"/>
-      <c r="AFV14" s="12"/>
-      <c r="AFW14" s="12"/>
-      <c r="AFX14" s="12"/>
-      <c r="AFY14" s="12"/>
-      <c r="AFZ14" s="12"/>
-      <c r="AGA14" s="12"/>
-      <c r="AGB14" s="12"/>
-      <c r="AGC14" s="12"/>
-      <c r="AGD14" s="12"/>
-      <c r="AGE14" s="12"/>
-      <c r="AGF14" s="12"/>
-      <c r="AGG14" s="12"/>
-      <c r="AGH14" s="12"/>
-      <c r="AGI14" s="12"/>
-      <c r="AGJ14" s="12"/>
-      <c r="AGK14" s="12"/>
-      <c r="AGL14" s="12"/>
-      <c r="AGM14" s="12"/>
-      <c r="AGN14" s="12"/>
-      <c r="AGO14" s="12"/>
-      <c r="AGP14" s="12"/>
-      <c r="AGQ14" s="12"/>
-      <c r="AGR14" s="12"/>
-      <c r="AGS14" s="12"/>
-      <c r="AGT14" s="12"/>
-      <c r="AGU14" s="12"/>
-      <c r="AGV14" s="12"/>
-      <c r="AGW14" s="12"/>
-      <c r="AGX14" s="12"/>
-      <c r="AGY14" s="12"/>
-      <c r="AGZ14" s="12"/>
-      <c r="AHA14" s="12"/>
-      <c r="AHB14" s="12"/>
-      <c r="AHC14" s="12"/>
-      <c r="AHD14" s="12"/>
-      <c r="AHE14" s="12"/>
-      <c r="AHF14" s="12"/>
-      <c r="AHG14" s="12"/>
-      <c r="AHH14" s="12"/>
-      <c r="AHI14" s="12"/>
-      <c r="AHJ14" s="12"/>
-      <c r="AHK14" s="12"/>
-      <c r="AHL14" s="12"/>
-      <c r="AHM14" s="12"/>
-      <c r="AHN14" s="12"/>
-      <c r="AHO14" s="12"/>
-      <c r="AHP14" s="12"/>
-      <c r="AHQ14" s="12"/>
-      <c r="AHR14" s="12"/>
-      <c r="AHS14" s="12"/>
-      <c r="AHT14" s="12"/>
-      <c r="AHU14" s="12"/>
-      <c r="AHV14" s="12"/>
-      <c r="AHW14" s="12"/>
-      <c r="AHX14" s="12"/>
-      <c r="AHY14" s="12"/>
-      <c r="AHZ14" s="12"/>
-      <c r="AIA14" s="12"/>
-      <c r="AIB14" s="12"/>
-      <c r="AIC14" s="12"/>
-      <c r="AID14" s="12"/>
-      <c r="AIE14" s="12"/>
-      <c r="AIF14" s="12"/>
-      <c r="AIG14" s="12"/>
-      <c r="AIH14" s="12"/>
-      <c r="AII14" s="12"/>
-      <c r="AIJ14" s="12"/>
-      <c r="AIK14" s="12"/>
-      <c r="AIL14" s="12"/>
-      <c r="AIM14" s="12"/>
-      <c r="AIN14" s="12"/>
-      <c r="AIO14" s="12"/>
-      <c r="AIP14" s="12"/>
-      <c r="AIQ14" s="12"/>
-      <c r="AIR14" s="12"/>
-      <c r="AIS14" s="12"/>
-      <c r="AIT14" s="12"/>
-      <c r="AIU14" s="12"/>
-      <c r="AIV14" s="12"/>
-      <c r="AIW14" s="12"/>
-      <c r="AIX14" s="12"/>
-      <c r="AIY14" s="12"/>
-      <c r="AIZ14" s="12"/>
-      <c r="AJA14" s="12"/>
-      <c r="AJB14" s="12"/>
-      <c r="AJC14" s="12"/>
-      <c r="AJD14" s="12"/>
-      <c r="AJE14" s="12"/>
-      <c r="AJF14" s="12"/>
-      <c r="AJG14" s="12"/>
-      <c r="AJH14" s="12"/>
-      <c r="AJI14" s="12"/>
-      <c r="AJJ14" s="12"/>
-      <c r="AJK14" s="12"/>
-      <c r="AJL14" s="12"/>
-      <c r="AJM14" s="12"/>
-      <c r="AJN14" s="12"/>
-      <c r="AJO14" s="12"/>
-      <c r="AJP14" s="12"/>
-      <c r="AJQ14" s="12"/>
-      <c r="AJR14" s="12"/>
-      <c r="AJS14" s="12"/>
-      <c r="AJT14" s="12"/>
-      <c r="AJU14" s="12"/>
-      <c r="AJV14" s="12"/>
-      <c r="AJW14" s="12"/>
-      <c r="AJX14" s="12"/>
-      <c r="AJY14" s="12"/>
-      <c r="AJZ14" s="12"/>
-      <c r="AKA14" s="12"/>
-      <c r="AKB14" s="12"/>
-      <c r="AKC14" s="12"/>
-      <c r="AKD14" s="12"/>
-      <c r="AKE14" s="12"/>
-      <c r="AKF14" s="12"/>
-      <c r="AKG14" s="12"/>
-      <c r="AKH14" s="12"/>
-      <c r="AKI14" s="12"/>
-      <c r="AKJ14" s="12"/>
-      <c r="AKK14" s="12"/>
-      <c r="AKL14" s="12"/>
-      <c r="AKM14" s="12"/>
-      <c r="AKN14" s="12"/>
-      <c r="AKO14" s="12"/>
-      <c r="AKP14" s="12"/>
-      <c r="AKQ14" s="12"/>
-      <c r="AKR14" s="12"/>
-      <c r="AKS14" s="12"/>
-      <c r="AKT14" s="12"/>
-      <c r="AKU14" s="12"/>
-      <c r="AKV14" s="12"/>
-      <c r="AKW14" s="12"/>
-      <c r="AKX14" s="12"/>
-      <c r="AKY14" s="12"/>
-      <c r="AKZ14" s="12"/>
-      <c r="ALA14" s="12"/>
-      <c r="ALB14" s="12"/>
-      <c r="ALC14" s="12"/>
-      <c r="ALD14" s="12"/>
-      <c r="ALE14" s="12"/>
-      <c r="ALF14" s="12"/>
-      <c r="ALG14" s="12"/>
-      <c r="ALH14" s="12"/>
-      <c r="ALI14" s="12"/>
-      <c r="ALJ14" s="12"/>
-      <c r="ALK14" s="12"/>
-      <c r="ALL14" s="12"/>
-      <c r="ALM14" s="12"/>
-      <c r="ALN14" s="12"/>
-      <c r="ALO14" s="12"/>
-      <c r="ALP14" s="12"/>
-      <c r="ALQ14" s="12"/>
-      <c r="ALR14" s="12"/>
-      <c r="ALS14" s="12"/>
-      <c r="ALT14" s="12"/>
-      <c r="ALU14" s="12"/>
-      <c r="ALV14" s="12"/>
-      <c r="ALW14" s="12"/>
-      <c r="ALX14" s="12"/>
-      <c r="ALY14" s="12"/>
-      <c r="ALZ14" s="12"/>
-      <c r="AMA14" s="12"/>
-      <c r="AMB14" s="12"/>
-      <c r="AMC14" s="12"/>
-      <c r="AMD14" s="12"/>
-      <c r="AME14" s="12"/>
-      <c r="AMF14" s="12"/>
-      <c r="AMG14" s="12"/>
-      <c r="AMH14" s="12"/>
-      <c r="AMI14" s="12"/>
-      <c r="AMJ14" s="12"/>
+    <row r="14" spans="1:1024">
+      <c r="A14" s="35"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
     </row>
     <row r="15" spans="1:1024" ht="15" customHeight="1">
-      <c r="A15" s="95"/>
-      <c r="B15" s="95"/>
-      <c r="C15" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="100"/>
+      <c r="A15" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="94"/>
+      <c r="C15" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="95"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="105" t="s">
+        <v>13</v>
+      </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -4893,17 +3991,19 @@
       <c r="AMI15" s="12"/>
       <c r="AMJ15" s="12"/>
     </row>
-    <row r="16" spans="1:1024">
-      <c r="A16" s="47">
-        <v>1</v>
-      </c>
-      <c r="B16" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="45"/>
+    <row r="16" spans="1:1024" ht="15" customHeight="1">
+      <c r="A16" s="94"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="107"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
@@ -5924,11 +5024,11 @@
       <c r="AMJ16" s="12"/>
     </row>
     <row r="17" spans="1:1024">
-      <c r="A17" s="48">
-        <v>2</v>
-      </c>
-      <c r="B17" s="46" t="s">
-        <v>34</v>
+      <c r="A17" s="47">
+        <v>1</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>33</v>
       </c>
       <c r="C17" s="44"/>
       <c r="D17" s="44"/>
@@ -6955,10 +6055,10 @@
     </row>
     <row r="18" spans="1:1024">
       <c r="A18" s="48">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="44"/>
       <c r="D18" s="44"/>
@@ -7985,10 +7085,10 @@
     </row>
     <row r="19" spans="1:1024">
       <c r="A19" s="48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="44"/>
       <c r="D19" s="44"/>
@@ -9015,10 +8115,10 @@
     </row>
     <row r="20" spans="1:1024">
       <c r="A20" s="48">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="44"/>
       <c r="D20" s="44"/>
@@ -10045,10 +9145,10 @@
     </row>
     <row r="21" spans="1:1024">
       <c r="A21" s="48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="44"/>
       <c r="D21" s="44"/>
@@ -11073,12 +10173,12 @@
       <c r="AMI21" s="12"/>
       <c r="AMJ21" s="12"/>
     </row>
-    <row r="22" spans="1:1024" ht="30">
+    <row r="22" spans="1:1024">
       <c r="A22" s="48">
-        <v>7</v>
-      </c>
-      <c r="B22" s="49" t="s">
-        <v>53</v>
+        <v>6</v>
+      </c>
+      <c r="B22" s="46" t="s">
+        <v>38</v>
       </c>
       <c r="C22" s="44"/>
       <c r="D22" s="44"/>
@@ -12103,12 +11203,12 @@
       <c r="AMI22" s="12"/>
       <c r="AMJ22" s="12"/>
     </row>
-    <row r="23" spans="1:1024">
+    <row r="23" spans="1:1024" ht="30">
       <c r="A23" s="48">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="49" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C23" s="44"/>
       <c r="D23" s="44"/>
@@ -13135,10 +12235,10 @@
     </row>
     <row r="24" spans="1:1024">
       <c r="A24" s="48">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" s="49" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C24" s="44"/>
       <c r="D24" s="44"/>
@@ -14163,12 +13263,12 @@
       <c r="AMI24" s="12"/>
       <c r="AMJ24" s="12"/>
     </row>
-    <row r="25" spans="1:1024" ht="30">
+    <row r="25" spans="1:1024">
       <c r="A25" s="48">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" s="49" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C25" s="44"/>
       <c r="D25" s="44"/>
@@ -15193,9 +14293,9 @@
       <c r="AMI25" s="12"/>
       <c r="AMJ25" s="12"/>
     </row>
-    <row r="26" spans="1:1024">
+    <row r="26" spans="1:1024" ht="30">
       <c r="A26" s="48">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26" s="49" t="s">
         <v>55</v>
@@ -16225,7 +15325,7 @@
     </row>
     <row r="27" spans="1:1024">
       <c r="A27" s="48">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B27" s="49" t="s">
         <v>54</v>
@@ -17253,12 +16353,12 @@
       <c r="AMI27" s="12"/>
       <c r="AMJ27" s="12"/>
     </row>
-    <row r="28" spans="1:1024" ht="30">
+    <row r="28" spans="1:1024">
       <c r="A28" s="48">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B28" s="49" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="C28" s="44"/>
       <c r="D28" s="44"/>
@@ -18283,12 +17383,12 @@
       <c r="AMI28" s="12"/>
       <c r="AMJ28" s="12"/>
     </row>
-    <row r="29" spans="1:1024">
+    <row r="29" spans="1:1024" ht="30">
       <c r="A29" s="48">
-        <v>12</v>
-      </c>
-      <c r="B29" s="46" t="s">
-        <v>39</v>
+        <v>11</v>
+      </c>
+      <c r="B29" s="49" t="s">
+        <v>21</v>
       </c>
       <c r="C29" s="44"/>
       <c r="D29" s="44"/>
@@ -19315,10 +18415,10 @@
     </row>
     <row r="30" spans="1:1024">
       <c r="A30" s="48">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B30" s="46" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C30" s="44"/>
       <c r="D30" s="44"/>
@@ -20345,10 +19445,10 @@
     </row>
     <row r="31" spans="1:1024">
       <c r="A31" s="48">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C31" s="44"/>
       <c r="D31" s="44"/>
@@ -21374,16 +20474,16 @@
       <c r="AMJ31" s="12"/>
     </row>
     <row r="32" spans="1:1024">
-      <c r="A32" s="118">
-        <v>15</v>
-      </c>
-      <c r="B32" s="119" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="53"/>
+      <c r="A32" s="48">
+        <v>14</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="45"/>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
@@ -22404,12 +21504,16 @@
       <c r="AMJ32" s="12"/>
     </row>
     <row r="33" spans="1:1024">
-      <c r="A33" s="123"/>
-      <c r="B33" s="115"/>
-      <c r="C33" s="116"/>
-      <c r="D33" s="116"/>
-      <c r="E33" s="116"/>
-      <c r="F33" s="117"/>
+      <c r="A33" s="81">
+        <v>15</v>
+      </c>
+      <c r="B33" s="82" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="52"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="53"/>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
@@ -23429,262 +22533,1276 @@
       <c r="AMI33" s="12"/>
       <c r="AMJ33" s="12"/>
     </row>
-    <row r="34" spans="1:1024" ht="15" customHeight="1">
-      <c r="A34" s="120" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="120"/>
-      <c r="C34" s="121" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="121"/>
-      <c r="E34" s="121"/>
-      <c r="F34" s="122"/>
+    <row r="34" spans="1:1024">
+      <c r="A34" s="83"/>
+      <c r="B34" s="78"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="79"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
+      <c r="S34" s="12"/>
+      <c r="T34" s="12"/>
+      <c r="U34" s="12"/>
+      <c r="V34" s="12"/>
+      <c r="W34" s="12"/>
+      <c r="X34" s="12"/>
+      <c r="Y34" s="12"/>
+      <c r="Z34" s="12"/>
+      <c r="AA34" s="12"/>
+      <c r="AB34" s="12"/>
+      <c r="AC34" s="12"/>
+      <c r="AD34" s="12"/>
+      <c r="AE34" s="12"/>
+      <c r="AF34" s="12"/>
+      <c r="AG34" s="12"/>
+      <c r="AH34" s="12"/>
+      <c r="AI34" s="12"/>
+      <c r="AJ34" s="12"/>
+      <c r="AK34" s="12"/>
+      <c r="AL34" s="12"/>
+      <c r="AM34" s="12"/>
+      <c r="AN34" s="12"/>
+      <c r="AO34" s="12"/>
+      <c r="AP34" s="12"/>
+      <c r="AQ34" s="12"/>
+      <c r="AR34" s="12"/>
+      <c r="AS34" s="12"/>
+      <c r="AT34" s="12"/>
+      <c r="AU34" s="12"/>
+      <c r="AV34" s="12"/>
+      <c r="AW34" s="12"/>
+      <c r="AX34" s="12"/>
+      <c r="AY34" s="12"/>
+      <c r="AZ34" s="12"/>
+      <c r="BA34" s="12"/>
+      <c r="BB34" s="12"/>
+      <c r="BC34" s="12"/>
+      <c r="BD34" s="12"/>
+      <c r="BE34" s="12"/>
+      <c r="BF34" s="12"/>
+      <c r="BG34" s="12"/>
+      <c r="BH34" s="12"/>
+      <c r="BI34" s="12"/>
+      <c r="BJ34" s="12"/>
+      <c r="BK34" s="12"/>
+      <c r="BL34" s="12"/>
+      <c r="BM34" s="12"/>
+      <c r="BN34" s="12"/>
+      <c r="BO34" s="12"/>
+      <c r="BP34" s="12"/>
+      <c r="BQ34" s="12"/>
+      <c r="BR34" s="12"/>
+      <c r="BS34" s="12"/>
+      <c r="BT34" s="12"/>
+      <c r="BU34" s="12"/>
+      <c r="BV34" s="12"/>
+      <c r="BW34" s="12"/>
+      <c r="BX34" s="12"/>
+      <c r="BY34" s="12"/>
+      <c r="BZ34" s="12"/>
+      <c r="CA34" s="12"/>
+      <c r="CB34" s="12"/>
+      <c r="CC34" s="12"/>
+      <c r="CD34" s="12"/>
+      <c r="CE34" s="12"/>
+      <c r="CF34" s="12"/>
+      <c r="CG34" s="12"/>
+      <c r="CH34" s="12"/>
+      <c r="CI34" s="12"/>
+      <c r="CJ34" s="12"/>
+      <c r="CK34" s="12"/>
+      <c r="CL34" s="12"/>
+      <c r="CM34" s="12"/>
+      <c r="CN34" s="12"/>
+      <c r="CO34" s="12"/>
+      <c r="CP34" s="12"/>
+      <c r="CQ34" s="12"/>
+      <c r="CR34" s="12"/>
+      <c r="CS34" s="12"/>
+      <c r="CT34" s="12"/>
+      <c r="CU34" s="12"/>
+      <c r="CV34" s="12"/>
+      <c r="CW34" s="12"/>
+      <c r="CX34" s="12"/>
+      <c r="CY34" s="12"/>
+      <c r="CZ34" s="12"/>
+      <c r="DA34" s="12"/>
+      <c r="DB34" s="12"/>
+      <c r="DC34" s="12"/>
+      <c r="DD34" s="12"/>
+      <c r="DE34" s="12"/>
+      <c r="DF34" s="12"/>
+      <c r="DG34" s="12"/>
+      <c r="DH34" s="12"/>
+      <c r="DI34" s="12"/>
+      <c r="DJ34" s="12"/>
+      <c r="DK34" s="12"/>
+      <c r="DL34" s="12"/>
+      <c r="DM34" s="12"/>
+      <c r="DN34" s="12"/>
+      <c r="DO34" s="12"/>
+      <c r="DP34" s="12"/>
+      <c r="DQ34" s="12"/>
+      <c r="DR34" s="12"/>
+      <c r="DS34" s="12"/>
+      <c r="DT34" s="12"/>
+      <c r="DU34" s="12"/>
+      <c r="DV34" s="12"/>
+      <c r="DW34" s="12"/>
+      <c r="DX34" s="12"/>
+      <c r="DY34" s="12"/>
+      <c r="DZ34" s="12"/>
+      <c r="EA34" s="12"/>
+      <c r="EB34" s="12"/>
+      <c r="EC34" s="12"/>
+      <c r="ED34" s="12"/>
+      <c r="EE34" s="12"/>
+      <c r="EF34" s="12"/>
+      <c r="EG34" s="12"/>
+      <c r="EH34" s="12"/>
+      <c r="EI34" s="12"/>
+      <c r="EJ34" s="12"/>
+      <c r="EK34" s="12"/>
+      <c r="EL34" s="12"/>
+      <c r="EM34" s="12"/>
+      <c r="EN34" s="12"/>
+      <c r="EO34" s="12"/>
+      <c r="EP34" s="12"/>
+      <c r="EQ34" s="12"/>
+      <c r="ER34" s="12"/>
+      <c r="ES34" s="12"/>
+      <c r="ET34" s="12"/>
+      <c r="EU34" s="12"/>
+      <c r="EV34" s="12"/>
+      <c r="EW34" s="12"/>
+      <c r="EX34" s="12"/>
+      <c r="EY34" s="12"/>
+      <c r="EZ34" s="12"/>
+      <c r="FA34" s="12"/>
+      <c r="FB34" s="12"/>
+      <c r="FC34" s="12"/>
+      <c r="FD34" s="12"/>
+      <c r="FE34" s="12"/>
+      <c r="FF34" s="12"/>
+      <c r="FG34" s="12"/>
+      <c r="FH34" s="12"/>
+      <c r="FI34" s="12"/>
+      <c r="FJ34" s="12"/>
+      <c r="FK34" s="12"/>
+      <c r="FL34" s="12"/>
+      <c r="FM34" s="12"/>
+      <c r="FN34" s="12"/>
+      <c r="FO34" s="12"/>
+      <c r="FP34" s="12"/>
+      <c r="FQ34" s="12"/>
+      <c r="FR34" s="12"/>
+      <c r="FS34" s="12"/>
+      <c r="FT34" s="12"/>
+      <c r="FU34" s="12"/>
+      <c r="FV34" s="12"/>
+      <c r="FW34" s="12"/>
+      <c r="FX34" s="12"/>
+      <c r="FY34" s="12"/>
+      <c r="FZ34" s="12"/>
+      <c r="GA34" s="12"/>
+      <c r="GB34" s="12"/>
+      <c r="GC34" s="12"/>
+      <c r="GD34" s="12"/>
+      <c r="GE34" s="12"/>
+      <c r="GF34" s="12"/>
+      <c r="GG34" s="12"/>
+      <c r="GH34" s="12"/>
+      <c r="GI34" s="12"/>
+      <c r="GJ34" s="12"/>
+      <c r="GK34" s="12"/>
+      <c r="GL34" s="12"/>
+      <c r="GM34" s="12"/>
+      <c r="GN34" s="12"/>
+      <c r="GO34" s="12"/>
+      <c r="GP34" s="12"/>
+      <c r="GQ34" s="12"/>
+      <c r="GR34" s="12"/>
+      <c r="GS34" s="12"/>
+      <c r="GT34" s="12"/>
+      <c r="GU34" s="12"/>
+      <c r="GV34" s="12"/>
+      <c r="GW34" s="12"/>
+      <c r="GX34" s="12"/>
+      <c r="GY34" s="12"/>
+      <c r="GZ34" s="12"/>
+      <c r="HA34" s="12"/>
+      <c r="HB34" s="12"/>
+      <c r="HC34" s="12"/>
+      <c r="HD34" s="12"/>
+      <c r="HE34" s="12"/>
+      <c r="HF34" s="12"/>
+      <c r="HG34" s="12"/>
+      <c r="HH34" s="12"/>
+      <c r="HI34" s="12"/>
+      <c r="HJ34" s="12"/>
+      <c r="HK34" s="12"/>
+      <c r="HL34" s="12"/>
+      <c r="HM34" s="12"/>
+      <c r="HN34" s="12"/>
+      <c r="HO34" s="12"/>
+      <c r="HP34" s="12"/>
+      <c r="HQ34" s="12"/>
+      <c r="HR34" s="12"/>
+      <c r="HS34" s="12"/>
+      <c r="HT34" s="12"/>
+      <c r="HU34" s="12"/>
+      <c r="HV34" s="12"/>
+      <c r="HW34" s="12"/>
+      <c r="HX34" s="12"/>
+      <c r="HY34" s="12"/>
+      <c r="HZ34" s="12"/>
+      <c r="IA34" s="12"/>
+      <c r="IB34" s="12"/>
+      <c r="IC34" s="12"/>
+      <c r="ID34" s="12"/>
+      <c r="IE34" s="12"/>
+      <c r="IF34" s="12"/>
+      <c r="IG34" s="12"/>
+      <c r="IH34" s="12"/>
+      <c r="II34" s="12"/>
+      <c r="IJ34" s="12"/>
+      <c r="IK34" s="12"/>
+      <c r="IL34" s="12"/>
+      <c r="IM34" s="12"/>
+      <c r="IN34" s="12"/>
+      <c r="IO34" s="12"/>
+      <c r="IP34" s="12"/>
+      <c r="IQ34" s="12"/>
+      <c r="IR34" s="12"/>
+      <c r="IS34" s="12"/>
+      <c r="IT34" s="12"/>
+      <c r="IU34" s="12"/>
+      <c r="IV34" s="12"/>
+      <c r="IW34" s="12"/>
+      <c r="IX34" s="12"/>
+      <c r="IY34" s="12"/>
+      <c r="IZ34" s="12"/>
+      <c r="JA34" s="12"/>
+      <c r="JB34" s="12"/>
+      <c r="JC34" s="12"/>
+      <c r="JD34" s="12"/>
+      <c r="JE34" s="12"/>
+      <c r="JF34" s="12"/>
+      <c r="JG34" s="12"/>
+      <c r="JH34" s="12"/>
+      <c r="JI34" s="12"/>
+      <c r="JJ34" s="12"/>
+      <c r="JK34" s="12"/>
+      <c r="JL34" s="12"/>
+      <c r="JM34" s="12"/>
+      <c r="JN34" s="12"/>
+      <c r="JO34" s="12"/>
+      <c r="JP34" s="12"/>
+      <c r="JQ34" s="12"/>
+      <c r="JR34" s="12"/>
+      <c r="JS34" s="12"/>
+      <c r="JT34" s="12"/>
+      <c r="JU34" s="12"/>
+      <c r="JV34" s="12"/>
+      <c r="JW34" s="12"/>
+      <c r="JX34" s="12"/>
+      <c r="JY34" s="12"/>
+      <c r="JZ34" s="12"/>
+      <c r="KA34" s="12"/>
+      <c r="KB34" s="12"/>
+      <c r="KC34" s="12"/>
+      <c r="KD34" s="12"/>
+      <c r="KE34" s="12"/>
+      <c r="KF34" s="12"/>
+      <c r="KG34" s="12"/>
+      <c r="KH34" s="12"/>
+      <c r="KI34" s="12"/>
+      <c r="KJ34" s="12"/>
+      <c r="KK34" s="12"/>
+      <c r="KL34" s="12"/>
+      <c r="KM34" s="12"/>
+      <c r="KN34" s="12"/>
+      <c r="KO34" s="12"/>
+      <c r="KP34" s="12"/>
+      <c r="KQ34" s="12"/>
+      <c r="KR34" s="12"/>
+      <c r="KS34" s="12"/>
+      <c r="KT34" s="12"/>
+      <c r="KU34" s="12"/>
+      <c r="KV34" s="12"/>
+      <c r="KW34" s="12"/>
+      <c r="KX34" s="12"/>
+      <c r="KY34" s="12"/>
+      <c r="KZ34" s="12"/>
+      <c r="LA34" s="12"/>
+      <c r="LB34" s="12"/>
+      <c r="LC34" s="12"/>
+      <c r="LD34" s="12"/>
+      <c r="LE34" s="12"/>
+      <c r="LF34" s="12"/>
+      <c r="LG34" s="12"/>
+      <c r="LH34" s="12"/>
+      <c r="LI34" s="12"/>
+      <c r="LJ34" s="12"/>
+      <c r="LK34" s="12"/>
+      <c r="LL34" s="12"/>
+      <c r="LM34" s="12"/>
+      <c r="LN34" s="12"/>
+      <c r="LO34" s="12"/>
+      <c r="LP34" s="12"/>
+      <c r="LQ34" s="12"/>
+      <c r="LR34" s="12"/>
+      <c r="LS34" s="12"/>
+      <c r="LT34" s="12"/>
+      <c r="LU34" s="12"/>
+      <c r="LV34" s="12"/>
+      <c r="LW34" s="12"/>
+      <c r="LX34" s="12"/>
+      <c r="LY34" s="12"/>
+      <c r="LZ34" s="12"/>
+      <c r="MA34" s="12"/>
+      <c r="MB34" s="12"/>
+      <c r="MC34" s="12"/>
+      <c r="MD34" s="12"/>
+      <c r="ME34" s="12"/>
+      <c r="MF34" s="12"/>
+      <c r="MG34" s="12"/>
+      <c r="MH34" s="12"/>
+      <c r="MI34" s="12"/>
+      <c r="MJ34" s="12"/>
+      <c r="MK34" s="12"/>
+      <c r="ML34" s="12"/>
+      <c r="MM34" s="12"/>
+      <c r="MN34" s="12"/>
+      <c r="MO34" s="12"/>
+      <c r="MP34" s="12"/>
+      <c r="MQ34" s="12"/>
+      <c r="MR34" s="12"/>
+      <c r="MS34" s="12"/>
+      <c r="MT34" s="12"/>
+      <c r="MU34" s="12"/>
+      <c r="MV34" s="12"/>
+      <c r="MW34" s="12"/>
+      <c r="MX34" s="12"/>
+      <c r="MY34" s="12"/>
+      <c r="MZ34" s="12"/>
+      <c r="NA34" s="12"/>
+      <c r="NB34" s="12"/>
+      <c r="NC34" s="12"/>
+      <c r="ND34" s="12"/>
+      <c r="NE34" s="12"/>
+      <c r="NF34" s="12"/>
+      <c r="NG34" s="12"/>
+      <c r="NH34" s="12"/>
+      <c r="NI34" s="12"/>
+      <c r="NJ34" s="12"/>
+      <c r="NK34" s="12"/>
+      <c r="NL34" s="12"/>
+      <c r="NM34" s="12"/>
+      <c r="NN34" s="12"/>
+      <c r="NO34" s="12"/>
+      <c r="NP34" s="12"/>
+      <c r="NQ34" s="12"/>
+      <c r="NR34" s="12"/>
+      <c r="NS34" s="12"/>
+      <c r="NT34" s="12"/>
+      <c r="NU34" s="12"/>
+      <c r="NV34" s="12"/>
+      <c r="NW34" s="12"/>
+      <c r="NX34" s="12"/>
+      <c r="NY34" s="12"/>
+      <c r="NZ34" s="12"/>
+      <c r="OA34" s="12"/>
+      <c r="OB34" s="12"/>
+      <c r="OC34" s="12"/>
+      <c r="OD34" s="12"/>
+      <c r="OE34" s="12"/>
+      <c r="OF34" s="12"/>
+      <c r="OG34" s="12"/>
+      <c r="OH34" s="12"/>
+      <c r="OI34" s="12"/>
+      <c r="OJ34" s="12"/>
+      <c r="OK34" s="12"/>
+      <c r="OL34" s="12"/>
+      <c r="OM34" s="12"/>
+      <c r="ON34" s="12"/>
+      <c r="OO34" s="12"/>
+      <c r="OP34" s="12"/>
+      <c r="OQ34" s="12"/>
+      <c r="OR34" s="12"/>
+      <c r="OS34" s="12"/>
+      <c r="OT34" s="12"/>
+      <c r="OU34" s="12"/>
+      <c r="OV34" s="12"/>
+      <c r="OW34" s="12"/>
+      <c r="OX34" s="12"/>
+      <c r="OY34" s="12"/>
+      <c r="OZ34" s="12"/>
+      <c r="PA34" s="12"/>
+      <c r="PB34" s="12"/>
+      <c r="PC34" s="12"/>
+      <c r="PD34" s="12"/>
+      <c r="PE34" s="12"/>
+      <c r="PF34" s="12"/>
+      <c r="PG34" s="12"/>
+      <c r="PH34" s="12"/>
+      <c r="PI34" s="12"/>
+      <c r="PJ34" s="12"/>
+      <c r="PK34" s="12"/>
+      <c r="PL34" s="12"/>
+      <c r="PM34" s="12"/>
+      <c r="PN34" s="12"/>
+      <c r="PO34" s="12"/>
+      <c r="PP34" s="12"/>
+      <c r="PQ34" s="12"/>
+      <c r="PR34" s="12"/>
+      <c r="PS34" s="12"/>
+      <c r="PT34" s="12"/>
+      <c r="PU34" s="12"/>
+      <c r="PV34" s="12"/>
+      <c r="PW34" s="12"/>
+      <c r="PX34" s="12"/>
+      <c r="PY34" s="12"/>
+      <c r="PZ34" s="12"/>
+      <c r="QA34" s="12"/>
+      <c r="QB34" s="12"/>
+      <c r="QC34" s="12"/>
+      <c r="QD34" s="12"/>
+      <c r="QE34" s="12"/>
+      <c r="QF34" s="12"/>
+      <c r="QG34" s="12"/>
+      <c r="QH34" s="12"/>
+      <c r="QI34" s="12"/>
+      <c r="QJ34" s="12"/>
+      <c r="QK34" s="12"/>
+      <c r="QL34" s="12"/>
+      <c r="QM34" s="12"/>
+      <c r="QN34" s="12"/>
+      <c r="QO34" s="12"/>
+      <c r="QP34" s="12"/>
+      <c r="QQ34" s="12"/>
+      <c r="QR34" s="12"/>
+      <c r="QS34" s="12"/>
+      <c r="QT34" s="12"/>
+      <c r="QU34" s="12"/>
+      <c r="QV34" s="12"/>
+      <c r="QW34" s="12"/>
+      <c r="QX34" s="12"/>
+      <c r="QY34" s="12"/>
+      <c r="QZ34" s="12"/>
+      <c r="RA34" s="12"/>
+      <c r="RB34" s="12"/>
+      <c r="RC34" s="12"/>
+      <c r="RD34" s="12"/>
+      <c r="RE34" s="12"/>
+      <c r="RF34" s="12"/>
+      <c r="RG34" s="12"/>
+      <c r="RH34" s="12"/>
+      <c r="RI34" s="12"/>
+      <c r="RJ34" s="12"/>
+      <c r="RK34" s="12"/>
+      <c r="RL34" s="12"/>
+      <c r="RM34" s="12"/>
+      <c r="RN34" s="12"/>
+      <c r="RO34" s="12"/>
+      <c r="RP34" s="12"/>
+      <c r="RQ34" s="12"/>
+      <c r="RR34" s="12"/>
+      <c r="RS34" s="12"/>
+      <c r="RT34" s="12"/>
+      <c r="RU34" s="12"/>
+      <c r="RV34" s="12"/>
+      <c r="RW34" s="12"/>
+      <c r="RX34" s="12"/>
+      <c r="RY34" s="12"/>
+      <c r="RZ34" s="12"/>
+      <c r="SA34" s="12"/>
+      <c r="SB34" s="12"/>
+      <c r="SC34" s="12"/>
+      <c r="SD34" s="12"/>
+      <c r="SE34" s="12"/>
+      <c r="SF34" s="12"/>
+      <c r="SG34" s="12"/>
+      <c r="SH34" s="12"/>
+      <c r="SI34" s="12"/>
+      <c r="SJ34" s="12"/>
+      <c r="SK34" s="12"/>
+      <c r="SL34" s="12"/>
+      <c r="SM34" s="12"/>
+      <c r="SN34" s="12"/>
+      <c r="SO34" s="12"/>
+      <c r="SP34" s="12"/>
+      <c r="SQ34" s="12"/>
+      <c r="SR34" s="12"/>
+      <c r="SS34" s="12"/>
+      <c r="ST34" s="12"/>
+      <c r="SU34" s="12"/>
+      <c r="SV34" s="12"/>
+      <c r="SW34" s="12"/>
+      <c r="SX34" s="12"/>
+      <c r="SY34" s="12"/>
+      <c r="SZ34" s="12"/>
+      <c r="TA34" s="12"/>
+      <c r="TB34" s="12"/>
+      <c r="TC34" s="12"/>
+      <c r="TD34" s="12"/>
+      <c r="TE34" s="12"/>
+      <c r="TF34" s="12"/>
+      <c r="TG34" s="12"/>
+      <c r="TH34" s="12"/>
+      <c r="TI34" s="12"/>
+      <c r="TJ34" s="12"/>
+      <c r="TK34" s="12"/>
+      <c r="TL34" s="12"/>
+      <c r="TM34" s="12"/>
+      <c r="TN34" s="12"/>
+      <c r="TO34" s="12"/>
+      <c r="TP34" s="12"/>
+      <c r="TQ34" s="12"/>
+      <c r="TR34" s="12"/>
+      <c r="TS34" s="12"/>
+      <c r="TT34" s="12"/>
+      <c r="TU34" s="12"/>
+      <c r="TV34" s="12"/>
+      <c r="TW34" s="12"/>
+      <c r="TX34" s="12"/>
+      <c r="TY34" s="12"/>
+      <c r="TZ34" s="12"/>
+      <c r="UA34" s="12"/>
+      <c r="UB34" s="12"/>
+      <c r="UC34" s="12"/>
+      <c r="UD34" s="12"/>
+      <c r="UE34" s="12"/>
+      <c r="UF34" s="12"/>
+      <c r="UG34" s="12"/>
+      <c r="UH34" s="12"/>
+      <c r="UI34" s="12"/>
+      <c r="UJ34" s="12"/>
+      <c r="UK34" s="12"/>
+      <c r="UL34" s="12"/>
+      <c r="UM34" s="12"/>
+      <c r="UN34" s="12"/>
+      <c r="UO34" s="12"/>
+      <c r="UP34" s="12"/>
+      <c r="UQ34" s="12"/>
+      <c r="UR34" s="12"/>
+      <c r="US34" s="12"/>
+      <c r="UT34" s="12"/>
+      <c r="UU34" s="12"/>
+      <c r="UV34" s="12"/>
+      <c r="UW34" s="12"/>
+      <c r="UX34" s="12"/>
+      <c r="UY34" s="12"/>
+      <c r="UZ34" s="12"/>
+      <c r="VA34" s="12"/>
+      <c r="VB34" s="12"/>
+      <c r="VC34" s="12"/>
+      <c r="VD34" s="12"/>
+      <c r="VE34" s="12"/>
+      <c r="VF34" s="12"/>
+      <c r="VG34" s="12"/>
+      <c r="VH34" s="12"/>
+      <c r="VI34" s="12"/>
+      <c r="VJ34" s="12"/>
+      <c r="VK34" s="12"/>
+      <c r="VL34" s="12"/>
+      <c r="VM34" s="12"/>
+      <c r="VN34" s="12"/>
+      <c r="VO34" s="12"/>
+      <c r="VP34" s="12"/>
+      <c r="VQ34" s="12"/>
+      <c r="VR34" s="12"/>
+      <c r="VS34" s="12"/>
+      <c r="VT34" s="12"/>
+      <c r="VU34" s="12"/>
+      <c r="VV34" s="12"/>
+      <c r="VW34" s="12"/>
+      <c r="VX34" s="12"/>
+      <c r="VY34" s="12"/>
+      <c r="VZ34" s="12"/>
+      <c r="WA34" s="12"/>
+      <c r="WB34" s="12"/>
+      <c r="WC34" s="12"/>
+      <c r="WD34" s="12"/>
+      <c r="WE34" s="12"/>
+      <c r="WF34" s="12"/>
+      <c r="WG34" s="12"/>
+      <c r="WH34" s="12"/>
+      <c r="WI34" s="12"/>
+      <c r="WJ34" s="12"/>
+      <c r="WK34" s="12"/>
+      <c r="WL34" s="12"/>
+      <c r="WM34" s="12"/>
+      <c r="WN34" s="12"/>
+      <c r="WO34" s="12"/>
+      <c r="WP34" s="12"/>
+      <c r="WQ34" s="12"/>
+      <c r="WR34" s="12"/>
+      <c r="WS34" s="12"/>
+      <c r="WT34" s="12"/>
+      <c r="WU34" s="12"/>
+      <c r="WV34" s="12"/>
+      <c r="WW34" s="12"/>
+      <c r="WX34" s="12"/>
+      <c r="WY34" s="12"/>
+      <c r="WZ34" s="12"/>
+      <c r="XA34" s="12"/>
+      <c r="XB34" s="12"/>
+      <c r="XC34" s="12"/>
+      <c r="XD34" s="12"/>
+      <c r="XE34" s="12"/>
+      <c r="XF34" s="12"/>
+      <c r="XG34" s="12"/>
+      <c r="XH34" s="12"/>
+      <c r="XI34" s="12"/>
+      <c r="XJ34" s="12"/>
+      <c r="XK34" s="12"/>
+      <c r="XL34" s="12"/>
+      <c r="XM34" s="12"/>
+      <c r="XN34" s="12"/>
+      <c r="XO34" s="12"/>
+      <c r="XP34" s="12"/>
+      <c r="XQ34" s="12"/>
+      <c r="XR34" s="12"/>
+      <c r="XS34" s="12"/>
+      <c r="XT34" s="12"/>
+      <c r="XU34" s="12"/>
+      <c r="XV34" s="12"/>
+      <c r="XW34" s="12"/>
+      <c r="XX34" s="12"/>
+      <c r="XY34" s="12"/>
+      <c r="XZ34" s="12"/>
+      <c r="YA34" s="12"/>
+      <c r="YB34" s="12"/>
+      <c r="YC34" s="12"/>
+      <c r="YD34" s="12"/>
+      <c r="YE34" s="12"/>
+      <c r="YF34" s="12"/>
+      <c r="YG34" s="12"/>
+      <c r="YH34" s="12"/>
+      <c r="YI34" s="12"/>
+      <c r="YJ34" s="12"/>
+      <c r="YK34" s="12"/>
+      <c r="YL34" s="12"/>
+      <c r="YM34" s="12"/>
+      <c r="YN34" s="12"/>
+      <c r="YO34" s="12"/>
+      <c r="YP34" s="12"/>
+      <c r="YQ34" s="12"/>
+      <c r="YR34" s="12"/>
+      <c r="YS34" s="12"/>
+      <c r="YT34" s="12"/>
+      <c r="YU34" s="12"/>
+      <c r="YV34" s="12"/>
+      <c r="YW34" s="12"/>
+      <c r="YX34" s="12"/>
+      <c r="YY34" s="12"/>
+      <c r="YZ34" s="12"/>
+      <c r="ZA34" s="12"/>
+      <c r="ZB34" s="12"/>
+      <c r="ZC34" s="12"/>
+      <c r="ZD34" s="12"/>
+      <c r="ZE34" s="12"/>
+      <c r="ZF34" s="12"/>
+      <c r="ZG34" s="12"/>
+      <c r="ZH34" s="12"/>
+      <c r="ZI34" s="12"/>
+      <c r="ZJ34" s="12"/>
+      <c r="ZK34" s="12"/>
+      <c r="ZL34" s="12"/>
+      <c r="ZM34" s="12"/>
+      <c r="ZN34" s="12"/>
+      <c r="ZO34" s="12"/>
+      <c r="ZP34" s="12"/>
+      <c r="ZQ34" s="12"/>
+      <c r="ZR34" s="12"/>
+      <c r="ZS34" s="12"/>
+      <c r="ZT34" s="12"/>
+      <c r="ZU34" s="12"/>
+      <c r="ZV34" s="12"/>
+      <c r="ZW34" s="12"/>
+      <c r="ZX34" s="12"/>
+      <c r="ZY34" s="12"/>
+      <c r="ZZ34" s="12"/>
+      <c r="AAA34" s="12"/>
+      <c r="AAB34" s="12"/>
+      <c r="AAC34" s="12"/>
+      <c r="AAD34" s="12"/>
+      <c r="AAE34" s="12"/>
+      <c r="AAF34" s="12"/>
+      <c r="AAG34" s="12"/>
+      <c r="AAH34" s="12"/>
+      <c r="AAI34" s="12"/>
+      <c r="AAJ34" s="12"/>
+      <c r="AAK34" s="12"/>
+      <c r="AAL34" s="12"/>
+      <c r="AAM34" s="12"/>
+      <c r="AAN34" s="12"/>
+      <c r="AAO34" s="12"/>
+      <c r="AAP34" s="12"/>
+      <c r="AAQ34" s="12"/>
+      <c r="AAR34" s="12"/>
+      <c r="AAS34" s="12"/>
+      <c r="AAT34" s="12"/>
+      <c r="AAU34" s="12"/>
+      <c r="AAV34" s="12"/>
+      <c r="AAW34" s="12"/>
+      <c r="AAX34" s="12"/>
+      <c r="AAY34" s="12"/>
+      <c r="AAZ34" s="12"/>
+      <c r="ABA34" s="12"/>
+      <c r="ABB34" s="12"/>
+      <c r="ABC34" s="12"/>
+      <c r="ABD34" s="12"/>
+      <c r="ABE34" s="12"/>
+      <c r="ABF34" s="12"/>
+      <c r="ABG34" s="12"/>
+      <c r="ABH34" s="12"/>
+      <c r="ABI34" s="12"/>
+      <c r="ABJ34" s="12"/>
+      <c r="ABK34" s="12"/>
+      <c r="ABL34" s="12"/>
+      <c r="ABM34" s="12"/>
+      <c r="ABN34" s="12"/>
+      <c r="ABO34" s="12"/>
+      <c r="ABP34" s="12"/>
+      <c r="ABQ34" s="12"/>
+      <c r="ABR34" s="12"/>
+      <c r="ABS34" s="12"/>
+      <c r="ABT34" s="12"/>
+      <c r="ABU34" s="12"/>
+      <c r="ABV34" s="12"/>
+      <c r="ABW34" s="12"/>
+      <c r="ABX34" s="12"/>
+      <c r="ABY34" s="12"/>
+      <c r="ABZ34" s="12"/>
+      <c r="ACA34" s="12"/>
+      <c r="ACB34" s="12"/>
+      <c r="ACC34" s="12"/>
+      <c r="ACD34" s="12"/>
+      <c r="ACE34" s="12"/>
+      <c r="ACF34" s="12"/>
+      <c r="ACG34" s="12"/>
+      <c r="ACH34" s="12"/>
+      <c r="ACI34" s="12"/>
+      <c r="ACJ34" s="12"/>
+      <c r="ACK34" s="12"/>
+      <c r="ACL34" s="12"/>
+      <c r="ACM34" s="12"/>
+      <c r="ACN34" s="12"/>
+      <c r="ACO34" s="12"/>
+      <c r="ACP34" s="12"/>
+      <c r="ACQ34" s="12"/>
+      <c r="ACR34" s="12"/>
+      <c r="ACS34" s="12"/>
+      <c r="ACT34" s="12"/>
+      <c r="ACU34" s="12"/>
+      <c r="ACV34" s="12"/>
+      <c r="ACW34" s="12"/>
+      <c r="ACX34" s="12"/>
+      <c r="ACY34" s="12"/>
+      <c r="ACZ34" s="12"/>
+      <c r="ADA34" s="12"/>
+      <c r="ADB34" s="12"/>
+      <c r="ADC34" s="12"/>
+      <c r="ADD34" s="12"/>
+      <c r="ADE34" s="12"/>
+      <c r="ADF34" s="12"/>
+      <c r="ADG34" s="12"/>
+      <c r="ADH34" s="12"/>
+      <c r="ADI34" s="12"/>
+      <c r="ADJ34" s="12"/>
+      <c r="ADK34" s="12"/>
+      <c r="ADL34" s="12"/>
+      <c r="ADM34" s="12"/>
+      <c r="ADN34" s="12"/>
+      <c r="ADO34" s="12"/>
+      <c r="ADP34" s="12"/>
+      <c r="ADQ34" s="12"/>
+      <c r="ADR34" s="12"/>
+      <c r="ADS34" s="12"/>
+      <c r="ADT34" s="12"/>
+      <c r="ADU34" s="12"/>
+      <c r="ADV34" s="12"/>
+      <c r="ADW34" s="12"/>
+      <c r="ADX34" s="12"/>
+      <c r="ADY34" s="12"/>
+      <c r="ADZ34" s="12"/>
+      <c r="AEA34" s="12"/>
+      <c r="AEB34" s="12"/>
+      <c r="AEC34" s="12"/>
+      <c r="AED34" s="12"/>
+      <c r="AEE34" s="12"/>
+      <c r="AEF34" s="12"/>
+      <c r="AEG34" s="12"/>
+      <c r="AEH34" s="12"/>
+      <c r="AEI34" s="12"/>
+      <c r="AEJ34" s="12"/>
+      <c r="AEK34" s="12"/>
+      <c r="AEL34" s="12"/>
+      <c r="AEM34" s="12"/>
+      <c r="AEN34" s="12"/>
+      <c r="AEO34" s="12"/>
+      <c r="AEP34" s="12"/>
+      <c r="AEQ34" s="12"/>
+      <c r="AER34" s="12"/>
+      <c r="AES34" s="12"/>
+      <c r="AET34" s="12"/>
+      <c r="AEU34" s="12"/>
+      <c r="AEV34" s="12"/>
+      <c r="AEW34" s="12"/>
+      <c r="AEX34" s="12"/>
+      <c r="AEY34" s="12"/>
+      <c r="AEZ34" s="12"/>
+      <c r="AFA34" s="12"/>
+      <c r="AFB34" s="12"/>
+      <c r="AFC34" s="12"/>
+      <c r="AFD34" s="12"/>
+      <c r="AFE34" s="12"/>
+      <c r="AFF34" s="12"/>
+      <c r="AFG34" s="12"/>
+      <c r="AFH34" s="12"/>
+      <c r="AFI34" s="12"/>
+      <c r="AFJ34" s="12"/>
+      <c r="AFK34" s="12"/>
+      <c r="AFL34" s="12"/>
+      <c r="AFM34" s="12"/>
+      <c r="AFN34" s="12"/>
+      <c r="AFO34" s="12"/>
+      <c r="AFP34" s="12"/>
+      <c r="AFQ34" s="12"/>
+      <c r="AFR34" s="12"/>
+      <c r="AFS34" s="12"/>
+      <c r="AFT34" s="12"/>
+      <c r="AFU34" s="12"/>
+      <c r="AFV34" s="12"/>
+      <c r="AFW34" s="12"/>
+      <c r="AFX34" s="12"/>
+      <c r="AFY34" s="12"/>
+      <c r="AFZ34" s="12"/>
+      <c r="AGA34" s="12"/>
+      <c r="AGB34" s="12"/>
+      <c r="AGC34" s="12"/>
+      <c r="AGD34" s="12"/>
+      <c r="AGE34" s="12"/>
+      <c r="AGF34" s="12"/>
+      <c r="AGG34" s="12"/>
+      <c r="AGH34" s="12"/>
+      <c r="AGI34" s="12"/>
+      <c r="AGJ34" s="12"/>
+      <c r="AGK34" s="12"/>
+      <c r="AGL34" s="12"/>
+      <c r="AGM34" s="12"/>
+      <c r="AGN34" s="12"/>
+      <c r="AGO34" s="12"/>
+      <c r="AGP34" s="12"/>
+      <c r="AGQ34" s="12"/>
+      <c r="AGR34" s="12"/>
+      <c r="AGS34" s="12"/>
+      <c r="AGT34" s="12"/>
+      <c r="AGU34" s="12"/>
+      <c r="AGV34" s="12"/>
+      <c r="AGW34" s="12"/>
+      <c r="AGX34" s="12"/>
+      <c r="AGY34" s="12"/>
+      <c r="AGZ34" s="12"/>
+      <c r="AHA34" s="12"/>
+      <c r="AHB34" s="12"/>
+      <c r="AHC34" s="12"/>
+      <c r="AHD34" s="12"/>
+      <c r="AHE34" s="12"/>
+      <c r="AHF34" s="12"/>
+      <c r="AHG34" s="12"/>
+      <c r="AHH34" s="12"/>
+      <c r="AHI34" s="12"/>
+      <c r="AHJ34" s="12"/>
+      <c r="AHK34" s="12"/>
+      <c r="AHL34" s="12"/>
+      <c r="AHM34" s="12"/>
+      <c r="AHN34" s="12"/>
+      <c r="AHO34" s="12"/>
+      <c r="AHP34" s="12"/>
+      <c r="AHQ34" s="12"/>
+      <c r="AHR34" s="12"/>
+      <c r="AHS34" s="12"/>
+      <c r="AHT34" s="12"/>
+      <c r="AHU34" s="12"/>
+      <c r="AHV34" s="12"/>
+      <c r="AHW34" s="12"/>
+      <c r="AHX34" s="12"/>
+      <c r="AHY34" s="12"/>
+      <c r="AHZ34" s="12"/>
+      <c r="AIA34" s="12"/>
+      <c r="AIB34" s="12"/>
+      <c r="AIC34" s="12"/>
+      <c r="AID34" s="12"/>
+      <c r="AIE34" s="12"/>
+      <c r="AIF34" s="12"/>
+      <c r="AIG34" s="12"/>
+      <c r="AIH34" s="12"/>
+      <c r="AII34" s="12"/>
+      <c r="AIJ34" s="12"/>
+      <c r="AIK34" s="12"/>
+      <c r="AIL34" s="12"/>
+      <c r="AIM34" s="12"/>
+      <c r="AIN34" s="12"/>
+      <c r="AIO34" s="12"/>
+      <c r="AIP34" s="12"/>
+      <c r="AIQ34" s="12"/>
+      <c r="AIR34" s="12"/>
+      <c r="AIS34" s="12"/>
+      <c r="AIT34" s="12"/>
+      <c r="AIU34" s="12"/>
+      <c r="AIV34" s="12"/>
+      <c r="AIW34" s="12"/>
+      <c r="AIX34" s="12"/>
+      <c r="AIY34" s="12"/>
+      <c r="AIZ34" s="12"/>
+      <c r="AJA34" s="12"/>
+      <c r="AJB34" s="12"/>
+      <c r="AJC34" s="12"/>
+      <c r="AJD34" s="12"/>
+      <c r="AJE34" s="12"/>
+      <c r="AJF34" s="12"/>
+      <c r="AJG34" s="12"/>
+      <c r="AJH34" s="12"/>
+      <c r="AJI34" s="12"/>
+      <c r="AJJ34" s="12"/>
+      <c r="AJK34" s="12"/>
+      <c r="AJL34" s="12"/>
+      <c r="AJM34" s="12"/>
+      <c r="AJN34" s="12"/>
+      <c r="AJO34" s="12"/>
+      <c r="AJP34" s="12"/>
+      <c r="AJQ34" s="12"/>
+      <c r="AJR34" s="12"/>
+      <c r="AJS34" s="12"/>
+      <c r="AJT34" s="12"/>
+      <c r="AJU34" s="12"/>
+      <c r="AJV34" s="12"/>
+      <c r="AJW34" s="12"/>
+      <c r="AJX34" s="12"/>
+      <c r="AJY34" s="12"/>
+      <c r="AJZ34" s="12"/>
+      <c r="AKA34" s="12"/>
+      <c r="AKB34" s="12"/>
+      <c r="AKC34" s="12"/>
+      <c r="AKD34" s="12"/>
+      <c r="AKE34" s="12"/>
+      <c r="AKF34" s="12"/>
+      <c r="AKG34" s="12"/>
+      <c r="AKH34" s="12"/>
+      <c r="AKI34" s="12"/>
+      <c r="AKJ34" s="12"/>
+      <c r="AKK34" s="12"/>
+      <c r="AKL34" s="12"/>
+      <c r="AKM34" s="12"/>
+      <c r="AKN34" s="12"/>
+      <c r="AKO34" s="12"/>
+      <c r="AKP34" s="12"/>
+      <c r="AKQ34" s="12"/>
+      <c r="AKR34" s="12"/>
+      <c r="AKS34" s="12"/>
+      <c r="AKT34" s="12"/>
+      <c r="AKU34" s="12"/>
+      <c r="AKV34" s="12"/>
+      <c r="AKW34" s="12"/>
+      <c r="AKX34" s="12"/>
+      <c r="AKY34" s="12"/>
+      <c r="AKZ34" s="12"/>
+      <c r="ALA34" s="12"/>
+      <c r="ALB34" s="12"/>
+      <c r="ALC34" s="12"/>
+      <c r="ALD34" s="12"/>
+      <c r="ALE34" s="12"/>
+      <c r="ALF34" s="12"/>
+      <c r="ALG34" s="12"/>
+      <c r="ALH34" s="12"/>
+      <c r="ALI34" s="12"/>
+      <c r="ALJ34" s="12"/>
+      <c r="ALK34" s="12"/>
+      <c r="ALL34" s="12"/>
+      <c r="ALM34" s="12"/>
+      <c r="ALN34" s="12"/>
+      <c r="ALO34" s="12"/>
+      <c r="ALP34" s="12"/>
+      <c r="ALQ34" s="12"/>
+      <c r="ALR34" s="12"/>
+      <c r="ALS34" s="12"/>
+      <c r="ALT34" s="12"/>
+      <c r="ALU34" s="12"/>
+      <c r="ALV34" s="12"/>
+      <c r="ALW34" s="12"/>
+      <c r="ALX34" s="12"/>
+      <c r="ALY34" s="12"/>
+      <c r="ALZ34" s="12"/>
+      <c r="AMA34" s="12"/>
+      <c r="AMB34" s="12"/>
+      <c r="AMC34" s="12"/>
+      <c r="AMD34" s="12"/>
+      <c r="AME34" s="12"/>
+      <c r="AMF34" s="12"/>
+      <c r="AMG34" s="12"/>
+      <c r="AMH34" s="12"/>
+      <c r="AMI34" s="12"/>
+      <c r="AMJ34" s="12"/>
     </row>
     <row r="35" spans="1:1024" ht="15" customHeight="1">
-      <c r="A35" s="102"/>
-      <c r="B35" s="102"/>
-      <c r="C35" s="81" t="s">
+      <c r="A35" s="116" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="116"/>
+      <c r="C35" s="108" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="108"/>
+      <c r="E35" s="108"/>
+      <c r="F35" s="109"/>
+    </row>
+    <row r="36" spans="1:1024" ht="15" customHeight="1">
+      <c r="A36" s="117"/>
+      <c r="B36" s="117"/>
+      <c r="C36" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="81" t="s">
+      <c r="D36" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="81" t="s">
+      <c r="E36" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="101"/>
-    </row>
-    <row r="36" spans="1:1024">
-      <c r="A36" s="58">
-        <v>1</v>
-      </c>
-      <c r="B36" s="77" t="s">
-        <v>99</v>
-      </c>
-      <c r="C36" s="77"/>
-      <c r="D36" s="77"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="77"/>
+      <c r="F36" s="110"/>
     </row>
     <row r="37" spans="1:1024">
       <c r="A37" s="58">
-        <v>2</v>
-      </c>
-      <c r="B37" s="77" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37" s="77"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="77"/>
+        <v>1</v>
+      </c>
+      <c r="B37" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="72"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
     </row>
     <row r="38" spans="1:1024">
       <c r="A38" s="58">
-        <v>3</v>
-      </c>
-      <c r="B38" s="77" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" s="77"/>
-      <c r="D38" s="77"/>
-      <c r="E38" s="77"/>
-      <c r="F38" s="77"/>
+        <v>2</v>
+      </c>
+      <c r="B38" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="72"/>
     </row>
     <row r="39" spans="1:1024">
       <c r="A39" s="58">
-        <v>4</v>
-      </c>
-      <c r="B39" s="59" t="s">
-        <v>98</v>
-      </c>
-      <c r="C39" s="77"/>
-      <c r="D39" s="77"/>
-      <c r="E39" s="77"/>
-      <c r="F39" s="77"/>
+        <v>3</v>
+      </c>
+      <c r="B39" s="72" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="72"/>
+      <c r="D39" s="72"/>
+      <c r="E39" s="72"/>
+      <c r="F39" s="72"/>
     </row>
     <row r="40" spans="1:1024">
       <c r="A40" s="58">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B40" s="59" t="s">
-        <v>102</v>
-      </c>
-      <c r="C40" s="77"/>
-      <c r="D40" s="77"/>
-      <c r="E40" s="77"/>
-      <c r="F40" s="77"/>
+        <v>97</v>
+      </c>
+      <c r="C40" s="72"/>
+      <c r="D40" s="72"/>
+      <c r="E40" s="72"/>
+      <c r="F40" s="72"/>
     </row>
     <row r="41" spans="1:1024">
       <c r="A41" s="58">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B41" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="C41" s="77"/>
-      <c r="D41" s="77"/>
-      <c r="E41" s="77"/>
-      <c r="F41" s="77"/>
+        <v>101</v>
+      </c>
+      <c r="C41" s="72"/>
+      <c r="D41" s="72"/>
+      <c r="E41" s="72"/>
+      <c r="F41" s="72"/>
     </row>
     <row r="42" spans="1:1024">
       <c r="A42" s="58">
-        <v>7</v>
-      </c>
-      <c r="B42" s="77" t="s">
-        <v>104</v>
-      </c>
-      <c r="C42" s="77"/>
-      <c r="D42" s="77"/>
-      <c r="E42" s="77"/>
-      <c r="F42" s="77"/>
+        <v>6</v>
+      </c>
+      <c r="B42" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="72"/>
+      <c r="D42" s="72"/>
+      <c r="E42" s="72"/>
+      <c r="F42" s="72"/>
     </row>
     <row r="43" spans="1:1024">
       <c r="A43" s="58">
-        <v>8</v>
-      </c>
-      <c r="B43" s="59" t="s">
-        <v>105</v>
-      </c>
-      <c r="C43" s="57"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="57"/>
-      <c r="F43" s="57"/>
+        <v>7</v>
+      </c>
+      <c r="B43" s="72" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="72"/>
+      <c r="D43" s="72"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="72"/>
     </row>
     <row r="44" spans="1:1024">
       <c r="A44" s="58">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B44" s="59" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C44" s="57"/>
       <c r="D44" s="57"/>
       <c r="E44" s="57"/>
       <c r="F44" s="57"/>
     </row>
-    <row r="46" spans="1:1024">
-      <c r="A46" s="106" t="s">
-        <v>81</v>
-      </c>
-      <c r="B46" s="106"/>
-      <c r="C46" s="105" t="s">
-        <v>12</v>
-      </c>
-      <c r="D46" s="105"/>
-      <c r="E46" s="105"/>
-      <c r="F46" s="107" t="s">
-        <v>13</v>
-      </c>
+    <row r="45" spans="1:1024">
+      <c r="A45" s="58">
+        <v>9</v>
+      </c>
+      <c r="B45" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
     </row>
     <row r="47" spans="1:1024">
-      <c r="A47" s="106"/>
-      <c r="B47" s="106"/>
-      <c r="C47" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="E47" s="60" t="s">
+      <c r="A47" s="114" t="s">
         <v>80</v>
       </c>
-      <c r="F47" s="107"/>
+      <c r="B47" s="114"/>
+      <c r="C47" s="113" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="113"/>
+      <c r="E47" s="113"/>
+      <c r="F47" s="115" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="48" spans="1:1024">
-      <c r="A48" s="58">
-        <v>1</v>
-      </c>
-      <c r="B48" s="59" t="s">
+      <c r="A48" s="114"/>
+      <c r="B48" s="114"/>
+      <c r="C48" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C48" s="57"/>
-      <c r="D48" s="57"/>
-      <c r="E48" s="57"/>
-      <c r="F48" s="57"/>
+      <c r="F48" s="115"/>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B49" s="59" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C49" s="57"/>
       <c r="D49" s="57"/>
       <c r="E49" s="57"/>
       <c r="F49" s="57"/>
     </row>
-    <row r="50" spans="1:6" ht="30">
+    <row r="50" spans="1:6">
       <c r="A50" s="58">
-        <v>3</v>
-      </c>
-      <c r="B50" s="54" t="s">
-        <v>84</v>
+        <v>2</v>
+      </c>
+      <c r="B50" s="59" t="s">
+        <v>82</v>
       </c>
       <c r="C50" s="57"/>
       <c r="D50" s="57"/>
       <c r="E50" s="57"/>
       <c r="F50" s="57"/>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" ht="30">
       <c r="A51" s="58">
-        <v>4</v>
-      </c>
-      <c r="B51" s="59" t="s">
-        <v>82</v>
+        <v>3</v>
+      </c>
+      <c r="B51" s="54" t="s">
+        <v>83</v>
       </c>
       <c r="C51" s="57"/>
       <c r="D51" s="57"/>
       <c r="E51" s="57"/>
       <c r="F51" s="57"/>
     </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="95" t="s">
-        <v>109</v>
-      </c>
-      <c r="B54" s="95"/>
-      <c r="C54" s="96" t="s">
-        <v>12</v>
-      </c>
-      <c r="D54" s="96"/>
-      <c r="E54" s="97"/>
-      <c r="F54" s="98" t="s">
-        <v>13</v>
-      </c>
+    <row r="52" spans="1:6">
+      <c r="A52" s="58">
+        <v>4</v>
+      </c>
+      <c r="B52" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="C52" s="57"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="57"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="95"/>
-      <c r="B55" s="95"/>
-      <c r="C55" s="36" t="s">
+      <c r="A55" s="94" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="94"/>
+      <c r="C55" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="95"/>
+      <c r="E55" s="96"/>
+      <c r="F55" s="105" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="94"/>
+      <c r="B56" s="94"/>
+      <c r="C56" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D55" s="22" t="s">
+      <c r="D56" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="22" t="s">
+      <c r="E56" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F55" s="99"/>
+      <c r="F56" s="106"/>
     </row>
-    <row r="56" spans="1:6" ht="26.25">
-      <c r="A56" s="24">
+    <row r="57" spans="1:6" ht="26.25">
+      <c r="A57" s="24">
         <v>1</v>
       </c>
-      <c r="B56" s="124" t="s">
-        <v>110</v>
-      </c>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="25"/>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="24">
-        <v>2</v>
-      </c>
-      <c r="B57" s="124" t="s">
-        <v>111</v>
+      <c r="B57" s="84" t="s">
+        <v>108</v>
       </c>
       <c r="C57" s="26"/>
       <c r="D57" s="26"/>
@@ -23693,10 +23811,10 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="24">
-        <v>3</v>
-      </c>
-      <c r="B58" s="124" t="s">
-        <v>112</v>
+        <v>2</v>
+      </c>
+      <c r="B58" s="84" t="s">
+        <v>109</v>
       </c>
       <c r="C58" s="26"/>
       <c r="D58" s="26"/>
@@ -23705,10 +23823,10 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="24">
-        <v>4</v>
-      </c>
-      <c r="B59" s="124" t="s">
-        <v>113</v>
+        <v>3</v>
+      </c>
+      <c r="B59" s="84" t="s">
+        <v>110</v>
       </c>
       <c r="C59" s="26"/>
       <c r="D59" s="26"/>
@@ -23716,61 +23834,73 @@
       <c r="F59" s="25"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="125">
-        <v>5</v>
-      </c>
-      <c r="B60" s="124" t="s">
-        <v>114</v>
-      </c>
-      <c r="C60" s="126"/>
-      <c r="D60" s="126"/>
-      <c r="E60" s="126"/>
-      <c r="F60" s="127"/>
+      <c r="A60" s="24">
+        <v>4</v>
+      </c>
+      <c r="B60" s="84" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="25"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="24">
-        <v>6</v>
-      </c>
-      <c r="B61" s="124" t="s">
-        <v>115</v>
-      </c>
-      <c r="C61" s="128"/>
-      <c r="D61" s="128"/>
-      <c r="E61" s="128"/>
-      <c r="F61" s="128"/>
+      <c r="A61" s="85">
+        <v>5</v>
+      </c>
+      <c r="B61" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" s="86"/>
+      <c r="D61" s="86"/>
+      <c r="E61" s="86"/>
+      <c r="F61" s="87"/>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="24">
+        <v>6</v>
+      </c>
+      <c r="B62" s="84" t="s">
+        <v>113</v>
+      </c>
+      <c r="C62" s="88"/>
+      <c r="D62" s="88"/>
+      <c r="E62" s="88"/>
+      <c r="F62" s="88"/>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="24">
         <v>7</v>
       </c>
-      <c r="B62" s="124" t="s">
-        <v>116</v>
-      </c>
-      <c r="C62" s="128"/>
-      <c r="D62" s="128"/>
-      <c r="E62" s="128"/>
-      <c r="F62" s="128"/>
+      <c r="B63" s="84" t="s">
+        <v>114</v>
+      </c>
+      <c r="C63" s="88"/>
+      <c r="D63" s="88"/>
+      <c r="E63" s="88"/>
+      <c r="F63" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="A54:B55"/>
-    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="A35:B36"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A9:B10"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="A46:B47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A34:B35"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="A55:B56"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="A47:B48"/>
+    <mergeCell ref="F47:F48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23779,10 +23909,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -23793,159 +23923,158 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="109" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="112" t="s">
+      <c r="A1" s="119" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="100"/>
+      <c r="C1" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="113"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="89" t="s">
+      <c r="D1" s="123"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="100" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="110"/>
-      <c r="B2" s="111"/>
-      <c r="C2" s="73" t="s">
+      <c r="A2" s="120"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="73" t="s">
+      <c r="E2" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="89"/>
+      <c r="F2" s="100"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="108" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="108"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="74"/>
+      <c r="A3" s="118" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="118"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="70"/>
     </row>
     <row r="4" spans="1:6" ht="26.25">
-      <c r="A4" s="69">
+      <c r="A4" s="37">
         <v>1</v>
       </c>
-      <c r="B4" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="72"/>
+      <c r="B4" s="127" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="40"/>
     </row>
     <row r="5" spans="1:6" ht="26.25">
-      <c r="A5" s="69">
+      <c r="A5" s="37">
         <v>2</v>
       </c>
-      <c r="B5" s="70" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="72"/>
+      <c r="B5" s="127" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="40"/>
     </row>
     <row r="6" spans="1:6" ht="26.25">
-      <c r="A6" s="69">
+      <c r="A6" s="37">
         <v>3</v>
       </c>
-      <c r="B6" s="70" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="72"/>
+      <c r="B6" s="127" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="40"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="108" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="108"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="74"/>
+      <c r="A7" s="118" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="118"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="70"/>
     </row>
     <row r="8" spans="1:6" ht="26.25">
-      <c r="A8" s="69">
+      <c r="A8" s="37">
         <v>1</v>
       </c>
-      <c r="B8" s="70" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="72"/>
+      <c r="B8" s="127" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40"/>
     </row>
     <row r="9" spans="1:6" ht="26.25">
-      <c r="A9" s="69">
+      <c r="A9" s="37">
         <v>2</v>
       </c>
-      <c r="B9" s="70" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="72"/>
+      <c r="B9" s="127" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="40"/>
     </row>
     <row r="10" spans="1:6" ht="26.25">
-      <c r="A10" s="69">
+      <c r="A10" s="37">
         <v>3</v>
       </c>
-      <c r="B10" s="70" t="s">
-        <v>90</v>
-      </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="72"/>
+      <c r="B10" s="127" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="40"/>
     </row>
     <row r="11" spans="1:6" ht="39">
-      <c r="A11" s="69">
+      <c r="A11" s="37">
         <v>4</v>
       </c>
-      <c r="B11" s="70" t="s">
-        <v>95</v>
-      </c>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="72"/>
+      <c r="B11" s="127" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="40"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="108" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="108"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="74"/>
+      <c r="A12" s="118" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="118"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="70"/>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="69">
-        <v>8</v>
-      </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="72"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="B14" s="76"/>
+    <row r="13" spans="1:6" ht="25.5">
+      <c r="A13" s="37">
+        <v>1</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -23958,4 +24087,234 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="52" customWidth="1"/>
+    <col min="6" max="6" width="48" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="A2" s="126"/>
+      <c r="B2" s="125" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="122" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="123"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="100" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="126"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="77" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="77" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="100"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="118" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="118"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="70"/>
+    </row>
+    <row r="5" spans="1:6" ht="25.5">
+      <c r="A5" s="37">
+        <v>1</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="42"/>
+    </row>
+    <row r="6" spans="1:6" ht="25.5">
+      <c r="A6" s="37">
+        <v>2</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="40"/>
+    </row>
+    <row r="7" spans="1:6" ht="25.5">
+      <c r="A7" s="37">
+        <v>3</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="42"/>
+    </row>
+    <row r="8" spans="1:6" ht="25.5">
+      <c r="A8" s="37">
+        <v>4</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="42"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="118" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="118"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="37">
+        <v>1</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="42"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="37">
+        <v>2</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="40"/>
+    </row>
+    <row r="12" spans="1:6" ht="25.5">
+      <c r="A12" s="37">
+        <v>3</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="40"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="37">
+        <v>4</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="40"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="118" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="118"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+    </row>
+    <row r="15" spans="1:6" ht="25.5">
+      <c r="A15" s="37">
+        <v>1</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="42"/>
+    </row>
+    <row r="16" spans="1:6" ht="25.5">
+      <c r="A16" s="37">
+        <v>2</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="40"/>
+    </row>
+    <row r="17" spans="1:6" ht="25.5">
+      <c r="A17" s="37">
+        <v>3</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="40"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="37">
+        <v>4</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>